<commit_message>
find temporal overlaps in detections check audio completeness
</commit_message>
<xml_diff>
--- a/Documentation/Summary.xlsx
+++ b/Documentation/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaitlin.palmer\Documents\GitHub\DCLDE2026\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BE2319-E04B-4748-8CA8-E336CF1DBA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E14C2C0-02D0-468E-851B-8F00F829AB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="1128" windowWidth="20556" windowHeight="11280" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
+    <workbookView xWindow="624" yWindow="1152" windowWidth="20556" windowHeight="11280" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="90">
   <si>
     <t>Annotations</t>
   </si>
@@ -75,6 +75,9 @@
     <t>West Vancouver Island</t>
   </si>
   <si>
+    <t>Detection</t>
+  </si>
+  <si>
     <t>Northern Mainland British Colombia</t>
   </si>
   <si>
@@ -264,9 +267,6 @@
     <t>AURAL-M2</t>
   </si>
   <si>
-    <t>Pamguard Detection</t>
-  </si>
-  <si>
     <t>First Detection</t>
   </si>
   <si>
@@ -283,6 +283,27 @@
   </si>
   <si>
     <t>SoundTrap 6249</t>
+  </si>
+  <si>
+    <t>Detector</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Pamguard WM</t>
+  </si>
+  <si>
+    <t>JASCO Detcetor</t>
+  </si>
+  <si>
+    <t>Orcasound Lab</t>
+  </si>
+  <si>
+    <t>Port Townsand</t>
+  </si>
+  <si>
+    <t>Bush Point</t>
   </si>
 </sst>
 </file>
@@ -598,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -684,6 +705,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4A8866-C81C-482A-B0A6-264BECA1C8D5}">
-  <dimension ref="A1:BY27"/>
+  <dimension ref="A1:BZ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1012,23 +1042,23 @@
     <col min="4" max="4" width="11.77734375" style="28" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="28" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" style="4" customWidth="1"/>
-    <col min="10" max="13" width="10.5546875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="13" width="10.5546875" style="4" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
+    <col min="16" max="16" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="O1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="P1" s="23"/>
+    <row r="1" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="P1" s="23" t="s">
+        <v>0</v>
+      </c>
       <c r="Q1" s="23"/>
       <c r="R1" s="23"/>
       <c r="S1" s="23"/>
@@ -1036,37 +1066,38 @@
       <c r="U1" s="23"/>
       <c r="V1" s="23"/>
       <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
     </row>
-    <row r="2" spans="1:77" s="24" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:78" s="24" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K2" s="25" t="s">
         <v>77</v>
@@ -1075,45 +1106,51 @@
         <v>78</v>
       </c>
       <c r="M2" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="48" t="s">
         <v>3</v>
       </c>
       <c r="O2" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="Q2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="R2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="S2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="T2" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="U2" s="24" t="s">
+      <c r="T2" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="V2" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="V2" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="W2" s="26" t="s">
-        <v>56</v>
+      <c r="X2" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
       <c r="C3" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G3">
         <v>32</v>
@@ -1124,37 +1161,46 @@
       <c r="L3" s="5">
         <v>43651</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="N3" s="47">
+        <v>446</v>
+      </c>
+      <c r="O3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>435</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
       <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>11</v>
       </c>
-      <c r="S3" s="14">
-        <v>0</v>
-      </c>
-      <c r="T3" s="16">
+      <c r="T3" s="14">
+        <v>0</v>
+      </c>
+      <c r="U3" s="16">
         <v>435</v>
       </c>
-      <c r="U3" s="14">
-        <v>0</v>
-      </c>
       <c r="V3" s="14">
         <v>0</v>
       </c>
-      <c r="W3" s="19">
+      <c r="W3" s="14">
+        <v>0</v>
+      </c>
+      <c r="X3" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
       <c r="C4" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G4">
         <v>32</v>
@@ -1165,35 +1211,39 @@
       <c r="L4" s="5">
         <v>43005</v>
       </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="16" t="s">
+      <c r="N4" s="47">
+        <v>496</v>
+      </c>
+      <c r="O4" t="s">
+        <v>84</v>
+      </c>
+      <c r="P4" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>436</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
       <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
         <v>60</v>
       </c>
-      <c r="S4" s="14">
-        <v>0</v>
-      </c>
-      <c r="T4" s="16">
+      <c r="T4" s="14">
+        <v>0</v>
+      </c>
+      <c r="U4" s="16">
         <v>436</v>
       </c>
-      <c r="U4" s="14">
-        <v>0</v>
-      </c>
       <c r="V4" s="14">
         <v>0</v>
       </c>
-      <c r="W4" s="19">
-        <v>0</v>
-      </c>
-      <c r="X4" s="4"/>
+      <c r="W4" s="14">
+        <v>0</v>
+      </c>
+      <c r="X4" s="19">
+        <v>0</v>
+      </c>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
@@ -1237,19 +1287,23 @@
       <c r="BM4" s="4"/>
       <c r="BN4" s="4"/>
       <c r="BO4" s="4"/>
-      <c r="BQ4" s="16"/>
-      <c r="BR4" s="14"/>
+      <c r="BP4" s="4"/>
+      <c r="BR4" s="16"/>
       <c r="BS4" s="14"/>
       <c r="BT4" s="14"/>
       <c r="BU4" s="14"/>
       <c r="BV4" s="14"/>
       <c r="BW4" s="14"/>
       <c r="BX4" s="14"/>
-      <c r="BY4" s="19"/>
+      <c r="BY4" s="14"/>
+      <c r="BZ4" s="19"/>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
       <c r="C5" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G5">
         <v>32</v>
@@ -1260,37 +1314,46 @@
       <c r="L5" s="5">
         <v>44037</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="N5" s="47">
+        <v>31</v>
+      </c>
+      <c r="O5" t="s">
+        <v>84</v>
+      </c>
+      <c r="P5" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
         <v>31</v>
       </c>
-      <c r="S5" s="14">
-        <v>0</v>
-      </c>
-      <c r="T5" s="39">
-        <v>0</v>
-      </c>
-      <c r="U5" s="14">
+      <c r="T5" s="14">
+        <v>0</v>
+      </c>
+      <c r="U5" s="39">
         <v>0</v>
       </c>
       <c r="V5" s="14">
         <v>0</v>
       </c>
-      <c r="W5" s="19">
+      <c r="W5" s="14">
+        <v>0</v>
+      </c>
+      <c r="X5" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
       <c r="C6" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6">
         <v>32</v>
@@ -1301,37 +1364,46 @@
       <c r="L6" s="5">
         <v>44075</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="N6" s="47">
+        <v>176</v>
+      </c>
+      <c r="O6" t="s">
+        <v>84</v>
+      </c>
+      <c r="P6" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>151</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
       <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
         <v>25</v>
       </c>
-      <c r="S6" s="14">
-        <v>0</v>
-      </c>
-      <c r="T6" s="16">
+      <c r="T6" s="14">
+        <v>0</v>
+      </c>
+      <c r="U6" s="16">
         <v>151</v>
       </c>
-      <c r="U6" s="14">
-        <v>0</v>
-      </c>
       <c r="V6" s="14">
         <v>0</v>
       </c>
-      <c r="W6" s="19">
+      <c r="W6" s="14">
+        <v>0</v>
+      </c>
+      <c r="X6" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
       <c r="C7" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G7">
         <v>32</v>
@@ -1342,37 +1414,46 @@
       <c r="L7" s="5">
         <v>44081</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="N7" s="47">
+        <v>167</v>
+      </c>
+      <c r="O7" t="s">
+        <v>84</v>
+      </c>
+      <c r="P7" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
         <v>167</v>
       </c>
-      <c r="S7" s="14">
-        <v>0</v>
-      </c>
-      <c r="T7" s="39">
-        <v>0</v>
-      </c>
-      <c r="U7" s="14">
+      <c r="T7" s="14">
+        <v>0</v>
+      </c>
+      <c r="U7" s="39">
         <v>0</v>
       </c>
       <c r="V7" s="14">
         <v>0</v>
       </c>
-      <c r="W7" s="19">
+      <c r="W7" s="14">
+        <v>0</v>
+      </c>
+      <c r="X7" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
       <c r="C8" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G8">
         <v>32</v>
@@ -1383,37 +1464,46 @@
       <c r="L8" s="5">
         <v>44103</v>
       </c>
-      <c r="O8" s="16" t="s">
+      <c r="N8" s="47">
+        <v>287</v>
+      </c>
+      <c r="O8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P8" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>198</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
       <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
         <v>89</v>
       </c>
-      <c r="S8" s="14">
-        <v>0</v>
-      </c>
-      <c r="T8" s="16">
+      <c r="T8" s="14">
+        <v>0</v>
+      </c>
+      <c r="U8" s="16">
         <v>198</v>
       </c>
-      <c r="U8" s="14">
-        <v>0</v>
-      </c>
       <c r="V8" s="14">
         <v>0</v>
       </c>
-      <c r="W8" s="19">
+      <c r="W8" s="14">
+        <v>0</v>
+      </c>
+      <c r="X8" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
       <c r="C9" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G9">
         <v>32</v>
@@ -1424,37 +1514,46 @@
       <c r="L9" s="5">
         <v>44102</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="N9" s="47">
+        <v>623</v>
+      </c>
+      <c r="O9" t="s">
+        <v>84</v>
+      </c>
+      <c r="P9" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>510</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
       <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
         <v>113</v>
       </c>
-      <c r="S9" s="14">
-        <v>0</v>
-      </c>
-      <c r="T9" s="16">
+      <c r="T9" s="14">
+        <v>0</v>
+      </c>
+      <c r="U9" s="16">
         <v>510</v>
       </c>
-      <c r="U9" s="14">
-        <v>0</v>
-      </c>
       <c r="V9" s="14">
         <v>0</v>
       </c>
-      <c r="W9" s="19">
+      <c r="W9" s="14">
+        <v>0</v>
+      </c>
+      <c r="X9" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
       <c r="C10" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G10">
         <v>32</v>
@@ -1465,37 +1564,46 @@
       <c r="L10" s="5">
         <v>44122</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="N10" s="47">
+        <v>118</v>
+      </c>
+      <c r="O10" t="s">
+        <v>84</v>
+      </c>
+      <c r="P10" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
         <v>118</v>
       </c>
-      <c r="S10" s="14">
-        <v>0</v>
-      </c>
-      <c r="T10" s="39">
-        <v>0</v>
-      </c>
-      <c r="U10" s="14">
+      <c r="T10" s="14">
+        <v>0</v>
+      </c>
+      <c r="U10" s="39">
         <v>0</v>
       </c>
       <c r="V10" s="14">
         <v>0</v>
       </c>
-      <c r="W10" s="19">
+      <c r="W10" s="14">
+        <v>0</v>
+      </c>
+      <c r="X10" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
       <c r="C11" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G11">
         <v>32</v>
@@ -1506,35 +1614,41 @@
       <c r="L11" s="5">
         <v>44112</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="N11" s="47">
+        <v>54</v>
+      </c>
+      <c r="O11" t="s">
+        <v>84</v>
+      </c>
+      <c r="P11" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>54</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
       <c r="R11">
         <v>0</v>
       </c>
-      <c r="S11" s="14">
-        <v>0</v>
-      </c>
-      <c r="T11" s="16">
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11" s="14">
+        <v>0</v>
+      </c>
+      <c r="U11" s="16">
         <v>54</v>
       </c>
-      <c r="U11" s="14">
-        <v>0</v>
-      </c>
       <c r="V11" s="14">
         <v>0</v>
       </c>
-      <c r="W11" s="19">
+      <c r="W11" s="14">
+        <v>0</v>
+      </c>
+      <c r="X11" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:77" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:78" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -1557,7 +1671,7 @@
         <v>64</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -1568,52 +1682,55 @@
         <v>41977</v>
       </c>
       <c r="M12" s="8"/>
-      <c r="N12" s="7">
+      <c r="N12" s="49">
         <v>14120</v>
       </c>
-      <c r="O12" s="34" t="s">
+      <c r="O12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="P12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P12" s="7">
+      <c r="Q12" s="7">
         <v>1626</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="R12" s="7">
         <v>9392</v>
       </c>
-      <c r="R12" s="7">
+      <c r="S12" s="7">
         <v>156</v>
       </c>
-      <c r="S12" s="7">
+      <c r="T12" s="7">
         <v>2946</v>
       </c>
-      <c r="T12" s="40">
+      <c r="U12" s="40">
         <v>130</v>
       </c>
-      <c r="U12" s="7">
+      <c r="V12" s="7">
         <v>834</v>
       </c>
-      <c r="V12" s="7">
-        <v>0</v>
-      </c>
-      <c r="W12" s="20">
+      <c r="W12" s="7">
+        <v>0</v>
+      </c>
+      <c r="X12" s="20">
         <v>418</v>
       </c>
     </row>
-    <row r="13" spans="1:77" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:78" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F13" s="9">
         <v>114</v>
@@ -1622,7 +1739,7 @@
         <v>16.384</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I13" s="10">
         <v>40589</v>
@@ -1637,49 +1754,52 @@
         <v>41053</v>
       </c>
       <c r="M13" s="10"/>
-      <c r="N13" s="9">
+      <c r="N13" s="50">
         <v>114056</v>
       </c>
-      <c r="O13" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="P13">
+      <c r="O13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13">
         <v>10384</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>2757</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>5054</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>95861</v>
       </c>
-      <c r="T13" s="17">
+      <c r="U13" s="17">
         <v>48</v>
       </c>
-      <c r="U13" s="9">
+      <c r="V13" s="9">
         <v>5336</v>
       </c>
-      <c r="V13" s="9">
+      <c r="W13" s="9">
         <v>4558</v>
       </c>
-      <c r="W13" s="21">
+      <c r="X13" s="21">
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:77" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:78" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F14" s="11">
         <v>35</v>
@@ -1688,7 +1808,7 @@
         <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I14" s="12">
         <v>41557</v>
@@ -1703,52 +1823,55 @@
         <v>41673</v>
       </c>
       <c r="M14" s="12"/>
-      <c r="N14" s="11">
+      <c r="N14" s="51">
         <v>44818</v>
       </c>
-      <c r="O14" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="P14">
+      <c r="O14" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14">
         <v>6886</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="R14" s="3">
         <v>10696</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>1178</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>26058</v>
       </c>
-      <c r="T14" s="18">
-        <v>0</v>
-      </c>
-      <c r="U14" s="11">
+      <c r="U14" s="18">
+        <v>0</v>
+      </c>
+      <c r="V14" s="11">
         <v>2309</v>
       </c>
-      <c r="V14" s="11">
+      <c r="W14" s="11">
         <v>3501</v>
       </c>
-      <c r="W14" s="22">
+      <c r="X14" s="22">
         <v>947</v>
       </c>
     </row>
-    <row r="15" spans="1:77" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:78" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F15" s="9">
         <v>55</v>
@@ -1772,49 +1895,52 @@
         <v>44741</v>
       </c>
       <c r="M15" s="10"/>
-      <c r="N15" s="9">
+      <c r="N15" s="50">
         <v>3129</v>
       </c>
-      <c r="O15" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="P15" s="9">
+      <c r="O15" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="P15" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="9">
         <v>2668</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="R15" s="9">
         <v>33</v>
       </c>
-      <c r="R15" s="9">
+      <c r="S15" s="9">
         <v>297</v>
       </c>
-      <c r="S15" s="9">
-        <v>0</v>
-      </c>
-      <c r="T15" s="16">
+      <c r="T15" s="9">
+        <v>0</v>
+      </c>
+      <c r="U15" s="16">
         <v>1610</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>694</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>364</v>
       </c>
-      <c r="W15" s="21">
+      <c r="X15" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:77" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:78" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F16" s="14">
         <v>72</v>
@@ -1823,7 +1949,7 @@
         <v>256</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I16" s="5">
         <v>44443</v>
@@ -1838,49 +1964,52 @@
         <v>44470</v>
       </c>
       <c r="M16" s="6"/>
-      <c r="N16" s="14">
+      <c r="N16" s="52">
         <v>4967</v>
       </c>
-      <c r="O16" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="P16" s="14">
+      <c r="O16" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="P16" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q16" s="14">
         <v>4777</v>
       </c>
-      <c r="Q16" s="14">
-        <v>0</v>
-      </c>
       <c r="R16" s="14">
+        <v>0</v>
+      </c>
+      <c r="S16" s="14">
         <v>190</v>
       </c>
-      <c r="S16" s="14">
+      <c r="T16" s="14">
         <v>131</v>
       </c>
-      <c r="T16" s="16">
+      <c r="U16" s="16">
         <v>4184</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>593</v>
       </c>
-      <c r="V16" s="14">
-        <v>0</v>
-      </c>
-      <c r="W16" s="19">
+      <c r="W16" s="14">
+        <v>0</v>
+      </c>
+      <c r="X16" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F17" s="14">
         <v>72</v>
@@ -1889,7 +2018,7 @@
         <v>256</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I17" s="5">
         <v>44513</v>
@@ -1904,49 +2033,52 @@
         <v>44528</v>
       </c>
       <c r="M17" s="6"/>
-      <c r="N17" s="14">
+      <c r="N17" s="52">
         <v>367</v>
       </c>
-      <c r="O17" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="P17" s="14">
+      <c r="O17" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="P17" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q17" s="14">
         <v>324</v>
       </c>
-      <c r="Q17" s="14">
-        <v>0</v>
-      </c>
       <c r="R17" s="14">
+        <v>0</v>
+      </c>
+      <c r="S17" s="14">
         <v>1</v>
       </c>
-      <c r="S17" s="14">
+      <c r="T17" s="14">
         <v>42</v>
       </c>
-      <c r="T17" s="39">
-        <v>0</v>
-      </c>
-      <c r="U17">
+      <c r="U17" s="39">
+        <v>0</v>
+      </c>
+      <c r="V17">
         <v>324</v>
       </c>
-      <c r="V17" s="27">
-        <v>0</v>
-      </c>
-      <c r="W17" s="19">
+      <c r="W17" s="27">
+        <v>0</v>
+      </c>
+      <c r="X17" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F18" s="14">
         <v>193</v>
@@ -1955,7 +2087,7 @@
         <v>256</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I18" s="5">
         <v>44444</v>
@@ -1970,49 +2102,52 @@
         <v>44518</v>
       </c>
       <c r="M18" s="6"/>
-      <c r="N18" s="14">
+      <c r="N18" s="52">
         <v>574</v>
       </c>
-      <c r="O18" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="P18" s="14">
+      <c r="O18" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="P18" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q18" s="14">
         <v>350</v>
       </c>
-      <c r="Q18" s="14">
-        <v>0</v>
-      </c>
       <c r="R18" s="14">
+        <v>0</v>
+      </c>
+      <c r="S18" s="14">
         <v>3</v>
       </c>
-      <c r="S18" s="14">
+      <c r="T18" s="14">
         <v>221</v>
       </c>
-      <c r="T18" s="16">
+      <c r="U18" s="16">
         <v>159</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>191</v>
       </c>
-      <c r="V18" s="27">
-        <v>0</v>
-      </c>
-      <c r="W18" s="19">
+      <c r="W18" s="27">
+        <v>0</v>
+      </c>
+      <c r="X18" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F19" s="14">
         <v>193</v>
@@ -2021,7 +2156,7 @@
         <v>256</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I19" s="5">
         <v>44528</v>
@@ -2036,49 +2171,52 @@
         <v>44455</v>
       </c>
       <c r="M19" s="6"/>
-      <c r="N19" s="14">
+      <c r="N19" s="52">
         <v>2407</v>
       </c>
-      <c r="O19" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="P19" s="14">
+      <c r="O19" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="P19" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q19" s="14">
         <v>2141</v>
       </c>
-      <c r="Q19" s="14">
-        <v>0</v>
-      </c>
       <c r="R19" s="14">
+        <v>0</v>
+      </c>
+      <c r="S19" s="14">
         <v>152</v>
       </c>
-      <c r="S19" s="14">
+      <c r="T19" s="14">
         <v>114</v>
       </c>
-      <c r="T19" s="16">
+      <c r="U19" s="16">
         <v>2070</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>71</v>
       </c>
-      <c r="V19" s="27">
-        <v>0</v>
-      </c>
-      <c r="W19" s="19">
+      <c r="W19" s="27">
+        <v>0</v>
+      </c>
+      <c r="X19" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F20" s="11">
         <v>245</v>
@@ -2087,7 +2225,7 @@
         <v>256</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I20" s="15">
         <v>44511</v>
@@ -2102,46 +2240,49 @@
         <v>44570</v>
       </c>
       <c r="M20" s="12"/>
-      <c r="N20" s="11">
+      <c r="N20" s="51">
         <v>7698</v>
       </c>
-      <c r="O20" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="P20" s="11">
+      <c r="O20" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="P20" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q20" s="11">
         <v>5655</v>
       </c>
-      <c r="Q20" s="11">
-        <v>0</v>
-      </c>
       <c r="R20" s="11">
+        <v>0</v>
+      </c>
+      <c r="S20" s="11">
         <v>383</v>
       </c>
-      <c r="S20" s="11">
+      <c r="T20" s="11">
         <v>1660</v>
       </c>
-      <c r="T20" s="16">
+      <c r="U20" s="16">
         <v>5630</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>25</v>
       </c>
-      <c r="V20" s="11">
-        <v>0</v>
-      </c>
-      <c r="W20" s="22">
+      <c r="W20" s="11">
+        <v>0</v>
+      </c>
+      <c r="X20" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" s="31">
         <v>48.686</v>
@@ -2156,7 +2297,7 @@
         <v>64</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
@@ -2167,40 +2308,46 @@
         <v>42651</v>
       </c>
       <c r="M21" s="10"/>
-      <c r="O21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P21" s="17">
+      <c r="N21" s="50">
+        <v>8340</v>
+      </c>
+      <c r="O21" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q21" s="17">
         <v>7446</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="R21" s="9">
         <v>3</v>
       </c>
-      <c r="R21" s="9">
+      <c r="S21" s="9">
         <v>852</v>
       </c>
-      <c r="S21" s="9">
+      <c r="T21" s="9">
         <v>39</v>
       </c>
-      <c r="T21" s="17">
+      <c r="U21" s="17">
         <v>2574</v>
       </c>
-      <c r="U21" s="9">
+      <c r="V21" s="9">
         <v>937</v>
       </c>
-      <c r="V21" s="9">
-        <v>0</v>
-      </c>
-      <c r="W21" s="21">
+      <c r="W21" s="9">
+        <v>0</v>
+      </c>
+      <c r="X21" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D22" s="33">
         <v>48.506999999999998</v>
@@ -2215,7 +2362,7 @@
         <v>64</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
@@ -2226,40 +2373,46 @@
         <v>42777</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="O22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P22" s="16">
+      <c r="N22" s="53">
+        <v>17196</v>
+      </c>
+      <c r="O22" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="P22" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q22" s="16">
         <v>15788</v>
       </c>
-      <c r="Q22" s="14">
-        <v>0</v>
-      </c>
       <c r="R22" s="14">
+        <v>0</v>
+      </c>
+      <c r="S22" s="14">
         <v>1177</v>
       </c>
-      <c r="S22" s="14">
+      <c r="T22" s="14">
         <v>231</v>
       </c>
-      <c r="T22" s="16">
+      <c r="U22" s="16">
         <v>7647</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>318</v>
       </c>
-      <c r="V22" s="27">
-        <v>0</v>
-      </c>
-      <c r="W22" s="19">
+      <c r="W22" s="27">
+        <v>0</v>
+      </c>
+      <c r="X22" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D23" s="33">
         <v>48.494999999999997</v>
@@ -2274,7 +2427,7 @@
         <v>64</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
@@ -2285,40 +2438,46 @@
         <v>42416</v>
       </c>
       <c r="M23" s="6"/>
-      <c r="O23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P23" s="16">
+      <c r="N23" s="53">
+        <v>9434</v>
+      </c>
+      <c r="O23" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="P23" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q23" s="16">
         <v>3039</v>
       </c>
-      <c r="Q23" s="14">
-        <v>0</v>
-      </c>
       <c r="R23" s="14">
+        <v>0</v>
+      </c>
+      <c r="S23" s="14">
         <v>3311</v>
       </c>
-      <c r="S23" s="14">
+      <c r="T23" s="14">
         <v>1084</v>
       </c>
-      <c r="T23" s="16">
+      <c r="U23" s="16">
         <v>395</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>994</v>
       </c>
-      <c r="V23" s="27">
-        <v>0</v>
-      </c>
-      <c r="W23" s="19">
+      <c r="W23" s="27">
+        <v>0</v>
+      </c>
+      <c r="X23" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D24" s="32">
         <v>48.774999999999999</v>
@@ -2333,7 +2492,7 @@
         <v>64</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -2344,40 +2503,46 @@
         <v>42776</v>
       </c>
       <c r="M24" s="12"/>
-      <c r="O24" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="P24" s="18">
+      <c r="N24" s="51">
+        <v>1966</v>
+      </c>
+      <c r="O24" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="P24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q24" s="18">
         <v>1333</v>
       </c>
-      <c r="Q24" s="11">
-        <v>0</v>
-      </c>
       <c r="R24" s="11">
+        <v>0</v>
+      </c>
+      <c r="S24" s="11">
         <v>607</v>
       </c>
-      <c r="S24" s="11">
+      <c r="T24" s="11">
         <v>26</v>
       </c>
-      <c r="T24" s="16">
+      <c r="U24" s="16">
         <v>519</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <v>242</v>
       </c>
-      <c r="V24" s="11">
-        <v>0</v>
-      </c>
-      <c r="W24" s="22">
+      <c r="W24" s="11">
+        <v>0</v>
+      </c>
+      <c r="X24" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:23" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>79</v>
@@ -2395,7 +2560,7 @@
         <v>128</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -2406,104 +2571,107 @@
         <v>44736</v>
       </c>
       <c r="M25" s="8"/>
-      <c r="N25" s="7">
+      <c r="N25" s="49">
         <v>1342</v>
       </c>
-      <c r="O25" s="17" t="s">
+      <c r="O25" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="P25" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q25" s="17">
+        <v>1242</v>
+      </c>
+      <c r="R25" s="9">
         <v>23</v>
       </c>
-      <c r="P25" s="17">
-        <v>1242</v>
-      </c>
-      <c r="Q25" s="9">
-        <v>23</v>
-      </c>
-      <c r="R25" s="9">
-        <v>0</v>
-      </c>
       <c r="S25" s="9">
         <v>0</v>
       </c>
-      <c r="T25" s="17">
+      <c r="T25" s="9">
+        <v>0</v>
+      </c>
+      <c r="U25" s="17">
         <v>1189</v>
       </c>
-      <c r="U25" s="9">
-        <v>0</v>
-      </c>
       <c r="V25" s="9">
         <v>0</v>
       </c>
-      <c r="W25" s="21">
+      <c r="W25" s="9">
+        <v>0</v>
+      </c>
+      <c r="X25" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="O26" s="41"/>
-      <c r="P26" s="42" t="s">
+    <row r="26" spans="1:24" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P26" s="41"/>
+      <c r="Q26" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="Q26" s="43" t="s">
+      <c r="R26" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="R26" s="43" t="s">
+      <c r="S26" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="S26" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="T26" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="U26" s="43" t="s">
+      <c r="T26" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="U26" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="V26" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="W26" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="V26" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>56</v>
+      <c r="X26" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="O27" s="44" t="s">
+    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P27" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="P27" s="45">
-        <f>SUM(P3:P25)</f>
+      <c r="Q27" s="45">
+        <f>SUM(Q3:Q25)</f>
         <v>65443</v>
       </c>
-      <c r="Q27" s="46">
-        <f t="shared" ref="Q27:W27" si="0">SUM(Q3:Q25)</f>
+      <c r="R27" s="46">
+        <f t="shared" ref="R27:X27" si="0">SUM(R3:R25)</f>
         <v>22904</v>
       </c>
-      <c r="R27" s="46">
-        <f>SUM(R3:R25)</f>
+      <c r="S27" s="46">
+        <f>SUM(S3:S25)</f>
         <v>13975</v>
       </c>
-      <c r="S27" s="46">
+      <c r="T27" s="46">
         <f t="shared" si="0"/>
         <v>128413</v>
       </c>
-      <c r="T27" s="45">
+      <c r="U27" s="45">
         <f t="shared" si="0"/>
         <v>27939</v>
       </c>
-      <c r="U27" s="46">
+      <c r="V27" s="46">
         <f t="shared" si="0"/>
         <v>12868</v>
       </c>
-      <c r="V27" s="46">
+      <c r="W27" s="46">
         <f t="shared" si="0"/>
         <v>8423</v>
       </c>
-      <c r="W27" s="2">
+      <c r="X27" s="2">
         <f t="shared" si="0"/>
         <v>1623</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="O1:W1"/>
+    <mergeCell ref="P1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bugs add K. Fraiser A. Liu data into summary
</commit_message>
<xml_diff>
--- a/Documentation/Summary.xlsx
+++ b/Documentation/Summary.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaitlin.palmer\Documents\GitHub\DCLDE2026\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB6EC96-D46C-45EC-9691-4F013489CFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5414999B-C927-487F-B3F0-692FDAC1532A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="324" yWindow="564" windowWidth="20556" windowHeight="11280" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
+    <workbookView xWindow="2616" yWindow="648" windowWidth="20556" windowHeight="11280" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="107">
   <si>
     <t>Annotations</t>
   </si>
@@ -304,6 +306,57 @@
   </si>
   <si>
     <t>Pre Processing Detection</t>
+  </si>
+  <si>
+    <t>Annotations Start</t>
+  </si>
+  <si>
+    <t>Annotations Finish</t>
+  </si>
+  <si>
+    <t>Species/Class Annotations</t>
+  </si>
+  <si>
+    <t>Ecotype/Population Annotations</t>
+  </si>
+  <si>
+    <t>Call (KW)/ File (All Else)</t>
+  </si>
+  <si>
+    <t>DFO WDLP</t>
+  </si>
+  <si>
+    <t>DFO CRP</t>
+  </si>
+  <si>
+    <t>SIO</t>
+  </si>
+  <si>
+    <t>Cape Elizabeth</t>
+  </si>
+  <si>
+    <t>Quinault Canyon</t>
+  </si>
+  <si>
+    <t>CE_01</t>
+  </si>
+  <si>
+    <t>CE_02</t>
+  </si>
+  <si>
+    <t>CE_03</t>
+  </si>
+  <si>
+    <t>QE_01</t>
+  </si>
+  <si>
+    <t>QE_02</t>
+  </si>
+  <si>
+    <t>QE_03</t>
+  </si>
+  <si>
+    <t>HARP</t>
   </si>
 </sst>
 </file>
@@ -352,7 +405,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -615,11 +668,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -711,9 +779,22 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4A8866-C81C-482A-B0A6-264BECA1C8D5}">
-  <dimension ref="A1:BZ27"/>
+  <dimension ref="A1:BZ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,17 +1139,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="P1" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
+      <c r="P1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
     </row>
     <row r="2" spans="1:78" s="23" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
@@ -1685,6 +1766,9 @@
       <c r="E11" s="27">
         <v>-122.76</v>
       </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
       <c r="G11">
         <v>32</v>
       </c>
@@ -1798,7 +1882,7 @@
     </row>
     <row r="13" spans="1:78" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>11</v>
@@ -1939,7 +2023,7 @@
     </row>
     <row r="15" spans="1:78" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>39</v>
@@ -2617,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>21</v>
       </c>
@@ -2685,68 +2769,313 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="P26" s="40"/>
-      <c r="Q26" s="41" t="s">
+    <row r="26" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="27">
+        <v>47.357999999999997</v>
+      </c>
+      <c r="E26" s="27">
+        <v>124.68333333333334</v>
+      </c>
+      <c r="F26" s="26">
+        <v>100</v>
+      </c>
+      <c r="G26" s="26">
+        <v>200</v>
+      </c>
+      <c r="H26" t="s">
+        <v>106</v>
+      </c>
+      <c r="K26" s="60">
+        <v>39616</v>
+      </c>
+      <c r="L26" s="60">
+        <v>39973</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="27">
+        <v>47.351999999999997</v>
+      </c>
+      <c r="E27" s="27">
+        <v>124.721</v>
+      </c>
+      <c r="F27" s="26">
+        <v>118</v>
+      </c>
+      <c r="G27" s="26">
+        <v>200</v>
+      </c>
+      <c r="H27" t="s">
+        <v>106</v>
+      </c>
+      <c r="K27" s="60">
+        <v>40684</v>
+      </c>
+      <c r="L27" s="60">
+        <v>40853</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="27">
+        <v>47.352333333333334</v>
+      </c>
+      <c r="E28" s="27">
+        <v>124.72133333333333</v>
+      </c>
+      <c r="F28" s="26">
+        <v>150</v>
+      </c>
+      <c r="G28" s="26">
+        <v>200</v>
+      </c>
+      <c r="H28" t="s">
+        <v>106</v>
+      </c>
+      <c r="K28" s="60">
+        <v>40884</v>
+      </c>
+      <c r="L28" s="60">
+        <v>40925</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="27">
+        <v>47.5</v>
+      </c>
+      <c r="E29" s="27">
+        <v>125.35333333333334</v>
+      </c>
+      <c r="F29" s="26">
+        <v>1400</v>
+      </c>
+      <c r="G29" s="26">
+        <v>200</v>
+      </c>
+      <c r="H29" t="s">
+        <v>106</v>
+      </c>
+      <c r="K29" s="60">
+        <v>40570</v>
+      </c>
+      <c r="L29" s="60">
+        <v>40823</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="27">
+        <v>47.500500000000002</v>
+      </c>
+      <c r="E30" s="27">
+        <v>125.3535</v>
+      </c>
+      <c r="F30" s="26">
+        <v>1394</v>
+      </c>
+      <c r="G30" s="26">
+        <v>200</v>
+      </c>
+      <c r="H30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K30" s="60">
+        <v>40736</v>
+      </c>
+      <c r="L30" s="60">
+        <v>41101</v>
+      </c>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="R26" s="42" t="s">
+      <c r="R30" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="S26" s="42" t="s">
+      <c r="S30" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="T26" s="42" t="s">
+      <c r="T30" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="U26" s="41" t="s">
+      <c r="U30" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="V26" s="42" t="s">
+      <c r="V30" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="W26" s="42" t="s">
+      <c r="W30" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="X26" s="1" t="s">
+      <c r="X30" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="P27" s="43" t="s">
+    <row r="31" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="27">
+        <v>47.500500000000002</v>
+      </c>
+      <c r="E31" s="27">
+        <v>125.35366666666667</v>
+      </c>
+      <c r="F31" s="26">
+        <v>1394</v>
+      </c>
+      <c r="G31" s="26">
+        <v>200</v>
+      </c>
+      <c r="H31" t="s">
+        <v>106</v>
+      </c>
+      <c r="K31" s="60">
+        <v>41166</v>
+      </c>
+      <c r="L31" s="60">
+        <v>41455</v>
+      </c>
+      <c r="P31" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="Q27" s="44">
-        <f>SUM(Q3:Q25)</f>
+      <c r="Q31" s="44">
+        <f>SUM(Q3:Q29)</f>
         <v>67779</v>
       </c>
-      <c r="R27" s="45">
-        <f t="shared" ref="R27:X27" si="0">SUM(R3:R25)</f>
+      <c r="R31" s="44">
+        <f t="shared" ref="R31:X31" si="0">SUM(R3:R29)</f>
         <v>22902</v>
       </c>
-      <c r="S27" s="45">
-        <f>SUM(S3:S25)</f>
+      <c r="S31" s="44">
+        <f t="shared" si="0"/>
         <v>13975</v>
       </c>
-      <c r="T27" s="45">
+      <c r="T31" s="44">
         <f t="shared" si="0"/>
         <v>128413</v>
       </c>
-      <c r="U27" s="44">
+      <c r="U31" s="44">
         <f t="shared" si="0"/>
         <v>30168</v>
       </c>
-      <c r="V27" s="45">
+      <c r="V31" s="44">
         <f t="shared" si="0"/>
         <v>12868</v>
       </c>
-      <c r="W27" s="45">
+      <c r="W31" s="44">
         <f t="shared" si="0"/>
         <v>8423</v>
       </c>
-      <c r="X27" s="2">
+      <c r="X31" s="44">
         <f t="shared" si="0"/>
         <v>1623</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>124</v>
+      </c>
+      <c r="D37" s="27">
+        <v>41</v>
+      </c>
+      <c r="E37" s="27">
+        <f>C37+(D37/60)</f>
+        <v>124.68333333333334</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>124</v>
+      </c>
+      <c r="D38" s="27">
+        <v>43.26</v>
+      </c>
+      <c r="E38" s="27">
+        <f t="shared" ref="E38:E42" si="1">C38+(D38/60)</f>
+        <v>124.721</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>124</v>
+      </c>
+      <c r="D39" s="27">
+        <v>43.28</v>
+      </c>
+      <c r="E39" s="27">
+        <f t="shared" si="1"/>
+        <v>124.72133333333333</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>125</v>
+      </c>
+      <c r="D40" s="27">
+        <v>21.2</v>
+      </c>
+      <c r="E40" s="27">
+        <f t="shared" si="1"/>
+        <v>125.35333333333334</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>125</v>
+      </c>
+      <c r="D41" s="27">
+        <v>21.21</v>
+      </c>
+      <c r="E41" s="27">
+        <f t="shared" si="1"/>
+        <v>125.3535</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>125</v>
+      </c>
+      <c r="D42" s="27">
+        <v>21.22</v>
+      </c>
+      <c r="E42" s="27">
+        <f t="shared" si="1"/>
+        <v>125.35366666666667</v>
       </c>
     </row>
   </sheetData>
@@ -2756,4 +3085,1759 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114EE0BB-9430-4707-8294-22F3EA198BF4}">
+  <dimension ref="A1:N54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:N52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="9" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.109375" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" customWidth="1"/>
+    <col min="13" max="13" width="6.5546875" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="24"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="27">
+        <v>48.5248469</v>
+      </c>
+      <c r="E3" s="27">
+        <v>-123.15916470000001</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>32</v>
+      </c>
+      <c r="I3" s="5">
+        <v>44101</v>
+      </c>
+      <c r="J3" s="5">
+        <v>43651</v>
+      </c>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="27">
+        <v>48.5248469</v>
+      </c>
+      <c r="E4" s="27">
+        <v>-123.15916470000001</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>32</v>
+      </c>
+      <c r="I4" s="5">
+        <v>44081</v>
+      </c>
+      <c r="J4" s="5">
+        <v>43005</v>
+      </c>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="27">
+        <v>48.5248469</v>
+      </c>
+      <c r="E5" s="27">
+        <v>-123.15916470000001</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>32</v>
+      </c>
+      <c r="I5" s="5">
+        <v>44082</v>
+      </c>
+      <c r="J5" s="5">
+        <v>44037</v>
+      </c>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="27">
+        <v>48.5248469</v>
+      </c>
+      <c r="E6" s="27">
+        <v>-123.15916470000001</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>32</v>
+      </c>
+      <c r="I6" s="5">
+        <v>43651</v>
+      </c>
+      <c r="J6" s="5">
+        <v>44075</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="27">
+        <v>48.5248469</v>
+      </c>
+      <c r="E7" s="27">
+        <v>-123.15916470000001</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>32</v>
+      </c>
+      <c r="I7" s="5">
+        <v>43005</v>
+      </c>
+      <c r="J7" s="5">
+        <v>44081</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="27">
+        <v>48.135399999999997</v>
+      </c>
+      <c r="E8" s="27">
+        <v>-122.76</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>32</v>
+      </c>
+      <c r="I8" s="5">
+        <v>44037</v>
+      </c>
+      <c r="J8" s="5">
+        <v>44103</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="27">
+        <v>48.0310074</v>
+      </c>
+      <c r="E9" s="27">
+        <v>-122.6082001</v>
+      </c>
+      <c r="F9">
+        <v>12.5</v>
+      </c>
+      <c r="G9">
+        <v>32</v>
+      </c>
+      <c r="I9" s="5">
+        <v>44075</v>
+      </c>
+      <c r="J9" s="5">
+        <v>44102</v>
+      </c>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="27">
+        <v>48.0310074</v>
+      </c>
+      <c r="E10" s="27">
+        <v>-122.6082001</v>
+      </c>
+      <c r="F10">
+        <v>12.5</v>
+      </c>
+      <c r="G10">
+        <v>32</v>
+      </c>
+      <c r="I10" s="5">
+        <v>44079</v>
+      </c>
+      <c r="J10" s="5">
+        <v>44122</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="27">
+        <v>48.135399999999997</v>
+      </c>
+      <c r="E11" s="27">
+        <v>-122.76</v>
+      </c>
+      <c r="G11">
+        <v>32</v>
+      </c>
+      <c r="I11" s="5">
+        <v>44103</v>
+      </c>
+      <c r="J11" s="5">
+        <v>44112</v>
+      </c>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="29">
+        <v>48.426000000000002</v>
+      </c>
+      <c r="E12" s="29">
+        <v>126.17400000000001</v>
+      </c>
+      <c r="F12" s="7">
+        <v>40</v>
+      </c>
+      <c r="G12" s="7">
+        <v>64</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="36">
+        <v>41414</v>
+      </c>
+      <c r="J12" s="8">
+        <v>41977</v>
+      </c>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="9">
+        <v>114</v>
+      </c>
+      <c r="G13" s="9">
+        <v>16.384</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="13">
+        <v>40681</v>
+      </c>
+      <c r="J13" s="10">
+        <v>41053</v>
+      </c>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="11">
+        <v>35</v>
+      </c>
+      <c r="G14" s="11">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="15">
+        <v>41557</v>
+      </c>
+      <c r="J14" s="12">
+        <v>41673</v>
+      </c>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="9">
+        <v>55</v>
+      </c>
+      <c r="G15" s="9">
+        <v>192</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="13">
+        <v>44628</v>
+      </c>
+      <c r="J15" s="13">
+        <v>44741</v>
+      </c>
+      <c r="K15" s="13"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="14">
+        <v>72</v>
+      </c>
+      <c r="G16" s="14">
+        <v>256</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="5">
+        <v>44444</v>
+      </c>
+      <c r="J16" s="5">
+        <v>44470</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="14">
+        <v>72</v>
+      </c>
+      <c r="G17" s="14">
+        <v>256</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="5">
+        <v>44527</v>
+      </c>
+      <c r="J17" s="5">
+        <v>44528</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="14">
+        <v>193</v>
+      </c>
+      <c r="G18" s="14">
+        <v>256</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="5">
+        <v>44511</v>
+      </c>
+      <c r="J18" s="5">
+        <v>44518</v>
+      </c>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="14">
+        <v>193</v>
+      </c>
+      <c r="G19" s="14">
+        <v>256</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="5">
+        <v>44443</v>
+      </c>
+      <c r="J19" s="5">
+        <v>44455</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="11">
+        <v>245</v>
+      </c>
+      <c r="G20" s="11">
+        <v>256</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="15">
+        <v>44513</v>
+      </c>
+      <c r="J20" s="15">
+        <v>44570</v>
+      </c>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="30">
+        <v>48.686</v>
+      </c>
+      <c r="E21" s="30">
+        <v>123.274</v>
+      </c>
+      <c r="F21" s="9">
+        <v>237</v>
+      </c>
+      <c r="G21" s="9">
+        <v>64</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="5">
+        <v>42291</v>
+      </c>
+      <c r="J21" s="10">
+        <v>42651</v>
+      </c>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="32">
+        <v>48.506999999999998</v>
+      </c>
+      <c r="E22" s="32">
+        <v>123.211</v>
+      </c>
+      <c r="F22" s="14">
+        <v>188</v>
+      </c>
+      <c r="G22" s="14">
+        <v>64</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="5">
+        <v>42292</v>
+      </c>
+      <c r="J22" s="6">
+        <v>42777</v>
+      </c>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="32">
+        <v>48.494999999999997</v>
+      </c>
+      <c r="E23" s="32">
+        <v>124.54</v>
+      </c>
+      <c r="F23" s="14">
+        <v>213</v>
+      </c>
+      <c r="G23" s="14">
+        <v>64</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" s="5">
+        <v>42291</v>
+      </c>
+      <c r="J23" s="6">
+        <v>42416</v>
+      </c>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="31">
+        <v>48.774999999999999</v>
+      </c>
+      <c r="E24" s="31">
+        <v>123.343</v>
+      </c>
+      <c r="F24" s="11">
+        <v>74</v>
+      </c>
+      <c r="G24" s="11">
+        <v>64</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="5">
+        <v>42416</v>
+      </c>
+      <c r="J24" s="12">
+        <v>42776</v>
+      </c>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="29">
+        <v>48.78</v>
+      </c>
+      <c r="E25" s="29">
+        <v>123.05200000000001</v>
+      </c>
+      <c r="F25" s="7">
+        <v>27</v>
+      </c>
+      <c r="G25" s="7">
+        <v>128</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="36">
+        <v>44736</v>
+      </c>
+      <c r="J25" s="8">
+        <v>44736</v>
+      </c>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="52" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="53" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D53" s="46"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="H53" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="I53" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="J53" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="K53" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="L53" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="M53" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D54" s="46"/>
+      <c r="F54" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="G54" s="44">
+        <f>SUM(Sheet3!E3:E25)</f>
+        <v>67779</v>
+      </c>
+      <c r="H54" s="45">
+        <f>SUM(Sheet3!F3:F25)</f>
+        <v>22902</v>
+      </c>
+      <c r="I54" s="45">
+        <f>SUM(Sheet3!G3:G25)</f>
+        <v>13975</v>
+      </c>
+      <c r="J54" s="45">
+        <f>SUM(Sheet3!H3:H25)</f>
+        <v>128413</v>
+      </c>
+      <c r="K54" s="44">
+        <f>SUM(Sheet3!I3:I25)</f>
+        <v>30168</v>
+      </c>
+      <c r="L54" s="45">
+        <f>SUM(Sheet3!J3:J25)</f>
+        <v>12868</v>
+      </c>
+      <c r="M54" s="45">
+        <f>SUM(Sheet3!K3:K25)</f>
+        <v>8423</v>
+      </c>
+      <c r="N54" s="2">
+        <f>SUM(Sheet3!L3:L25)</f>
+        <v>1623</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C891EA49-1228-4754-8524-0795D1247222}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L25" sqref="A1:L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="53"/>
+      <c r="E1" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+    </row>
+    <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="16">
+        <v>435</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>11</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0</v>
+      </c>
+      <c r="I3" s="16">
+        <v>435</v>
+      </c>
+      <c r="J3" s="14">
+        <v>0</v>
+      </c>
+      <c r="K3" s="14">
+        <v>0</v>
+      </c>
+      <c r="L3" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="16">
+        <v>436</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0</v>
+      </c>
+      <c r="I4" s="16">
+        <v>436</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0</v>
+      </c>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>31</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0</v>
+      </c>
+      <c r="I5" s="38">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="16">
+        <v>151</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="16">
+        <v>151</v>
+      </c>
+      <c r="J6" s="14">
+        <v>0</v>
+      </c>
+      <c r="K6" s="14">
+        <v>0</v>
+      </c>
+      <c r="L6" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>167</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0</v>
+      </c>
+      <c r="I7" s="38">
+        <v>0</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0</v>
+      </c>
+      <c r="K7" s="14">
+        <v>0</v>
+      </c>
+      <c r="L7" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="16">
+        <v>198</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>89</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="16">
+        <v>198</v>
+      </c>
+      <c r="J8" s="14">
+        <v>0</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="16">
+        <v>510</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>113</v>
+      </c>
+      <c r="H9" s="14">
+        <v>0</v>
+      </c>
+      <c r="I9" s="16">
+        <v>510</v>
+      </c>
+      <c r="J9" s="14">
+        <v>0</v>
+      </c>
+      <c r="K9" s="14">
+        <v>0</v>
+      </c>
+      <c r="L9" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>118</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0</v>
+      </c>
+      <c r="I10" s="38">
+        <v>0</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0</v>
+      </c>
+      <c r="K10" s="14">
+        <v>0</v>
+      </c>
+      <c r="L10" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="16">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0</v>
+      </c>
+      <c r="I11" s="16">
+        <v>54</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0</v>
+      </c>
+      <c r="K11" s="14">
+        <v>0</v>
+      </c>
+      <c r="L11" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="54">
+        <v>1626</v>
+      </c>
+      <c r="F12" s="7">
+        <v>9392</v>
+      </c>
+      <c r="G12" s="7">
+        <v>156</v>
+      </c>
+      <c r="H12" s="7">
+        <v>2946</v>
+      </c>
+      <c r="I12" s="39">
+        <v>130</v>
+      </c>
+      <c r="J12" s="7">
+        <v>834</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0</v>
+      </c>
+      <c r="L12" s="20">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="16">
+        <v>10384</v>
+      </c>
+      <c r="F13">
+        <v>2757</v>
+      </c>
+      <c r="G13">
+        <v>5054</v>
+      </c>
+      <c r="H13">
+        <v>95861</v>
+      </c>
+      <c r="I13" s="17">
+        <v>48</v>
+      </c>
+      <c r="J13" s="9">
+        <v>5336</v>
+      </c>
+      <c r="K13" s="9">
+        <v>4558</v>
+      </c>
+      <c r="L13" s="21">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="16">
+        <v>6886</v>
+      </c>
+      <c r="F14" s="3">
+        <v>10696</v>
+      </c>
+      <c r="G14">
+        <v>1178</v>
+      </c>
+      <c r="H14">
+        <v>26058</v>
+      </c>
+      <c r="I14" s="18">
+        <v>0</v>
+      </c>
+      <c r="J14" s="11">
+        <v>2309</v>
+      </c>
+      <c r="K14" s="11">
+        <v>3501</v>
+      </c>
+      <c r="L14" s="22">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="17">
+        <v>2668</v>
+      </c>
+      <c r="F15" s="9">
+        <v>33</v>
+      </c>
+      <c r="G15" s="9">
+        <v>297</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
+      <c r="I15" s="16">
+        <v>1610</v>
+      </c>
+      <c r="J15">
+        <v>694</v>
+      </c>
+      <c r="K15">
+        <v>364</v>
+      </c>
+      <c r="L15" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="16">
+        <v>4777</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0</v>
+      </c>
+      <c r="G16" s="14">
+        <v>190</v>
+      </c>
+      <c r="H16" s="14">
+        <v>131</v>
+      </c>
+      <c r="I16" s="16">
+        <v>4184</v>
+      </c>
+      <c r="J16">
+        <v>593</v>
+      </c>
+      <c r="K16" s="14">
+        <v>0</v>
+      </c>
+      <c r="L16" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="16">
+        <v>324</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0</v>
+      </c>
+      <c r="G17" s="14">
+        <v>1</v>
+      </c>
+      <c r="H17" s="14">
+        <v>42</v>
+      </c>
+      <c r="I17" s="38">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>324</v>
+      </c>
+      <c r="K17" s="26">
+        <v>0</v>
+      </c>
+      <c r="L17" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="14">
+        <v>350</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0</v>
+      </c>
+      <c r="G18" s="14">
+        <v>3</v>
+      </c>
+      <c r="H18" s="14">
+        <v>221</v>
+      </c>
+      <c r="I18" s="16">
+        <v>159</v>
+      </c>
+      <c r="J18">
+        <v>191</v>
+      </c>
+      <c r="K18" s="26">
+        <v>0</v>
+      </c>
+      <c r="L18" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="14">
+        <v>2141</v>
+      </c>
+      <c r="F19" s="14">
+        <v>0</v>
+      </c>
+      <c r="G19" s="14">
+        <v>152</v>
+      </c>
+      <c r="H19" s="14">
+        <v>114</v>
+      </c>
+      <c r="I19" s="16">
+        <v>2070</v>
+      </c>
+      <c r="J19">
+        <v>71</v>
+      </c>
+      <c r="K19" s="26">
+        <v>0</v>
+      </c>
+      <c r="L19" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="11">
+        <v>5655</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <v>383</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1660</v>
+      </c>
+      <c r="I20" s="16">
+        <v>5630</v>
+      </c>
+      <c r="J20">
+        <v>25</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0</v>
+      </c>
+      <c r="L20" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="17">
+        <v>7446</v>
+      </c>
+      <c r="F21" s="9">
+        <v>3</v>
+      </c>
+      <c r="G21" s="9">
+        <v>852</v>
+      </c>
+      <c r="H21" s="9">
+        <v>39</v>
+      </c>
+      <c r="I21" s="17">
+        <v>2574</v>
+      </c>
+      <c r="J21" s="9">
+        <v>937</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="16">
+        <v>15788</v>
+      </c>
+      <c r="F22" s="14">
+        <v>0</v>
+      </c>
+      <c r="G22" s="14">
+        <v>1177</v>
+      </c>
+      <c r="H22" s="14">
+        <v>231</v>
+      </c>
+      <c r="I22" s="16">
+        <v>7647</v>
+      </c>
+      <c r="J22">
+        <v>318</v>
+      </c>
+      <c r="K22" s="26">
+        <v>0</v>
+      </c>
+      <c r="L22" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="16">
+        <v>3039</v>
+      </c>
+      <c r="F23" s="14">
+        <v>0</v>
+      </c>
+      <c r="G23" s="14">
+        <v>3311</v>
+      </c>
+      <c r="H23" s="14">
+        <v>1084</v>
+      </c>
+      <c r="I23" s="16">
+        <v>395</v>
+      </c>
+      <c r="J23">
+        <v>994</v>
+      </c>
+      <c r="K23" s="26">
+        <v>0</v>
+      </c>
+      <c r="L23" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="18">
+        <v>1333</v>
+      </c>
+      <c r="F24" s="11">
+        <v>0</v>
+      </c>
+      <c r="G24" s="11">
+        <v>607</v>
+      </c>
+      <c r="H24" s="11">
+        <v>26</v>
+      </c>
+      <c r="I24" s="18">
+        <v>519</v>
+      </c>
+      <c r="J24">
+        <v>242</v>
+      </c>
+      <c r="K24" s="11">
+        <v>0</v>
+      </c>
+      <c r="L24" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="56">
+        <v>3578</v>
+      </c>
+      <c r="F25" s="56">
+        <v>21</v>
+      </c>
+      <c r="G25" s="56">
+        <v>0</v>
+      </c>
+      <c r="H25" s="56">
+        <v>0</v>
+      </c>
+      <c r="I25" s="54">
+        <v>3418</v>
+      </c>
+      <c r="J25" s="56">
+        <v>0</v>
+      </c>
+      <c r="K25" s="56">
+        <v>0</v>
+      </c>
+      <c r="L25" s="57">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add in VPFA data to summary table
</commit_message>
<xml_diff>
--- a/Documentation/Summary.xlsx
+++ b/Documentation/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaitlin.palmer\Documents\GitHub\DCLDE2026\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5414999B-C927-487F-B3F0-692FDAC1532A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71775F0-A0D1-4EF2-9ED7-9489F0DA276A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="648" windowWidth="20556" windowHeight="11280" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
+    <workbookView xWindow="1092" yWindow="1140" windowWidth="20556" windowHeight="11280" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="120">
   <si>
     <t>Annotations</t>
   </si>
@@ -357,6 +357,45 @@
   </si>
   <si>
     <t>HARP</t>
+  </si>
+  <si>
+    <t>JASCO/VPFA</t>
+  </si>
+  <si>
+    <t>Haro Strait Northbound</t>
+  </si>
+  <si>
+    <t>Haro Strait Southbound</t>
+  </si>
+  <si>
+    <t>HS_N</t>
+  </si>
+  <si>
+    <t>HS_S</t>
+  </si>
+  <si>
+    <t>JASCO/VPFA/ONC</t>
+  </si>
+  <si>
+    <t>RobBnk</t>
+  </si>
+  <si>
+    <t>Boundary Pass</t>
+  </si>
+  <si>
+    <t>BndryPass</t>
+  </si>
+  <si>
+    <t>Roberts Bank/Strait of Georgia East</t>
+  </si>
+  <si>
+    <t>GeoSpectrum M8 Hydrophone Element (142)</t>
+  </si>
+  <si>
+    <t>AMAR 418</t>
+  </si>
+  <si>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
@@ -405,7 +444,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -683,11 +722,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -788,13 +836,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,26 +1159,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4A8866-C81C-482A-B0A6-264BECA1C8D5}">
-  <dimension ref="A1:BZ42"/>
+  <dimension ref="A1:BZ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26:L31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" style="27" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="27" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
     <col min="9" max="9" width="12.21875" style="4" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="4" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="10.5546875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="1.21875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="6.21875" style="4" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="13.44140625" style="46" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.44140625" customWidth="1"/>
     <col min="16" max="16" width="31.5546875" bestFit="1" customWidth="1"/>
@@ -1139,17 +1190,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="P1" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
+      <c r="P1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
     </row>
     <row r="2" spans="1:78" s="23" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
@@ -1247,6 +1298,9 @@
       <c r="G3">
         <v>32</v>
       </c>
+      <c r="H3" t="s">
+        <v>119</v>
+      </c>
       <c r="K3" s="5">
         <v>44101</v>
       </c>
@@ -1305,6 +1359,9 @@
       </c>
       <c r="G4">
         <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>119</v>
       </c>
       <c r="K4" s="5">
         <v>44081</v>
@@ -1418,6 +1475,9 @@
       <c r="G5">
         <v>32</v>
       </c>
+      <c r="H5" t="s">
+        <v>119</v>
+      </c>
       <c r="K5" s="5">
         <v>44082</v>
       </c>
@@ -1477,6 +1537,9 @@
       <c r="G6">
         <v>32</v>
       </c>
+      <c r="H6" t="s">
+        <v>119</v>
+      </c>
       <c r="K6" s="5">
         <v>43651</v>
       </c>
@@ -1536,6 +1599,9 @@
       <c r="G7">
         <v>32</v>
       </c>
+      <c r="H7" t="s">
+        <v>119</v>
+      </c>
       <c r="K7" s="5">
         <v>43005</v>
       </c>
@@ -1595,6 +1661,9 @@
       <c r="G8">
         <v>32</v>
       </c>
+      <c r="H8" t="s">
+        <v>119</v>
+      </c>
       <c r="K8" s="5">
         <v>44037</v>
       </c>
@@ -1654,6 +1723,9 @@
       <c r="G9">
         <v>32</v>
       </c>
+      <c r="H9" t="s">
+        <v>119</v>
+      </c>
       <c r="K9" s="5">
         <v>44075</v>
       </c>
@@ -1713,6 +1785,9 @@
       <c r="G10">
         <v>32</v>
       </c>
+      <c r="H10" t="s">
+        <v>119</v>
+      </c>
       <c r="K10" s="5">
         <v>44079</v>
       </c>
@@ -1771,6 +1846,9 @@
       </c>
       <c r="G11">
         <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>119</v>
       </c>
       <c r="K11" s="5">
         <v>44103</v>
@@ -2794,10 +2872,10 @@
       <c r="H26" t="s">
         <v>106</v>
       </c>
-      <c r="K26" s="60">
+      <c r="K26" s="58">
         <v>39616</v>
       </c>
-      <c r="L26" s="60">
+      <c r="L26" s="58">
         <v>39973</v>
       </c>
     </row>
@@ -2823,10 +2901,10 @@
       <c r="H27" t="s">
         <v>106</v>
       </c>
-      <c r="K27" s="60">
+      <c r="K27" s="58">
         <v>40684</v>
       </c>
-      <c r="L27" s="60">
+      <c r="L27" s="58">
         <v>40853</v>
       </c>
     </row>
@@ -2852,14 +2930,14 @@
       <c r="H28" t="s">
         <v>106</v>
       </c>
-      <c r="K28" s="60">
+      <c r="K28" s="58">
         <v>40884</v>
       </c>
-      <c r="L28" s="60">
+      <c r="L28" s="58">
         <v>40925</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>99</v>
       </c>
@@ -2881,14 +2959,14 @@
       <c r="H29" t="s">
         <v>106</v>
       </c>
-      <c r="K29" s="60">
+      <c r="K29" s="58">
         <v>40570</v>
       </c>
-      <c r="L29" s="60">
+      <c r="L29" s="58">
         <v>40823</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>99</v>
       </c>
@@ -2910,39 +2988,14 @@
       <c r="H30" t="s">
         <v>106</v>
       </c>
-      <c r="K30" s="60">
+      <c r="K30" s="58">
         <v>40736</v>
       </c>
-      <c r="L30" s="60">
+      <c r="L30" s="58">
         <v>41101</v>
       </c>
-      <c r="P30" s="40"/>
-      <c r="Q30" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="R30" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="S30" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="T30" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="U30" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="V30" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="W30" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="X30" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>99</v>
       </c>
@@ -2964,117 +3017,241 @@
       <c r="H31" t="s">
         <v>106</v>
       </c>
-      <c r="K31" s="60">
+      <c r="K31" s="58">
         <v>41166</v>
       </c>
-      <c r="L31" s="60">
+      <c r="L31" s="58">
         <v>41455</v>
       </c>
-      <c r="P31" s="43" t="s">
+    </row>
+    <row r="32" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="9">
+        <v>48.518050000000002</v>
+      </c>
+      <c r="E32" s="9">
+        <v>-123.19166666666599</v>
+      </c>
+      <c r="F32" s="62">
+        <v>251</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="49"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33">
+        <v>48.5167</v>
+      </c>
+      <c r="E33">
+        <v>-123.207616666666</v>
+      </c>
+      <c r="F33">
+        <v>210</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34">
+        <v>48.760779999999997</v>
+      </c>
+      <c r="E34">
+        <v>-123.06793999999999</v>
+      </c>
+      <c r="F34">
+        <v>193</v>
+      </c>
+      <c r="G34">
+        <v>128</v>
+      </c>
+      <c r="H34" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="27">
+        <v>49.042645</v>
+      </c>
+      <c r="E35" s="27">
+        <v>-123.31744</v>
+      </c>
+      <c r="F35">
+        <v>168</v>
+      </c>
+      <c r="G35">
+        <v>64</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>124</v>
+      </c>
+      <c r="D38" s="27">
+        <v>41</v>
+      </c>
+      <c r="E38" s="27">
+        <f>C38+(D38/60)</f>
+        <v>124.68333333333334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>124</v>
+      </c>
+      <c r="D39" s="27">
+        <v>43.26</v>
+      </c>
+      <c r="E39" s="27">
+        <f t="shared" ref="E39:E43" si="0">C39+(D39/60)</f>
+        <v>124.721</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <v>124</v>
+      </c>
+      <c r="D40" s="27">
+        <v>43.28</v>
+      </c>
+      <c r="E40" s="27">
+        <f t="shared" si="0"/>
+        <v>124.72133333333333</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <v>125</v>
+      </c>
+      <c r="D41" s="27">
+        <v>21.2</v>
+      </c>
+      <c r="E41" s="27">
+        <f t="shared" si="0"/>
+        <v>125.35333333333334</v>
+      </c>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="R41" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="S41" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="T41" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="U41" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="V41" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="W41" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="X41" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>125</v>
+      </c>
+      <c r="D42" s="27">
+        <v>21.21</v>
+      </c>
+      <c r="E42" s="27">
+        <f t="shared" si="0"/>
+        <v>125.3535</v>
+      </c>
+      <c r="P42" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="Q31" s="44">
+      <c r="Q42" s="16">
         <f>SUM(Q3:Q29)</f>
         <v>67779</v>
       </c>
-      <c r="R31" s="44">
-        <f t="shared" ref="R31:X31" si="0">SUM(R3:R29)</f>
+      <c r="R42" s="16">
+        <f>SUM(R3:R29)</f>
         <v>22902</v>
       </c>
-      <c r="S31" s="44">
+      <c r="S42" s="16">
+        <f>SUM(S3:S29)</f>
+        <v>13975</v>
+      </c>
+      <c r="T42" s="16">
+        <f>SUM(T3:T29)</f>
+        <v>128413</v>
+      </c>
+      <c r="U42" s="16">
+        <f>SUM(U3:U29)</f>
+        <v>30168</v>
+      </c>
+      <c r="V42" s="16">
+        <f>SUM(V3:V29)</f>
+        <v>12868</v>
+      </c>
+      <c r="W42" s="16">
+        <f>SUM(W3:W29)</f>
+        <v>8423</v>
+      </c>
+      <c r="X42" s="16">
+        <f>SUM(X3:X29)</f>
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>125</v>
+      </c>
+      <c r="D43" s="27">
+        <v>21.22</v>
+      </c>
+      <c r="E43" s="27">
         <f t="shared" si="0"/>
-        <v>13975</v>
-      </c>
-      <c r="T31" s="44">
-        <f t="shared" si="0"/>
-        <v>128413</v>
-      </c>
-      <c r="U31" s="44">
-        <f t="shared" si="0"/>
-        <v>30168</v>
-      </c>
-      <c r="V31" s="44">
-        <f t="shared" si="0"/>
-        <v>12868</v>
-      </c>
-      <c r="W31" s="44">
-        <f t="shared" si="0"/>
-        <v>8423</v>
-      </c>
-      <c r="X31" s="44">
-        <f t="shared" si="0"/>
-        <v>1623</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C37">
-        <v>124</v>
-      </c>
-      <c r="D37" s="27">
-        <v>41</v>
-      </c>
-      <c r="E37" s="27">
-        <f>C37+(D37/60)</f>
-        <v>124.68333333333334</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C38">
-        <v>124</v>
-      </c>
-      <c r="D38" s="27">
-        <v>43.26</v>
-      </c>
-      <c r="E38" s="27">
-        <f t="shared" ref="E38:E42" si="1">C38+(D38/60)</f>
-        <v>124.721</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C39">
-        <v>124</v>
-      </c>
-      <c r="D39" s="27">
-        <v>43.28</v>
-      </c>
-      <c r="E39" s="27">
-        <f t="shared" si="1"/>
-        <v>124.72133333333333</v>
-      </c>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C40">
-        <v>125</v>
-      </c>
-      <c r="D40" s="27">
-        <v>21.2</v>
-      </c>
-      <c r="E40" s="27">
-        <f t="shared" si="1"/>
-        <v>125.35333333333334</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C41">
-        <v>125</v>
-      </c>
-      <c r="D41" s="27">
-        <v>21.21</v>
-      </c>
-      <c r="E41" s="27">
-        <f t="shared" si="1"/>
-        <v>125.3535</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C42">
-        <v>125</v>
-      </c>
-      <c r="D42" s="27">
-        <v>21.22</v>
-      </c>
-      <c r="E42" s="27">
-        <f t="shared" si="1"/>
         <v>125.35366666666667</v>
       </c>
     </row>
@@ -3091,7 +3268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114EE0BB-9430-4707-8294-22F3EA198BF4}">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:N52"/>
     </sheetView>
   </sheetViews>
@@ -3928,7 +4105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C891EA49-1228-4754-8524-0795D1247222}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L25" sqref="A1:L25"/>
     </sheetView>
   </sheetViews>
@@ -3949,18 +4126,18 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="53"/>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59" t="s">
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
     </row>
     <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">

</xml_diff>

<commit_message>
Malahat out sio in
</commit_message>
<xml_diff>
--- a/Documentation/Summary.xlsx
+++ b/Documentation/Summary.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaity\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaity\Documents\GitHub\DCLDE2026\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{555B7967-6C0A-44D1-968A-E13AEA6D8769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8133CAF8-F995-4535-B221-46280839E9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
+    <workbookView xWindow="1344" yWindow="144" windowWidth="17280" windowHeight="11076" activeTab="1" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="NoMalahat" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="121">
   <si>
     <t>Annotations</t>
   </si>
@@ -397,6 +398,9 @@
   </si>
   <si>
     <t>HaroStraitSouth</t>
+  </si>
+  <si>
+    <t>Cpe_Elz</t>
   </si>
 </sst>
 </file>
@@ -407,7 +411,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,6 +439,13 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -736,7 +747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -830,12 +841,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -851,12 +856,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1173,12 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4A8866-C81C-482A-B0A6-264BECA1C8D5}">
   <dimension ref="A1:BZ43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="13" topLeftCell="L39" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="C1" sqref="C1"/>
-      <selection pane="topRight" activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
-      <selection pane="bottomRight" activeCell="P41" sqref="P41:X42"/>
+    <sheetView topLeftCell="K30" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,11 +1203,11 @@
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" style="24" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="24" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="9" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" style="55" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" style="53" customWidth="1"/>
     <col min="9" max="9" width="12.21875" style="4" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11.77734375" style="4" customWidth="1"/>
     <col min="11" max="11" width="13.21875" style="4" customWidth="1"/>
@@ -1206,17 +1223,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="P1" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
+      <c r="P1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
     </row>
     <row r="2" spans="1:78" s="21" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -1240,7 +1257,7 @@
       <c r="G2" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="54" t="s">
         <v>74</v>
       </c>
       <c r="I2" s="22" t="s">
@@ -1314,7 +1331,7 @@
       <c r="G3">
         <v>32</v>
       </c>
-      <c r="H3" s="55" t="s">
+      <c r="H3" s="53" t="s">
         <v>114</v>
       </c>
       <c r="K3" s="5">
@@ -1376,7 +1393,7 @@
       <c r="G4">
         <v>32</v>
       </c>
-      <c r="H4" s="55" t="s">
+      <c r="H4" s="53" t="s">
         <v>114</v>
       </c>
       <c r="K4" s="5">
@@ -1484,7 +1501,7 @@
       <c r="G5">
         <v>32</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="53" t="s">
         <v>114</v>
       </c>
       <c r="K5" s="5">
@@ -1546,7 +1563,7 @@
       <c r="G6">
         <v>32</v>
       </c>
-      <c r="H6" s="55" t="s">
+      <c r="H6" s="53" t="s">
         <v>114</v>
       </c>
       <c r="K6" s="5">
@@ -1608,7 +1625,7 @@
       <c r="G7">
         <v>32</v>
       </c>
-      <c r="H7" s="55" t="s">
+      <c r="H7" s="53" t="s">
         <v>114</v>
       </c>
       <c r="K7" s="5">
@@ -1670,7 +1687,7 @@
       <c r="G8">
         <v>32</v>
       </c>
-      <c r="H8" s="55" t="s">
+      <c r="H8" s="53" t="s">
         <v>114</v>
       </c>
       <c r="K8" s="5">
@@ -1732,7 +1749,7 @@
       <c r="G9">
         <v>32</v>
       </c>
-      <c r="H9" s="55" t="s">
+      <c r="H9" s="53" t="s">
         <v>114</v>
       </c>
       <c r="K9" s="5">
@@ -1794,7 +1811,7 @@
       <c r="G10">
         <v>32</v>
       </c>
-      <c r="H10" s="55" t="s">
+      <c r="H10" s="53" t="s">
         <v>114</v>
       </c>
       <c r="K10" s="5">
@@ -1856,7 +1873,7 @@
       <c r="G11">
         <v>32</v>
       </c>
-      <c r="H11" s="55" t="s">
+      <c r="H11" s="53" t="s">
         <v>114</v>
       </c>
       <c r="K11" s="5">
@@ -1921,7 +1938,7 @@
       <c r="G12" s="6">
         <v>64</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="55" t="s">
         <v>59</v>
       </c>
       <c r="I12" s="7"/>
@@ -1989,7 +2006,7 @@
       <c r="G13" s="8">
         <v>16.384</v>
       </c>
-      <c r="H13" s="55" t="s">
+      <c r="H13" s="53" t="s">
         <v>75</v>
       </c>
       <c r="I13" s="9">
@@ -2058,7 +2075,7 @@
       <c r="G14" s="10">
         <v>16</v>
       </c>
-      <c r="H14" s="55" t="s">
+      <c r="H14" s="53" t="s">
         <v>73</v>
       </c>
       <c r="I14" s="11">
@@ -2130,7 +2147,7 @@
       <c r="G15" s="8">
         <v>192</v>
       </c>
-      <c r="H15" s="58" t="s">
+      <c r="H15" s="56" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="12">
@@ -2199,7 +2216,7 @@
       <c r="G16">
         <v>256</v>
       </c>
-      <c r="H16" s="55" t="s">
+      <c r="H16" s="53" t="s">
         <v>48</v>
       </c>
       <c r="I16" s="5">
@@ -2267,7 +2284,7 @@
       <c r="G17">
         <v>256</v>
       </c>
-      <c r="H17" s="55" t="s">
+      <c r="H17" s="53" t="s">
         <v>49</v>
       </c>
       <c r="I17" s="5">
@@ -2335,7 +2352,7 @@
       <c r="G18">
         <v>256</v>
       </c>
-      <c r="H18" s="55" t="s">
+      <c r="H18" s="53" t="s">
         <v>50</v>
       </c>
       <c r="I18" s="5">
@@ -2403,7 +2420,7 @@
       <c r="G19">
         <v>256</v>
       </c>
-      <c r="H19" s="55" t="s">
+      <c r="H19" s="53" t="s">
         <v>51</v>
       </c>
       <c r="I19" s="5">
@@ -2471,7 +2488,7 @@
       <c r="G20" s="10">
         <v>256</v>
       </c>
-      <c r="H20" s="55" t="s">
+      <c r="H20" s="53" t="s">
         <v>52</v>
       </c>
       <c r="I20" s="13">
@@ -2543,7 +2560,7 @@
       <c r="G21" s="8">
         <v>64</v>
       </c>
-      <c r="H21" s="58" t="s">
+      <c r="H21" s="56" t="s">
         <v>72</v>
       </c>
       <c r="I21" s="9"/>
@@ -2608,7 +2625,7 @@
       <c r="G22">
         <v>64</v>
       </c>
-      <c r="H22" s="55" t="s">
+      <c r="H22" s="53" t="s">
         <v>72</v>
       </c>
       <c r="K22" s="5">
@@ -2670,7 +2687,7 @@
       <c r="G23">
         <v>64</v>
       </c>
-      <c r="H23" s="55" t="s">
+      <c r="H23" s="53" t="s">
         <v>72</v>
       </c>
       <c r="K23" s="5">
@@ -2732,7 +2749,7 @@
       <c r="G24" s="10">
         <v>64</v>
       </c>
-      <c r="H24" s="59" t="s">
+      <c r="H24" s="57" t="s">
         <v>72</v>
       </c>
       <c r="I24" s="11"/>
@@ -2800,7 +2817,7 @@
       <c r="G25" s="6">
         <v>128</v>
       </c>
-      <c r="H25" s="59" t="s">
+      <c r="H25" s="57" t="s">
         <v>58</v>
       </c>
       <c r="I25" s="7"/>
@@ -2868,7 +2885,7 @@
       <c r="G26">
         <v>200</v>
       </c>
-      <c r="H26" s="55" t="s">
+      <c r="H26" s="53" t="s">
         <v>106</v>
       </c>
       <c r="K26" s="51">
@@ -2900,7 +2917,7 @@
       <c r="G27">
         <v>200</v>
       </c>
-      <c r="H27" s="55" t="s">
+      <c r="H27" s="53" t="s">
         <v>106</v>
       </c>
       <c r="K27" s="51">
@@ -2932,7 +2949,7 @@
       <c r="G28">
         <v>200</v>
       </c>
-      <c r="H28" s="55" t="s">
+      <c r="H28" s="53" t="s">
         <v>106</v>
       </c>
       <c r="K28" s="51">
@@ -2964,7 +2981,7 @@
       <c r="G29">
         <v>200</v>
       </c>
-      <c r="H29" s="55" t="s">
+      <c r="H29" s="53" t="s">
         <v>106</v>
       </c>
       <c r="K29" s="51">
@@ -2996,7 +3013,7 @@
       <c r="G30">
         <v>200</v>
       </c>
-      <c r="H30" s="55" t="s">
+      <c r="H30" s="53" t="s">
         <v>106</v>
       </c>
       <c r="K30" s="51">
@@ -3028,7 +3045,7 @@
       <c r="G31">
         <v>200</v>
       </c>
-      <c r="H31" s="55" t="s">
+      <c r="H31" s="53" t="s">
         <v>106</v>
       </c>
       <c r="K31" s="51">
@@ -3060,7 +3077,7 @@
       <c r="F32" s="8">
         <v>251</v>
       </c>
-      <c r="H32" s="58" t="s">
+      <c r="H32" s="56" t="s">
         <v>72</v>
       </c>
       <c r="I32" s="9"/>
@@ -3110,59 +3127,55 @@
       <c r="B33" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="60" t="s">
+      <c r="C33" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="60">
+      <c r="D33">
         <v>48.5167</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33">
         <v>-123.207616666666</v>
       </c>
-      <c r="F33" s="60">
+      <c r="F33">
         <v>210</v>
       </c>
-      <c r="G33" s="60"/>
-      <c r="H33" s="61" t="s">
+      <c r="H33" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="I33" s="62"/>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62">
+      <c r="K33" s="4">
         <v>42924</v>
       </c>
-      <c r="L33" s="62">
+      <c r="L33" s="4">
         <v>43032</v>
       </c>
-      <c r="M33" s="62"/>
-      <c r="N33" s="63">
+      <c r="N33" s="41">
         <v>5170</v>
       </c>
-      <c r="O33" s="60" t="s">
+      <c r="O33" t="s">
         <v>82</v>
       </c>
-      <c r="P33" s="60" t="s">
+      <c r="P33" t="s">
         <v>10</v>
       </c>
       <c r="Q33" s="14">
         <v>4786</v>
       </c>
-      <c r="R33" s="60">
-        <v>0</v>
-      </c>
-      <c r="S33" s="60">
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
         <v>384</v>
       </c>
-      <c r="T33" s="60">
+      <c r="T33">
         <v>0</v>
       </c>
       <c r="U33" s="14">
         <v>2658</v>
       </c>
-      <c r="V33" s="60">
+      <c r="V33">
         <v>57</v>
       </c>
-      <c r="W33" s="60">
+      <c r="W33">
         <v>0</v>
       </c>
       <c r="X33" s="31">
@@ -3173,61 +3186,58 @@
       <c r="B34" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="60" t="s">
+      <c r="C34" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="60">
+      <c r="D34">
         <v>48.760779999999997</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34">
         <v>-123.06793999999999</v>
       </c>
-      <c r="F34" s="60">
+      <c r="F34">
         <v>193</v>
       </c>
-      <c r="G34" s="60">
+      <c r="G34">
         <v>128</v>
       </c>
-      <c r="H34" s="61" t="s">
+      <c r="H34" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62">
+      <c r="K34" s="4">
         <v>43345</v>
       </c>
-      <c r="L34" s="62">
+      <c r="L34" s="4">
         <v>43557</v>
       </c>
-      <c r="M34" s="62"/>
-      <c r="N34" s="63">
+      <c r="N34" s="41">
         <v>2032</v>
       </c>
-      <c r="O34" s="60" t="s">
+      <c r="O34" t="s">
         <v>82</v>
       </c>
-      <c r="P34" s="60" t="s">
+      <c r="P34" t="s">
         <v>10</v>
       </c>
       <c r="Q34" s="14">
         <v>1936</v>
       </c>
-      <c r="R34" s="60">
+      <c r="R34">
         <v>6</v>
       </c>
-      <c r="S34" s="60">
+      <c r="S34">
         <v>52</v>
       </c>
-      <c r="T34" s="60">
+      <c r="T34">
         <v>27</v>
       </c>
       <c r="U34" s="14">
         <v>988</v>
       </c>
-      <c r="V34" s="60">
+      <c r="V34">
         <v>47</v>
       </c>
-      <c r="W34" s="60">
+      <c r="W34">
         <v>0</v>
       </c>
       <c r="X34" s="31">
@@ -3256,7 +3266,7 @@
       <c r="G35" s="10">
         <v>64</v>
       </c>
-      <c r="H35" s="59" t="s">
+      <c r="H35" s="57" t="s">
         <v>115</v>
       </c>
       <c r="I35" s="11"/>
@@ -3445,14 +3455,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCCC199-A41A-4F1A-82DB-36CD09435BF7}">
-  <dimension ref="A1:BW41"/>
+  <dimension ref="A1:BW37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G21" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40:U41"/>
+    <sheetView tabSelected="1" topLeftCell="M23" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
     <col min="9" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
@@ -3462,21 +3473,21 @@
     <row r="1" spans="1:75" x14ac:dyDescent="0.3">
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
-      <c r="H1" s="55"/>
+      <c r="H1" s="53"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="41"/>
-      <c r="M1" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
+      <c r="M1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
     </row>
     <row r="2" spans="1:75" s="21" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -3500,7 +3511,7 @@
       <c r="G2" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="54" t="s">
         <v>74</v>
       </c>
       <c r="I2" s="22" t="s">
@@ -3565,7 +3576,7 @@
       <c r="G3">
         <v>32</v>
       </c>
-      <c r="H3" s="55" t="s">
+      <c r="H3" s="53" t="s">
         <v>114</v>
       </c>
       <c r="I3" s="5">
@@ -3627,7 +3638,7 @@
       <c r="G4">
         <v>32</v>
       </c>
-      <c r="H4" s="55" t="s">
+      <c r="H4" s="53" t="s">
         <v>114</v>
       </c>
       <c r="I4" s="5">
@@ -3735,7 +3746,7 @@
       <c r="G5">
         <v>32</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="53" t="s">
         <v>114</v>
       </c>
       <c r="I5" s="5">
@@ -3797,7 +3808,7 @@
       <c r="G6">
         <v>32</v>
       </c>
-      <c r="H6" s="55" t="s">
+      <c r="H6" s="53" t="s">
         <v>114</v>
       </c>
       <c r="I6" s="5">
@@ -3859,7 +3870,7 @@
       <c r="G7">
         <v>32</v>
       </c>
-      <c r="H7" s="55" t="s">
+      <c r="H7" s="53" t="s">
         <v>114</v>
       </c>
       <c r="I7" s="5">
@@ -3921,7 +3932,7 @@
       <c r="G8">
         <v>32</v>
       </c>
-      <c r="H8" s="55" t="s">
+      <c r="H8" s="53" t="s">
         <v>114</v>
       </c>
       <c r="I8" s="5">
@@ -3983,7 +3994,7 @@
       <c r="G9">
         <v>32</v>
       </c>
-      <c r="H9" s="55" t="s">
+      <c r="H9" s="53" t="s">
         <v>114</v>
       </c>
       <c r="I9" s="5">
@@ -4045,7 +4056,7 @@
       <c r="G10">
         <v>32</v>
       </c>
-      <c r="H10" s="55" t="s">
+      <c r="H10" s="53" t="s">
         <v>114</v>
       </c>
       <c r="I10" s="5">
@@ -4107,7 +4118,7 @@
       <c r="G11">
         <v>32</v>
       </c>
-      <c r="H11" s="55" t="s">
+      <c r="H11" s="53" t="s">
         <v>114</v>
       </c>
       <c r="I11" s="5">
@@ -4143,10 +4154,10 @@
       <c r="S11">
         <v>0</v>
       </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11" s="31">
+      <c r="T11" s="63">
+        <v>0</v>
+      </c>
+      <c r="U11" s="20">
         <v>0</v>
       </c>
     </row>
@@ -4172,7 +4183,7 @@
       <c r="G12" s="6">
         <v>64</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="55" t="s">
         <v>59</v>
       </c>
       <c r="I12" s="32">
@@ -4190,28 +4201,28 @@
       <c r="M12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N12" s="47">
+      <c r="N12" s="64">
         <v>1626</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="65">
         <v>9392</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="65">
         <v>156</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="65">
         <v>2946</v>
       </c>
       <c r="R12" s="34">
         <v>130</v>
       </c>
-      <c r="S12" s="6">
+      <c r="S12" s="65">
         <v>834</v>
       </c>
-      <c r="T12" s="6">
-        <v>0</v>
-      </c>
-      <c r="U12" s="48">
+      <c r="T12" s="65">
+        <v>0</v>
+      </c>
+      <c r="U12" s="18">
         <v>418</v>
       </c>
     </row>
@@ -4237,7 +4248,7 @@
       <c r="G13" s="8">
         <v>16.384</v>
       </c>
-      <c r="H13" s="55" t="s">
+      <c r="H13" s="53" t="s">
         <v>75</v>
       </c>
       <c r="I13" s="12">
@@ -4255,28 +4266,28 @@
       <c r="M13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="66">
         <v>10384</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="67">
         <v>2757</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="67">
         <v>5054</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="67">
         <v>95861</v>
       </c>
-      <c r="R13" s="15">
+      <c r="R13" s="68">
         <v>48</v>
       </c>
-      <c r="S13" s="8">
+      <c r="S13" s="69">
         <v>5336</v>
       </c>
-      <c r="T13" s="8">
+      <c r="T13" s="70">
         <v>4558</v>
       </c>
-      <c r="U13" s="29">
+      <c r="U13" s="19">
         <v>258</v>
       </c>
     </row>
@@ -4299,7 +4310,7 @@
       <c r="G14" s="10">
         <v>16</v>
       </c>
-      <c r="H14" s="55" t="s">
+      <c r="H14" s="53" t="s">
         <v>73</v>
       </c>
       <c r="I14" s="13">
@@ -4317,28 +4328,28 @@
       <c r="M14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="66">
         <v>6886</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14" s="73">
         <v>10696</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="67">
         <v>1178</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="67">
         <v>26058</v>
       </c>
-      <c r="R14" s="16">
-        <v>0</v>
-      </c>
-      <c r="S14" s="10">
+      <c r="R14" s="71">
+        <v>0</v>
+      </c>
+      <c r="S14" s="72">
         <v>2309</v>
       </c>
-      <c r="T14" s="10">
+      <c r="T14" s="72">
         <v>3501</v>
       </c>
-      <c r="U14" s="30">
+      <c r="U14" s="20">
         <v>947</v>
       </c>
     </row>
@@ -4364,7 +4375,7 @@
       <c r="G15" s="8">
         <v>192</v>
       </c>
-      <c r="H15" s="58" t="s">
+      <c r="H15" s="56" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="12">
@@ -4382,28 +4393,28 @@
       <c r="M15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="68">
         <v>2668</v>
       </c>
-      <c r="O15" s="8">
+      <c r="O15" s="69">
         <v>33</v>
       </c>
-      <c r="P15" s="8">
+      <c r="P15" s="69">
         <v>297</v>
       </c>
-      <c r="Q15" s="8">
-        <v>0</v>
-      </c>
-      <c r="R15" s="14">
+      <c r="Q15" s="69">
+        <v>0</v>
+      </c>
+      <c r="R15" s="66">
         <v>1610</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="67">
         <v>694</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="70">
         <v>364</v>
       </c>
-      <c r="U15" s="29">
+      <c r="U15" s="19">
         <v>0</v>
       </c>
     </row>
@@ -4426,7 +4437,7 @@
       <c r="G16">
         <v>256</v>
       </c>
-      <c r="H16" s="55" t="s">
+      <c r="H16" s="53" t="s">
         <v>48</v>
       </c>
       <c r="I16" s="5">
@@ -4444,28 +4455,28 @@
       <c r="M16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="14">
+      <c r="N16" s="66">
         <v>4777</v>
       </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
+      <c r="O16" s="67">
+        <v>0</v>
+      </c>
+      <c r="P16" s="67">
         <v>190</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="67">
         <v>131</v>
       </c>
-      <c r="R16" s="14">
+      <c r="R16" s="66">
         <v>4184</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="67">
         <v>593</v>
       </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16" s="31">
+      <c r="T16" s="70">
+        <v>0</v>
+      </c>
+      <c r="U16" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4488,7 +4499,7 @@
       <c r="G17">
         <v>256</v>
       </c>
-      <c r="H17" s="55" t="s">
+      <c r="H17" s="53" t="s">
         <v>49</v>
       </c>
       <c r="I17" s="5">
@@ -4506,28 +4517,28 @@
       <c r="M17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N17" s="14">
+      <c r="N17" s="66">
         <v>324</v>
       </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
+      <c r="O17" s="67">
+        <v>0</v>
+      </c>
+      <c r="P17" s="67">
         <v>1</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="67">
         <v>42</v>
       </c>
-      <c r="R17" s="14">
-        <v>0</v>
-      </c>
-      <c r="S17">
+      <c r="R17" s="66">
+        <v>0</v>
+      </c>
+      <c r="S17" s="67">
         <v>324</v>
       </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17" s="31">
+      <c r="T17" s="70">
+        <v>0</v>
+      </c>
+      <c r="U17" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4550,7 +4561,7 @@
       <c r="G18">
         <v>256</v>
       </c>
-      <c r="H18" s="55" t="s">
+      <c r="H18" s="53" t="s">
         <v>50</v>
       </c>
       <c r="I18" s="5">
@@ -4568,28 +4579,28 @@
       <c r="M18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N18" s="14">
+      <c r="N18" s="66">
         <v>350</v>
       </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
+      <c r="O18" s="67">
+        <v>0</v>
+      </c>
+      <c r="P18" s="67">
         <v>3</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="67">
         <v>221</v>
       </c>
-      <c r="R18" s="14">
+      <c r="R18" s="66">
         <v>159</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="67">
         <v>191</v>
       </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18" s="31">
+      <c r="T18" s="70">
+        <v>0</v>
+      </c>
+      <c r="U18" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4612,7 +4623,7 @@
       <c r="G19">
         <v>256</v>
       </c>
-      <c r="H19" s="55" t="s">
+      <c r="H19" s="53" t="s">
         <v>51</v>
       </c>
       <c r="I19" s="5">
@@ -4648,10 +4659,10 @@
       <c r="S19">
         <v>71</v>
       </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19" s="31">
+      <c r="T19" s="63">
+        <v>0</v>
+      </c>
+      <c r="U19" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4674,7 +4685,7 @@
       <c r="G20" s="10">
         <v>256</v>
       </c>
-      <c r="H20" s="55" t="s">
+      <c r="H20" s="53" t="s">
         <v>52</v>
       </c>
       <c r="I20" s="13">
@@ -4713,7 +4724,7 @@
       <c r="T20" s="10">
         <v>0</v>
       </c>
-      <c r="U20" s="30">
+      <c r="U20" s="20">
         <v>0</v>
       </c>
     </row>
@@ -4739,7 +4750,7 @@
       <c r="G21" s="6">
         <v>128</v>
       </c>
-      <c r="H21" s="59" t="s">
+      <c r="H21" s="57" t="s">
         <v>58</v>
       </c>
       <c r="I21" s="32">
@@ -4778,7 +4789,7 @@
       <c r="T21" s="6">
         <v>0</v>
       </c>
-      <c r="U21" s="48">
+      <c r="U21" s="18">
         <v>0</v>
       </c>
     </row>
@@ -4804,497 +4815,422 @@
       <c r="G22">
         <v>200</v>
       </c>
-      <c r="H22" s="55" t="s">
+      <c r="H22" s="53" t="s">
         <v>106</v>
       </c>
       <c r="I22" s="51">
         <v>39616</v>
       </c>
       <c r="J22" s="51">
-        <v>39973</v>
-      </c>
-      <c r="K22" s="41"/>
-      <c r="N22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="U22" s="31"/>
+        <v>40925</v>
+      </c>
+      <c r="K22" s="41">
+        <v>2159</v>
+      </c>
+      <c r="L22" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="M22" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="14">
+        <v>626</v>
+      </c>
+      <c r="O22" s="62">
+        <v>0</v>
+      </c>
+      <c r="P22" s="62">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="62">
+        <v>0</v>
+      </c>
+      <c r="R22" s="14">
+        <v>0</v>
+      </c>
+      <c r="S22" s="62">
+        <v>279</v>
+      </c>
+      <c r="T22" s="62">
+        <v>0</v>
+      </c>
+      <c r="U22" s="17">
+        <v>347</v>
+      </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="D23" s="24">
-        <v>47.351999999999997</v>
+        <v>47.5</v>
       </c>
       <c r="E23" s="24">
-        <v>124.721</v>
+        <v>125.35333333333334</v>
       </c>
       <c r="F23">
-        <v>118</v>
+        <v>1400</v>
       </c>
       <c r="G23">
         <v>200</v>
       </c>
-      <c r="H23" s="55" t="s">
+      <c r="H23" s="53" t="s">
         <v>106</v>
       </c>
       <c r="I23" s="51">
-        <v>40684</v>
+        <v>40570</v>
       </c>
       <c r="J23" s="51">
-        <v>40853</v>
-      </c>
-      <c r="K23" s="41"/>
-      <c r="N23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="U23" s="31"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="24">
-        <v>47.352333333333334</v>
-      </c>
-      <c r="E24" s="24">
-        <v>124.72133333333333</v>
-      </c>
-      <c r="F24">
-        <v>150</v>
-      </c>
-      <c r="G24">
-        <v>200</v>
-      </c>
-      <c r="H24" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="I24" s="51">
-        <v>40884</v>
-      </c>
-      <c r="J24" s="51">
-        <v>40925</v>
-      </c>
-      <c r="K24" s="41"/>
-      <c r="N24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="U24" s="31"/>
+        <v>41455</v>
+      </c>
+      <c r="K23" s="41">
+        <v>636</v>
+      </c>
+      <c r="L23" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="M23" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="N23" s="14">
+        <v>2012</v>
+      </c>
+      <c r="O23" s="62">
+        <v>0</v>
+      </c>
+      <c r="P23" s="62">
+        <v>47</v>
+      </c>
+      <c r="Q23" s="62">
+        <v>100</v>
+      </c>
+      <c r="R23" s="14">
+        <v>83</v>
+      </c>
+      <c r="S23" s="62">
+        <v>1928</v>
+      </c>
+      <c r="T23" s="62">
+        <v>0</v>
+      </c>
+      <c r="U23" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="8">
+        <v>48.518050000000002</v>
+      </c>
+      <c r="E24" s="8">
+        <v>-123.19166666666599</v>
+      </c>
+      <c r="F24" s="8">
+        <v>251</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="9">
+        <v>42924</v>
+      </c>
+      <c r="J24" s="9">
+        <v>43032</v>
+      </c>
+      <c r="K24" s="44">
+        <v>5326</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N24" s="15">
+        <v>4853</v>
+      </c>
+      <c r="O24" s="8">
+        <v>0</v>
+      </c>
+      <c r="P24" s="8">
+        <v>473</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>0</v>
+      </c>
+      <c r="R24" s="15">
+        <v>3212</v>
+      </c>
+      <c r="S24" s="8">
+        <v>0</v>
+      </c>
+      <c r="T24" s="8">
+        <v>0</v>
+      </c>
+      <c r="U24" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="24">
-        <v>47.5</v>
-      </c>
-      <c r="E25" s="24">
-        <v>125.35333333333334</v>
+        <v>119</v>
+      </c>
+      <c r="D25">
+        <v>48.5167</v>
+      </c>
+      <c r="E25">
+        <v>-123.207616666666</v>
       </c>
       <c r="F25">
-        <v>1400</v>
-      </c>
-      <c r="G25">
-        <v>200</v>
-      </c>
-      <c r="H25" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="I25" s="51">
-        <v>40570</v>
-      </c>
-      <c r="J25" s="51">
-        <v>40823</v>
-      </c>
-      <c r="K25" s="41"/>
-      <c r="N25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="U25" s="31"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="H25" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" s="4">
+        <v>42924</v>
+      </c>
+      <c r="J25" s="4">
+        <v>43032</v>
+      </c>
+      <c r="K25" s="41">
+        <v>5170</v>
+      </c>
+      <c r="L25" t="s">
+        <v>82</v>
+      </c>
+      <c r="M25" t="s">
+        <v>10</v>
+      </c>
+      <c r="N25" s="14">
+        <v>4786</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>384</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25" s="14">
+        <v>2658</v>
+      </c>
+      <c r="S25">
+        <v>57</v>
+      </c>
+      <c r="T25" s="63">
+        <v>0</v>
+      </c>
+      <c r="U25" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" s="24">
-        <v>47.500500000000002</v>
-      </c>
-      <c r="E26" s="24">
-        <v>125.3535</v>
+        <v>117</v>
+      </c>
+      <c r="D26">
+        <v>48.760779999999997</v>
+      </c>
+      <c r="E26">
+        <v>-123.06793999999999</v>
       </c>
       <c r="F26">
-        <v>1394</v>
+        <v>193</v>
       </c>
       <c r="G26">
-        <v>200</v>
-      </c>
-      <c r="H26" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="I26" s="51">
-        <v>40736</v>
-      </c>
-      <c r="J26" s="51">
-        <v>41101</v>
-      </c>
-      <c r="K26" s="41"/>
-      <c r="N26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="U26" s="31"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="H26" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="I26" s="4">
+        <v>43345</v>
+      </c>
+      <c r="J26" s="4">
+        <v>43557</v>
+      </c>
+      <c r="K26" s="41">
+        <v>2032</v>
+      </c>
+      <c r="L26" t="s">
+        <v>82</v>
+      </c>
+      <c r="M26" t="s">
+        <v>10</v>
+      </c>
+      <c r="N26" s="14">
+        <v>1936</v>
+      </c>
+      <c r="O26">
+        <v>6</v>
+      </c>
+      <c r="P26">
+        <v>52</v>
+      </c>
+      <c r="Q26">
+        <v>27</v>
+      </c>
+      <c r="R26" s="14">
+        <v>988</v>
+      </c>
+      <c r="S26">
+        <v>47</v>
+      </c>
+      <c r="T26" s="63">
+        <v>0</v>
+      </c>
+      <c r="U26" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>110</v>
+      </c>
       <c r="B27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" t="s">
-        <v>105</v>
-      </c>
-      <c r="D27" s="24">
-        <v>47.500500000000002</v>
-      </c>
-      <c r="E27" s="24">
-        <v>125.35366666666667</v>
-      </c>
-      <c r="F27">
-        <v>1394</v>
-      </c>
-      <c r="G27">
-        <v>200</v>
-      </c>
-      <c r="H27" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="I27" s="51">
-        <v>41166</v>
-      </c>
-      <c r="J27" s="51">
-        <v>41455</v>
-      </c>
-      <c r="K27" s="41"/>
-      <c r="N27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="U27" s="31"/>
-    </row>
-    <row r="28" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="8">
-        <v>48.518050000000002</v>
-      </c>
-      <c r="E28" s="8">
-        <v>-123.19166666666599</v>
-      </c>
-      <c r="F28" s="8">
-        <v>251</v>
-      </c>
-      <c r="H28" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="I28" s="9">
-        <v>42924</v>
-      </c>
-      <c r="J28" s="9">
-        <v>43032</v>
-      </c>
-      <c r="K28" s="44">
-        <v>5326</v>
-      </c>
-      <c r="L28" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="28">
+        <v>49.042645</v>
+      </c>
+      <c r="E27" s="28">
+        <v>-123.31744</v>
+      </c>
+      <c r="F27" s="10">
+        <v>168</v>
+      </c>
+      <c r="G27" s="10">
+        <v>64</v>
+      </c>
+      <c r="H27" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="I27" s="11">
+        <v>42270</v>
+      </c>
+      <c r="J27" s="11">
+        <v>43189</v>
+      </c>
+      <c r="K27" s="45">
+        <v>2138</v>
+      </c>
+      <c r="L27" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="M28" s="8" t="s">
+      <c r="M27" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N28" s="15">
-        <v>4853</v>
-      </c>
-      <c r="O28" s="8">
-        <v>0</v>
-      </c>
-      <c r="P28" s="8">
-        <v>473</v>
-      </c>
-      <c r="Q28" s="8">
-        <v>0</v>
-      </c>
-      <c r="R28" s="15">
-        <v>3212</v>
-      </c>
-      <c r="S28" s="8">
-        <v>0</v>
-      </c>
-      <c r="T28" s="8">
-        <v>0</v>
-      </c>
-      <c r="U28" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" s="60">
-        <v>48.5167</v>
-      </c>
-      <c r="E29" s="60">
-        <v>-123.207616666666</v>
-      </c>
-      <c r="F29" s="60">
-        <v>210</v>
-      </c>
-      <c r="G29" s="60"/>
-      <c r="H29" s="61" t="s">
-        <v>72</v>
-      </c>
-      <c r="I29" s="62">
-        <v>42924</v>
-      </c>
-      <c r="J29" s="62">
-        <v>43032</v>
-      </c>
-      <c r="K29" s="63">
-        <v>5170</v>
-      </c>
-      <c r="L29" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="M29" s="60" t="s">
-        <v>10</v>
-      </c>
-      <c r="N29" s="14">
-        <v>4786</v>
-      </c>
-      <c r="O29" s="60">
-        <v>0</v>
-      </c>
-      <c r="P29" s="60">
-        <v>384</v>
-      </c>
-      <c r="Q29" s="60">
-        <v>0</v>
-      </c>
-      <c r="R29" s="14">
-        <v>2658</v>
-      </c>
-      <c r="S29" s="60">
-        <v>57</v>
-      </c>
-      <c r="T29" s="60">
-        <v>0</v>
-      </c>
-      <c r="U29" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="60" t="s">
+      <c r="N27" s="16">
+        <v>1932</v>
+      </c>
+      <c r="O27" s="10">
+        <v>36</v>
+      </c>
+      <c r="P27" s="10">
         <v>117</v>
       </c>
-      <c r="D30" s="60">
-        <v>48.760779999999997</v>
-      </c>
-      <c r="E30" s="60">
-        <v>-123.06793999999999</v>
-      </c>
-      <c r="F30" s="60">
-        <v>193</v>
-      </c>
-      <c r="G30" s="60">
-        <v>128</v>
-      </c>
-      <c r="H30" s="61" t="s">
-        <v>113</v>
-      </c>
-      <c r="I30" s="62">
-        <v>43345</v>
-      </c>
-      <c r="J30" s="62">
-        <v>43557</v>
-      </c>
-      <c r="K30" s="63">
-        <v>2032</v>
-      </c>
-      <c r="L30" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="M30" s="60" t="s">
-        <v>10</v>
-      </c>
-      <c r="N30" s="14">
-        <v>1936</v>
-      </c>
-      <c r="O30" s="60">
+      <c r="Q27" s="10">
+        <v>53</v>
+      </c>
+      <c r="R27" s="16">
+        <v>1297</v>
+      </c>
+      <c r="S27" s="10">
+        <v>248</v>
+      </c>
+      <c r="T27" s="10">
+        <v>0</v>
+      </c>
+      <c r="U27" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="13:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="13:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M36" s="35"/>
+      <c r="N36" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="O36" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P36" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="P30" s="60">
-        <v>52</v>
-      </c>
-      <c r="Q30" s="60">
-        <v>27</v>
-      </c>
-      <c r="R30" s="14">
-        <v>988</v>
-      </c>
-      <c r="S30" s="60">
-        <v>47</v>
-      </c>
-      <c r="T30" s="60">
-        <v>0</v>
-      </c>
-      <c r="U30" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" s="28">
-        <v>49.042645</v>
-      </c>
-      <c r="E31" s="28">
-        <v>-123.31744</v>
-      </c>
-      <c r="F31" s="10">
-        <v>168</v>
-      </c>
-      <c r="G31" s="10">
-        <v>64</v>
-      </c>
-      <c r="H31" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="I31" s="11">
-        <v>42270</v>
-      </c>
-      <c r="J31" s="11">
-        <v>43189</v>
-      </c>
-      <c r="K31" s="45">
-        <v>2138</v>
-      </c>
-      <c r="L31" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="M31" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="N31" s="16">
-        <v>1932</v>
-      </c>
-      <c r="O31" s="10">
-        <v>36</v>
-      </c>
-      <c r="P31" s="10">
-        <v>117</v>
-      </c>
-      <c r="Q31" s="10">
+      <c r="Q36" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="R36" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="R31" s="16">
-        <v>1297</v>
-      </c>
-      <c r="S31" s="10">
-        <v>248</v>
-      </c>
-      <c r="T31" s="10">
-        <v>0</v>
-      </c>
-      <c r="U31" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="13:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="13:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M40" s="35"/>
-      <c r="N40" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="O40" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="P40" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q40" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="R40" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="S40" s="37" t="s">
+      <c r="S36" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="T40" s="37" t="s">
+      <c r="T36" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="U40" s="1" t="s">
+      <c r="U36" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="13:21" x14ac:dyDescent="0.3">
-      <c r="M41" s="52" t="s">
+    <row r="37" spans="13:21" x14ac:dyDescent="0.3">
+      <c r="M37" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="N41" s="14">
-        <f>SUM(N2:N34)</f>
-        <v>53680</v>
-      </c>
-      <c r="O41" s="14">
-        <f t="shared" ref="O41:U41" si="0">SUM(O2:O34)</f>
+      <c r="N37" s="14">
+        <f>SUM(N2:N30)</f>
+        <v>56318</v>
+      </c>
+      <c r="O37" s="14">
+        <f t="shared" ref="O37:U37" si="0">SUM(O2:O30)</f>
         <v>22941</v>
       </c>
-      <c r="P41" s="14">
+      <c r="P37" s="14">
         <f t="shared" si="0"/>
-        <v>9054</v>
-      </c>
-      <c r="Q41" s="14">
+        <v>9111</v>
+      </c>
+      <c r="Q37" s="14">
         <f t="shared" si="0"/>
-        <v>127113</v>
-      </c>
-      <c r="R41" s="14">
+        <v>127213</v>
+      </c>
+      <c r="R37" s="14">
         <f t="shared" si="0"/>
-        <v>27188</v>
-      </c>
-      <c r="S41" s="14">
+        <v>27271</v>
+      </c>
+      <c r="S37" s="14">
         <f t="shared" si="0"/>
-        <v>10729</v>
-      </c>
-      <c r="T41" s="14">
+        <v>12936</v>
+      </c>
+      <c r="T37" s="14">
         <f t="shared" si="0"/>
         <v>8423</v>
       </c>
-      <c r="U41" s="14">
+      <c r="U37" s="14">
         <f t="shared" si="0"/>
-        <v>1623</v>
+        <v>1970</v>
       </c>
     </row>
   </sheetData>
@@ -6161,18 +6097,18 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="46"/>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54" t="s">
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
     </row>
     <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -7046,4 +6982,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B3E686-61FC-4D96-843D-9FBF976B2DF6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates text function fix bugs
</commit_message>
<xml_diff>
--- a/Documentation/Summary.xlsx
+++ b/Documentation/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaity\Documents\GitHub\DCLDE2026\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8133CAF8-F995-4535-B221-46280839E9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC017079-A9F1-4937-8418-31F14270283B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1344" yWindow="144" windowWidth="17280" windowHeight="11076" activeTab="1" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
+    <workbookView xWindow="1392" yWindow="132" windowWidth="19716" windowHeight="11136" activeTab="1" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="126">
   <si>
     <t>Annotations</t>
   </si>
@@ -401,6 +401,21 @@
   </si>
   <si>
     <t>Cpe_Elz</t>
+  </si>
+  <si>
+    <t>SMRU</t>
+  </si>
+  <si>
+    <t>Lime Kiln</t>
+  </si>
+  <si>
+    <t>LmKln</t>
+  </si>
+  <si>
+    <t>HTI</t>
+  </si>
+  <si>
+    <t>Calls</t>
   </si>
 </sst>
 </file>
@@ -747,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -856,28 +871,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1223,17 +1231,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="P1" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
+      <c r="P1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
     </row>
     <row r="2" spans="1:78" s="21" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -3457,12 +3465,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCCC199-A41A-4F1A-82DB-36CD09435BF7}">
   <dimension ref="A1:BW37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M23" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
     <col min="2" max="2" width="26.88671875" customWidth="1"/>
     <col min="9" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
@@ -3477,17 +3486,17 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="41"/>
-      <c r="M1" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
+      <c r="M1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
     </row>
     <row r="2" spans="1:75" s="21" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -4154,7 +4163,7 @@
       <c r="S11">
         <v>0</v>
       </c>
-      <c r="T11" s="63">
+      <c r="T11">
         <v>0</v>
       </c>
       <c r="U11" s="20">
@@ -4198,28 +4207,28 @@
       <c r="L12" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="N12" s="64">
+      <c r="N12" s="47">
         <v>1626</v>
       </c>
-      <c r="O12" s="65">
+      <c r="O12" s="6">
         <v>9392</v>
       </c>
-      <c r="P12" s="65">
+      <c r="P12" s="6">
         <v>156</v>
       </c>
-      <c r="Q12" s="65">
+      <c r="Q12" s="6">
         <v>2946</v>
       </c>
       <c r="R12" s="34">
         <v>130</v>
       </c>
-      <c r="S12" s="65">
+      <c r="S12" s="6">
         <v>834</v>
       </c>
-      <c r="T12" s="65">
+      <c r="T12" s="6">
         <v>0</v>
       </c>
       <c r="U12" s="18">
@@ -4263,28 +4272,28 @@
       <c r="L13" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="M13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="N13" s="66">
+      <c r="M13" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="14">
         <v>10384</v>
       </c>
-      <c r="O13" s="67">
+      <c r="O13">
         <v>2757</v>
       </c>
-      <c r="P13" s="67">
+      <c r="P13">
         <v>5054</v>
       </c>
-      <c r="Q13" s="67">
+      <c r="Q13">
         <v>95861</v>
       </c>
-      <c r="R13" s="68">
+      <c r="R13" s="15">
         <v>48</v>
       </c>
-      <c r="S13" s="69">
+      <c r="S13" s="8">
         <v>5336</v>
       </c>
-      <c r="T13" s="70">
+      <c r="T13">
         <v>4558</v>
       </c>
       <c r="U13" s="19">
@@ -4325,28 +4334,28 @@
       <c r="L14" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="M14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="N14" s="66">
+      <c r="M14" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" s="14">
         <v>6886</v>
       </c>
-      <c r="O14" s="73">
+      <c r="O14" s="58">
         <v>10696</v>
       </c>
-      <c r="P14" s="67">
+      <c r="P14">
         <v>1178</v>
       </c>
-      <c r="Q14" s="67">
+      <c r="Q14">
         <v>26058</v>
       </c>
-      <c r="R14" s="71">
-        <v>0</v>
-      </c>
-      <c r="S14" s="72">
+      <c r="R14" s="16">
+        <v>0</v>
+      </c>
+      <c r="S14" s="10">
         <v>2309</v>
       </c>
-      <c r="T14" s="72">
+      <c r="T14" s="10">
         <v>3501</v>
       </c>
       <c r="U14" s="20">
@@ -4393,25 +4402,25 @@
       <c r="M15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="68">
+      <c r="N15" s="15">
         <v>2668</v>
       </c>
-      <c r="O15" s="69">
+      <c r="O15" s="8">
         <v>33</v>
       </c>
-      <c r="P15" s="69">
+      <c r="P15" s="8">
         <v>297</v>
       </c>
-      <c r="Q15" s="69">
-        <v>0</v>
-      </c>
-      <c r="R15" s="66">
+      <c r="Q15" s="8">
+        <v>0</v>
+      </c>
+      <c r="R15" s="14">
         <v>1610</v>
       </c>
-      <c r="S15" s="67">
+      <c r="S15">
         <v>694</v>
       </c>
-      <c r="T15" s="70">
+      <c r="T15">
         <v>364</v>
       </c>
       <c r="U15" s="19">
@@ -4455,25 +4464,25 @@
       <c r="M16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="66">
+      <c r="N16" s="14">
         <v>4777</v>
       </c>
-      <c r="O16" s="67">
-        <v>0</v>
-      </c>
-      <c r="P16" s="67">
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
         <v>190</v>
       </c>
-      <c r="Q16" s="67">
+      <c r="Q16">
         <v>131</v>
       </c>
-      <c r="R16" s="66">
+      <c r="R16" s="14">
         <v>4184</v>
       </c>
-      <c r="S16" s="67">
+      <c r="S16">
         <v>593</v>
       </c>
-      <c r="T16" s="70">
+      <c r="T16">
         <v>0</v>
       </c>
       <c r="U16" s="17">
@@ -4517,25 +4526,25 @@
       <c r="M17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N17" s="66">
+      <c r="N17" s="14">
         <v>324</v>
       </c>
-      <c r="O17" s="67">
-        <v>0</v>
-      </c>
-      <c r="P17" s="67">
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
         <v>1</v>
       </c>
-      <c r="Q17" s="67">
+      <c r="Q17">
         <v>42</v>
       </c>
-      <c r="R17" s="66">
-        <v>0</v>
-      </c>
-      <c r="S17" s="67">
+      <c r="R17" s="14">
+        <v>0</v>
+      </c>
+      <c r="S17">
         <v>324</v>
       </c>
-      <c r="T17" s="70">
+      <c r="T17">
         <v>0</v>
       </c>
       <c r="U17" s="17">
@@ -4579,25 +4588,25 @@
       <c r="M18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N18" s="66">
+      <c r="N18" s="14">
         <v>350</v>
       </c>
-      <c r="O18" s="67">
-        <v>0</v>
-      </c>
-      <c r="P18" s="67">
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
         <v>3</v>
       </c>
-      <c r="Q18" s="67">
+      <c r="Q18">
         <v>221</v>
       </c>
-      <c r="R18" s="66">
+      <c r="R18" s="14">
         <v>159</v>
       </c>
-      <c r="S18" s="67">
+      <c r="S18">
         <v>191</v>
       </c>
-      <c r="T18" s="70">
+      <c r="T18">
         <v>0</v>
       </c>
       <c r="U18" s="17">
@@ -4659,7 +4668,7 @@
       <c r="S19">
         <v>71</v>
       </c>
-      <c r="T19" s="63">
+      <c r="T19">
         <v>0</v>
       </c>
       <c r="U19" s="17">
@@ -4685,7 +4694,7 @@
       <c r="G20" s="10">
         <v>256</v>
       </c>
-      <c r="H20" s="53" t="s">
+      <c r="H20" s="57" t="s">
         <v>52</v>
       </c>
       <c r="I20" s="13">
@@ -4827,31 +4836,31 @@
       <c r="K22" s="41">
         <v>2159</v>
       </c>
-      <c r="L22" s="61" t="s">
+      <c r="L22" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="M22" s="60" t="s">
+      <c r="M22" s="14" t="s">
         <v>16</v>
       </c>
       <c r="N22" s="14">
         <v>626</v>
       </c>
-      <c r="O22" s="62">
-        <v>0</v>
-      </c>
-      <c r="P22" s="62">
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
         <v>10</v>
       </c>
-      <c r="Q22" s="62">
+      <c r="Q22">
         <v>0</v>
       </c>
       <c r="R22" s="14">
         <v>0</v>
       </c>
-      <c r="S22" s="62">
+      <c r="S22">
         <v>279</v>
       </c>
-      <c r="T22" s="62">
+      <c r="T22">
         <v>0</v>
       </c>
       <c r="U22" s="17">
@@ -4889,31 +4898,31 @@
       <c r="K23" s="41">
         <v>636</v>
       </c>
-      <c r="L23" s="61" t="s">
+      <c r="L23" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="M23" s="60" t="s">
+      <c r="M23" s="14" t="s">
         <v>16</v>
       </c>
       <c r="N23" s="14">
         <v>2012</v>
       </c>
-      <c r="O23" s="62">
-        <v>0</v>
-      </c>
-      <c r="P23" s="62">
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
         <v>47</v>
       </c>
-      <c r="Q23" s="62">
+      <c r="Q23">
         <v>100</v>
       </c>
       <c r="R23" s="14">
         <v>83</v>
       </c>
-      <c r="S23" s="62">
+      <c r="S23">
         <v>1928</v>
       </c>
-      <c r="T23" s="62">
+      <c r="T23">
         <v>0</v>
       </c>
       <c r="U23" s="17">
@@ -4954,7 +4963,7 @@
       <c r="L24" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="M24" s="8" t="s">
+      <c r="M24" s="29" t="s">
         <v>10</v>
       </c>
       <c r="N24" s="15">
@@ -5013,7 +5022,7 @@
       <c r="L25" t="s">
         <v>82</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="31" t="s">
         <v>10</v>
       </c>
       <c r="N25" s="14">
@@ -5034,7 +5043,7 @@
       <c r="S25">
         <v>57</v>
       </c>
-      <c r="T25" s="63">
+      <c r="T25">
         <v>0</v>
       </c>
       <c r="U25" s="17">
@@ -5075,7 +5084,7 @@
       <c r="L26" t="s">
         <v>82</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="31" t="s">
         <v>10</v>
       </c>
       <c r="N26" s="14">
@@ -5096,7 +5105,7 @@
       <c r="S26">
         <v>47</v>
       </c>
-      <c r="T26" s="63">
+      <c r="T26">
         <v>0</v>
       </c>
       <c r="U26" s="17">
@@ -5104,10 +5113,10 @@
       </c>
     </row>
     <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="10" t="s">
         <v>112</v>
       </c>
       <c r="C27" s="10" t="s">
@@ -5140,7 +5149,7 @@
       <c r="L27" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="M27" s="10" t="s">
+      <c r="M27" s="30" t="s">
         <v>10</v>
       </c>
       <c r="N27" s="16">
@@ -5165,6 +5174,71 @@
         <v>0</v>
       </c>
       <c r="U27" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28">
+        <v>48.51</v>
+      </c>
+      <c r="E28">
+        <v>-123.15</v>
+      </c>
+      <c r="F28">
+        <v>23</v>
+      </c>
+      <c r="G28" s="61">
+        <v>150</v>
+      </c>
+      <c r="H28" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="I28" s="63">
+        <v>42680</v>
+      </c>
+      <c r="J28" s="63">
+        <v>44087</v>
+      </c>
+      <c r="K28">
+        <v>1667</v>
+      </c>
+      <c r="L28" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="M28" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="N28" s="14">
+        <v>1336</v>
+      </c>
+      <c r="O28">
+        <v>94</v>
+      </c>
+      <c r="P28">
+        <v>97</v>
+      </c>
+      <c r="Q28">
+        <v>140</v>
+      </c>
+      <c r="R28" s="15">
+        <v>760</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5202,23 +5276,23 @@
       </c>
       <c r="N37" s="14">
         <f>SUM(N2:N30)</f>
-        <v>56318</v>
+        <v>57654</v>
       </c>
       <c r="O37" s="14">
         <f t="shared" ref="O37:U37" si="0">SUM(O2:O30)</f>
-        <v>22941</v>
+        <v>23035</v>
       </c>
       <c r="P37" s="14">
         <f t="shared" si="0"/>
-        <v>9111</v>
+        <v>9208</v>
       </c>
       <c r="Q37" s="14">
         <f t="shared" si="0"/>
-        <v>127213</v>
+        <v>127353</v>
       </c>
       <c r="R37" s="14">
         <f t="shared" si="0"/>
-        <v>27271</v>
+        <v>28031</v>
       </c>
       <c r="S37" s="14">
         <f t="shared" si="0"/>
@@ -5245,8 +5319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114EE0BB-9430-4707-8294-22F3EA198BF4}">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:N52"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5987,18 +6061,155 @@
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="A26" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="8">
+        <v>48.518050000000002</v>
+      </c>
+      <c r="E26" s="8">
+        <v>-123.19166666666599</v>
+      </c>
+      <c r="F26" s="8">
+        <v>251</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" s="9">
+        <v>42924</v>
+      </c>
+      <c r="J26" s="9">
+        <v>43032</v>
+      </c>
       <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27">
+        <v>48.5167</v>
+      </c>
+      <c r="E27">
+        <v>-123.207616666666</v>
+      </c>
+      <c r="F27">
+        <v>210</v>
+      </c>
+      <c r="H27" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="4">
+        <v>42924</v>
+      </c>
+      <c r="J27" s="4">
+        <v>43032</v>
+      </c>
       <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28">
+        <v>48.760779999999997</v>
+      </c>
+      <c r="E28">
+        <v>-123.06793999999999</v>
+      </c>
+      <c r="F28">
+        <v>193</v>
+      </c>
+      <c r="G28">
+        <v>128</v>
+      </c>
+      <c r="H28" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="I28" s="4">
+        <v>43345</v>
+      </c>
+      <c r="J28" s="4">
+        <v>43557</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="28">
+        <v>49.042645</v>
+      </c>
+      <c r="E29" s="28">
+        <v>-123.31744</v>
+      </c>
+      <c r="F29" s="10">
+        <v>168</v>
+      </c>
+      <c r="G29" s="10">
+        <v>64</v>
+      </c>
+      <c r="H29" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="I29" s="11">
+        <v>42270</v>
+      </c>
+      <c r="J29" s="11">
+        <v>43189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30">
+        <v>48.51</v>
+      </c>
+      <c r="E30">
+        <v>-123.15</v>
+      </c>
+      <c r="F30">
+        <v>23</v>
+      </c>
+      <c r="G30" s="61">
+        <v>150</v>
+      </c>
+      <c r="H30" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="I30" s="63">
+        <v>42680</v>
+      </c>
+      <c r="J30" s="63">
+        <v>44087</v>
+      </c>
     </row>
     <row r="52" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="53" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6076,7 +6287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C891EA49-1228-4754-8524-0795D1247222}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="L25" sqref="A1:L25"/>
     </sheetView>
   </sheetViews>
@@ -6097,18 +6308,18 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="46"/>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59" t="s">
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
     </row>
     <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">

</xml_diff>

<commit_message>
update dep locs and manuscript
</commit_message>
<xml_diff>
--- a/Documentation/Summary.xlsx
+++ b/Documentation/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaity\Documents\GitHub\DCLDE2026\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC017079-A9F1-4937-8418-31F14270283B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD80C26-1BEA-4EDB-B0BE-EE5FCB276D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1392" yWindow="132" windowWidth="19716" windowHeight="11136" activeTab="1" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
+    <workbookView xWindow="1392" yWindow="132" windowWidth="19716" windowHeight="11136" activeTab="3" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="126">
   <si>
     <t>Annotations</t>
   </si>
@@ -762,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -874,18 +874,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1231,17 +1226,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="P1" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
+      <c r="P1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
     </row>
     <row r="2" spans="1:78" s="21" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -3465,8 +3460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCCC199-A41A-4F1A-82DB-36CD09435BF7}">
   <dimension ref="A1:BW37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3486,17 +3481,17 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="41"/>
-      <c r="M1" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
+      <c r="M1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
     </row>
     <row r="2" spans="1:75" s="21" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -5196,25 +5191,25 @@
       <c r="F28">
         <v>23</v>
       </c>
-      <c r="G28" s="61">
+      <c r="G28">
         <v>150</v>
       </c>
-      <c r="H28" s="62" t="s">
+      <c r="H28" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="I28" s="63">
+      <c r="I28" s="59">
         <v>42680</v>
       </c>
-      <c r="J28" s="63">
+      <c r="J28" s="59">
         <v>44087</v>
       </c>
       <c r="K28">
         <v>1667</v>
       </c>
-      <c r="L28" s="61" t="s">
+      <c r="L28" t="s">
         <v>83</v>
       </c>
-      <c r="M28" s="64" t="s">
+      <c r="M28" s="31" t="s">
         <v>125</v>
       </c>
       <c r="N28" s="14">
@@ -5319,7 +5314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114EE0BB-9430-4707-8294-22F3EA198BF4}">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30:J30"/>
     </sheetView>
   </sheetViews>
@@ -6198,16 +6193,16 @@
       <c r="F30">
         <v>23</v>
       </c>
-      <c r="G30" s="61">
+      <c r="G30">
         <v>150</v>
       </c>
-      <c r="H30" s="62" t="s">
+      <c r="H30" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="I30" s="63">
+      <c r="I30" s="59">
         <v>42680</v>
       </c>
-      <c r="J30" s="63">
+      <c r="J30" s="59">
         <v>44087</v>
       </c>
     </row>
@@ -6285,10 +6280,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C891EA49-1228-4754-8524-0795D1247222}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L25" sqref="A1:L25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L27" sqref="A2:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6297,10 +6292,11 @@
     <col min="2" max="2" width="16.109375" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
     <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" customWidth="1"/>
     <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.21875" bestFit="1" customWidth="1"/>
@@ -6308,18 +6304,18 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="46"/>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60" t="s">
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -6799,8 +6795,8 @@
       <c r="C15" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="29" t="s">
-        <v>12</v>
+      <c r="D15" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E15" s="15">
         <v>2668</v>
@@ -6834,8 +6830,8 @@
       <c r="C16" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="31" t="s">
-        <v>12</v>
+      <c r="D16" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E16" s="14">
         <v>4777</v>
@@ -6862,15 +6858,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="31" t="s">
-        <v>12</v>
+      <c r="D17" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E17" s="14">
         <v>324</v>
@@ -6897,15 +6893,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="31" t="s">
-        <v>12</v>
+      <c r="D18" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E18">
         <v>350</v>
@@ -6932,15 +6928,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="31" t="s">
-        <v>12</v>
+      <c r="D19" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E19">
         <v>2141</v>
@@ -6967,7 +6963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="10" t="s">
         <v>31</v>
@@ -6975,8 +6971,8 @@
       <c r="C20" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="30" t="s">
-        <v>12</v>
+      <c r="D20" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E20" s="10">
         <v>5655</v>
@@ -7003,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>15</v>
       </c>
@@ -7041,7 +7037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>41</v>
       </c>
@@ -7076,7 +7072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>42</v>
       </c>
@@ -7111,7 +7107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="10" t="s">
         <v>43</v>
@@ -7147,7 +7143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>21</v>
       </c>
@@ -7183,6 +7179,85 @@
       </c>
       <c r="L25" s="50">
         <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="14">
+        <v>626</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" s="14">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>279</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" s="17">
+        <v>347</v>
+      </c>
+      <c r="M26" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="14">
+        <v>2012</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>47</v>
+      </c>
+      <c r="H27">
+        <v>100</v>
+      </c>
+      <c r="I27" s="14">
+        <v>83</v>
+      </c>
+      <c r="J27">
+        <v>1928</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" s="17">
+        <v>0</v>
+      </c>
+      <c r="M27" s="14" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add UAF data to deployment summary
</commit_message>
<xml_diff>
--- a/Documentation/Summary.xlsx
+++ b/Documentation/Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaity\Documents\GitHub\DCLDE2026\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B40B24-E6E8-4F01-A895-DB84F4ED9F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ECFF6A-6972-4B76-8BA2-2786B2D3E0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2484" yWindow="348" windowWidth="19716" windowHeight="10488" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
+    <workbookView xWindow="576" yWindow="0" windowWidth="20928" windowHeight="10488" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Table 2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="144">
   <si>
     <t>Annotations</t>
   </si>
@@ -427,9 +428,6 @@
   </si>
   <si>
     <t>RB</t>
-  </si>
-  <si>
-    <t>XX</t>
   </si>
   <si>
     <r>
@@ -445,6 +443,45 @@
       </rPr>
       <t>xxx</t>
     </r>
+  </si>
+  <si>
+    <t>ST300-67391498</t>
+  </si>
+  <si>
+    <t>ST300-5354</t>
+  </si>
+  <si>
+    <t>ST300-67424266</t>
+  </si>
+  <si>
+    <t>ST300-67383303</t>
+  </si>
+  <si>
+    <t>ST500-5360</t>
+  </si>
+  <si>
+    <t>ST600-6897</t>
+  </si>
+  <si>
+    <t>ST500-671879205</t>
+  </si>
+  <si>
+    <t>ST300-335826997</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8-10</t>
+  </si>
+  <si>
+    <t>SAR</t>
+  </si>
+  <si>
+    <t>Kenai Fjords and Prince William Sound*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTI-96 min with TASCAM DR100 /ST300 </t>
   </si>
 </sst>
 </file>
@@ -803,7 +840,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -916,17 +953,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -946,10 +976,24 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1264,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4A8866-C81C-482A-B0A6-264BECA1C8D5}">
-  <dimension ref="A1:BZ38"/>
+  <dimension ref="A1:CA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1294,20 +1338,21 @@
     <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="P1" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-    </row>
-    <row r="2" spans="1:78" s="21" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:79" x14ac:dyDescent="0.3">
+      <c r="P1" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+    </row>
+    <row r="2" spans="1:79" s="21" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
@@ -1372,16 +1417,19 @@
         <v>53</v>
       </c>
       <c r="V2" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="W2" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="W2" s="21" t="s">
+      <c r="X2" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="X2" s="23" t="s">
+      <c r="Y2" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1391,10 +1439,10 @@
       <c r="C3" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="69">
+      <c r="D3" s="66">
         <v>48.5248469</v>
       </c>
-      <c r="E3" s="69">
+      <c r="E3" s="66">
         <v>-123.15916470000001</v>
       </c>
       <c r="F3">
@@ -1442,21 +1490,24 @@
       <c r="W3">
         <v>0</v>
       </c>
-      <c r="X3" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="69">
+      <c r="D4" s="66">
         <v>48.5248469</v>
       </c>
-      <c r="E4" s="69">
+      <c r="E4" s="66">
         <v>-123.15916470000001</v>
       </c>
       <c r="F4">
@@ -1504,10 +1555,12 @@
       <c r="W4">
         <v>0</v>
       </c>
-      <c r="X4" s="17">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="4"/>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="17">
+        <v>0</v>
+      </c>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
@@ -1551,20 +1604,21 @@
       <c r="BN4" s="4"/>
       <c r="BO4" s="4"/>
       <c r="BP4" s="4"/>
-      <c r="BR4" s="14"/>
-      <c r="BZ4" s="17"/>
-    </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="BQ4" s="4"/>
+      <c r="BS4" s="14"/>
+      <c r="CA4" s="17"/>
+    </row>
+    <row r="5" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="69">
+      <c r="D5" s="66">
         <v>48.5248469</v>
       </c>
-      <c r="E5" s="69">
+      <c r="E5" s="66">
         <v>-123.15916470000001</v>
       </c>
       <c r="F5">
@@ -1612,21 +1666,24 @@
       <c r="W5">
         <v>0</v>
       </c>
-      <c r="X5" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="69">
+      <c r="D6" s="66">
         <v>48.5248469</v>
       </c>
-      <c r="E6" s="69">
+      <c r="E6" s="66">
         <v>-123.15916470000001</v>
       </c>
       <c r="F6">
@@ -1674,21 +1731,24 @@
       <c r="W6">
         <v>0</v>
       </c>
-      <c r="X6" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="69">
+      <c r="D7" s="66">
         <v>48.5248469</v>
       </c>
-      <c r="E7" s="69">
+      <c r="E7" s="66">
         <v>-123.15916470000001</v>
       </c>
       <c r="F7">
@@ -1736,21 +1796,24 @@
       <c r="W7">
         <v>0</v>
       </c>
-      <c r="X7" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>86</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="69">
+      <c r="D8" s="66">
         <v>48.135399999999997</v>
       </c>
-      <c r="E8" s="69">
+      <c r="E8" s="66">
         <v>-122.76</v>
       </c>
       <c r="F8">
@@ -1798,21 +1861,24 @@
       <c r="W8">
         <v>0</v>
       </c>
-      <c r="X8" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="69">
+      <c r="D9" s="66">
         <v>48.0310074</v>
       </c>
-      <c r="E9" s="69">
+      <c r="E9" s="66">
         <v>-122.6082001</v>
       </c>
       <c r="F9">
@@ -1860,21 +1926,24 @@
       <c r="W9">
         <v>0</v>
       </c>
-      <c r="X9" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="69">
+      <c r="D10" s="66">
         <v>48.0310074</v>
       </c>
-      <c r="E10" s="69">
+      <c r="E10" s="66">
         <v>-122.6082001</v>
       </c>
       <c r="F10">
@@ -1922,21 +1991,24 @@
       <c r="W10">
         <v>0</v>
       </c>
-      <c r="X10" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>86</v>
       </c>
       <c r="C11" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="69">
+      <c r="D11" s="66">
         <v>48.135399999999997</v>
       </c>
-      <c r="E11" s="69">
+      <c r="E11" s="66">
         <v>-122.76</v>
       </c>
       <c r="F11">
@@ -1984,11 +2056,14 @@
       <c r="W11">
         <v>0</v>
       </c>
-      <c r="X11" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:78" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:79" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
@@ -1998,11 +2073,11 @@
       <c r="C12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="70">
+      <c r="D12" s="67">
         <v>48.426000000000002</v>
       </c>
-      <c r="E12" s="70">
-        <v>126.17400000000001</v>
+      <c r="E12" s="67">
+        <v>-126.17400000000001</v>
       </c>
       <c r="F12" s="6">
         <v>40</v>
@@ -2047,16 +2122,19 @@
         <v>130</v>
       </c>
       <c r="V12" s="6">
+        <v>0</v>
+      </c>
+      <c r="W12" s="6">
         <v>834</v>
       </c>
-      <c r="W12" s="6">
-        <v>0</v>
-      </c>
-      <c r="X12" s="48">
+      <c r="X12" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="48">
         <v>418</v>
       </c>
     </row>
-    <row r="13" spans="1:78" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:79" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>96</v>
       </c>
@@ -2066,10 +2144,10 @@
       <c r="C13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="71" t="s">
+      <c r="D13" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="71" t="s">
+      <c r="E13" s="68" t="s">
         <v>60</v>
       </c>
       <c r="F13" s="8">
@@ -2119,26 +2197,29 @@
         <v>48</v>
       </c>
       <c r="V13" s="8">
+        <v>0</v>
+      </c>
+      <c r="W13" s="8">
         <v>5336</v>
       </c>
-      <c r="W13" s="8">
+      <c r="X13" s="8">
         <v>4558</v>
       </c>
-      <c r="X13" s="29">
+      <c r="Y13" s="29">
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:78" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:79" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="72" t="s">
+      <c r="D14" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="72" t="s">
+      <c r="E14" s="69" t="s">
         <v>60</v>
       </c>
       <c r="F14" s="10">
@@ -2188,16 +2269,19 @@
         <v>0</v>
       </c>
       <c r="V14" s="10">
+        <v>0</v>
+      </c>
+      <c r="W14" s="10">
         <v>2309</v>
       </c>
-      <c r="W14" s="10">
+      <c r="X14" s="10">
         <v>3501</v>
       </c>
-      <c r="X14" s="30">
+      <c r="Y14" s="30">
         <v>947</v>
       </c>
     </row>
-    <row r="15" spans="1:78" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:79" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>95</v>
       </c>
@@ -2207,10 +2291,10 @@
       <c r="C15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="71" t="s">
+      <c r="E15" s="68" t="s">
         <v>60</v>
       </c>
       <c r="F15" s="8">
@@ -2260,26 +2344,29 @@
         <v>1610</v>
       </c>
       <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
         <v>694</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>364</v>
       </c>
-      <c r="X15" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:78" x14ac:dyDescent="0.3">
+      <c r="Y15" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="69" t="s">
+      <c r="D16" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="69" t="s">
+      <c r="E16" s="66" t="s">
         <v>60</v>
       </c>
       <c r="F16">
@@ -2328,26 +2415,29 @@
         <v>4184</v>
       </c>
       <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
         <v>593</v>
       </c>
-      <c r="W16">
-        <v>0</v>
-      </c>
-      <c r="X16" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="69" t="s">
+      <c r="D17" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="69" t="s">
+      <c r="E17" s="66" t="s">
         <v>60</v>
       </c>
       <c r="F17">
@@ -2396,26 +2486,29 @@
         <v>0</v>
       </c>
       <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
         <v>324</v>
       </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="69" t="s">
+      <c r="D18" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="69" t="s">
+      <c r="E18" s="66" t="s">
         <v>60</v>
       </c>
       <c r="F18">
@@ -2464,26 +2557,29 @@
         <v>159</v>
       </c>
       <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
         <v>191</v>
       </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="X18" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>37</v>
       </c>
       <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="69" t="s">
+      <c r="D19" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="69" t="s">
+      <c r="E19" s="66" t="s">
         <v>60</v>
       </c>
       <c r="F19">
@@ -2532,26 +2628,29 @@
         <v>2070</v>
       </c>
       <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
         <v>71</v>
       </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
-      <c r="X19" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="72" t="s">
+      <c r="D20" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="72" t="s">
+      <c r="E20" s="69" t="s">
         <v>60</v>
       </c>
       <c r="F20" s="10">
@@ -2601,16 +2700,19 @@
         <v>5630</v>
       </c>
       <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
         <v>25</v>
       </c>
-      <c r="W20" s="10">
-        <v>0</v>
-      </c>
-      <c r="X20" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X20" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>15</v>
       </c>
@@ -2620,11 +2722,11 @@
       <c r="C21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="71">
+      <c r="D21" s="68">
         <v>48.686</v>
       </c>
-      <c r="E21" s="71">
-        <v>123.274</v>
+      <c r="E21" s="68">
+        <v>-123.274</v>
       </c>
       <c r="F21" s="8">
         <v>237</v>
@@ -2669,27 +2771,30 @@
         <v>2574</v>
       </c>
       <c r="V21" s="8">
+        <v>0</v>
+      </c>
+      <c r="W21" s="8">
         <v>937</v>
       </c>
-      <c r="W21" s="8">
-        <v>0</v>
-      </c>
-      <c r="X21" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X21" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="69">
+      <c r="D22" s="66">
         <v>48.506999999999998</v>
       </c>
-      <c r="E22" s="69">
-        <v>123.211</v>
+      <c r="E22" s="66">
+        <v>-123.211</v>
       </c>
       <c r="F22">
         <v>188</v>
@@ -2731,27 +2836,30 @@
         <v>7647</v>
       </c>
       <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
         <v>318</v>
       </c>
-      <c r="W22">
-        <v>0</v>
-      </c>
-      <c r="X22" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="69">
+      <c r="D23" s="66">
         <v>48.494999999999997</v>
       </c>
-      <c r="E23" s="69">
-        <v>124.54</v>
+      <c r="E23" s="66">
+        <v>-124.54</v>
       </c>
       <c r="F23">
         <v>213</v>
@@ -2793,27 +2901,30 @@
         <v>395</v>
       </c>
       <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
         <v>994</v>
       </c>
-      <c r="W23">
-        <v>0</v>
-      </c>
-      <c r="X23" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="72">
+      <c r="D24" s="69">
         <v>48.774999999999999</v>
       </c>
-      <c r="E24" s="72">
-        <v>123.343</v>
+      <c r="E24" s="69">
+        <v>-123.343</v>
       </c>
       <c r="F24" s="10">
         <v>74</v>
@@ -2858,16 +2969,19 @@
         <v>519</v>
       </c>
       <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
         <v>242</v>
       </c>
-      <c r="W24" s="10">
-        <v>0</v>
-      </c>
-      <c r="X24" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X24" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>21</v>
       </c>
@@ -2877,11 +2991,11 @@
       <c r="C25" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="70">
+      <c r="D25" s="67">
         <v>48.78</v>
       </c>
-      <c r="E25" s="70">
-        <v>123.05200000000001</v>
+      <c r="E25" s="67">
+        <v>-123.05200000000001</v>
       </c>
       <c r="F25" s="6">
         <v>27</v>
@@ -2931,11 +3045,14 @@
       <c r="W25" s="6">
         <v>0</v>
       </c>
-      <c r="X25" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X25" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -2945,11 +3062,11 @@
       <c r="C26" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="69">
+      <c r="D26" s="66">
         <v>47.357999999999997</v>
       </c>
-      <c r="E26" s="69">
-        <v>124.68333333333334</v>
+      <c r="E26" s="66">
+        <v>-124.683333333333</v>
       </c>
       <c r="F26">
         <v>100</v>
@@ -2960,16 +3077,16 @@
       <c r="H26" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="K26" s="68">
+      <c r="K26" s="65">
         <v>39616</v>
       </c>
-      <c r="L26" s="68">
+      <c r="L26" s="65">
         <v>40925</v>
       </c>
       <c r="N26" s="41">
         <v>2159</v>
       </c>
-      <c r="O26" s="77" t="s">
+      <c r="O26" t="s">
         <v>82</v>
       </c>
       <c r="P26" s="15" t="s">
@@ -2991,27 +3108,30 @@
         <v>0</v>
       </c>
       <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
         <v>279</v>
       </c>
-      <c r="W26">
-        <v>0</v>
-      </c>
-      <c r="X26" s="31">
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="31">
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>99</v>
       </c>
       <c r="C27" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="69">
+      <c r="D27" s="66">
         <v>47.5</v>
       </c>
-      <c r="E27" s="69">
-        <v>125.35333333333334</v>
+      <c r="E27" s="66">
+        <v>-125.353333333333</v>
       </c>
       <c r="F27">
         <v>1400</v>
@@ -3022,16 +3142,16 @@
       <c r="H27" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="K27" s="68">
+      <c r="K27" s="65">
         <v>40570</v>
       </c>
-      <c r="L27" s="68">
+      <c r="L27" s="65">
         <v>41455</v>
       </c>
       <c r="N27" s="41">
         <v>636</v>
       </c>
-      <c r="O27" s="77" t="s">
+      <c r="O27" t="s">
         <v>82</v>
       </c>
       <c r="P27" s="14" t="s">
@@ -3053,16 +3173,19 @@
         <v>83</v>
       </c>
       <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
         <v>1928</v>
       </c>
-      <c r="W27">
-        <v>0</v>
-      </c>
-      <c r="X27" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>102</v>
       </c>
@@ -3072,10 +3195,10 @@
       <c r="C28" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="73">
+      <c r="D28" s="70">
         <v>48.518050000000002</v>
       </c>
-      <c r="E28" s="73">
+      <c r="E28" s="70">
         <v>-123.19166666666599</v>
       </c>
       <c r="F28" s="8">
@@ -3123,21 +3246,24 @@
       <c r="W28" s="8">
         <v>0</v>
       </c>
-      <c r="X28" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X28" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>104</v>
       </c>
       <c r="C29" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="74">
+      <c r="D29" s="71">
         <v>48.5167</v>
       </c>
-      <c r="E29" s="74">
+      <c r="E29" s="71">
         <v>-123.207616666666</v>
       </c>
       <c r="F29">
@@ -3177,26 +3303,29 @@
         <v>2658</v>
       </c>
       <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
         <v>57</v>
       </c>
-      <c r="W29">
-        <v>0</v>
-      </c>
-      <c r="X29" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>106</v>
       </c>
       <c r="C30" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="74">
+      <c r="D30" s="71">
         <v>48.760779999999997</v>
       </c>
-      <c r="E30" s="74">
+      <c r="E30" s="71">
         <v>-123.06793999999999</v>
       </c>
       <c r="F30">
@@ -3239,16 +3368,19 @@
         <v>988</v>
       </c>
       <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
         <v>47</v>
       </c>
-      <c r="W30">
-        <v>0</v>
-      </c>
-      <c r="X30" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -3258,10 +3390,10 @@
       <c r="C31" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="72">
+      <c r="D31" s="69">
         <v>49.042645</v>
       </c>
-      <c r="E31" s="72">
+      <c r="E31" s="69">
         <v>-123.31744</v>
       </c>
       <c r="F31" s="10">
@@ -3307,16 +3439,19 @@
         <v>1297</v>
       </c>
       <c r="V31" s="10">
+        <v>0</v>
+      </c>
+      <c r="W31" s="10">
         <v>248</v>
       </c>
-      <c r="W31" s="10">
-        <v>0</v>
-      </c>
-      <c r="X31" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X31" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>116</v>
       </c>
@@ -3326,10 +3461,10 @@
       <c r="C32" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="75">
+      <c r="D32" s="72">
         <v>48.51</v>
       </c>
-      <c r="E32" s="75">
+      <c r="E32" s="72">
         <v>-123.15</v>
       </c>
       <c r="F32" s="6">
@@ -3339,14 +3474,14 @@
         <v>150</v>
       </c>
       <c r="H32" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
-      <c r="K32" s="62">
+      <c r="K32" s="60">
         <v>42680</v>
       </c>
-      <c r="L32" s="62">
+      <c r="L32" s="60">
         <v>44087</v>
       </c>
       <c r="M32" s="6">
@@ -3359,219 +3494,678 @@
       <c r="P32" s="48" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A33" s="63" t="s">
+      <c r="V32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A33" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="63" t="s">
+      <c r="B33" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="63" t="s">
+      <c r="C33" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="74">
+      <c r="D33" s="71">
         <v>60.307499999999997</v>
       </c>
-      <c r="E33" s="74">
-        <v>146.97300000000001</v>
+      <c r="E33" s="71">
+        <v>-146.97300000000001</v>
       </c>
       <c r="F33">
         <v>42</v>
       </c>
-      <c r="G33" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="H33" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="K33"/>
-      <c r="L33"/>
+      <c r="G33" s="63">
+        <v>24</v>
+      </c>
+      <c r="H33" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="K33" s="59">
+        <v>43710</v>
+      </c>
+      <c r="L33" s="59">
+        <v>43662</v>
+      </c>
       <c r="M33"/>
-      <c r="O33" t="s">
+      <c r="N33" s="41">
+        <v>9</v>
+      </c>
+      <c r="O33" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="P33" s="78" t="s">
+      <c r="P33" s="73" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A34" s="63"/>
-      <c r="B34" s="63" t="s">
+      <c r="Q33" s="84">
+        <v>9</v>
+      </c>
+      <c r="R33" s="84">
+        <v>0</v>
+      </c>
+      <c r="S33" s="84">
+        <v>0</v>
+      </c>
+      <c r="T33" s="84">
+        <v>0</v>
+      </c>
+      <c r="U33" s="15">
+        <v>0</v>
+      </c>
+      <c r="V33" s="84">
+        <v>0</v>
+      </c>
+      <c r="W33" s="84">
+        <v>9</v>
+      </c>
+      <c r="X33" s="84">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A34" s="61"/>
+      <c r="B34" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="C34" s="63" t="s">
+      <c r="C34" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="74">
+      <c r="D34" s="71">
         <v>59.876666666666665</v>
       </c>
-      <c r="E34" s="74">
-        <v>151.8485</v>
+      <c r="E34" s="71">
+        <v>-151.8485</v>
       </c>
       <c r="F34">
         <v>21</v>
       </c>
-      <c r="G34" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="H34" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="K34"/>
-      <c r="L34"/>
+      <c r="G34" s="63">
+        <v>24</v>
+      </c>
+      <c r="H34" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="K34" s="59">
+        <v>44406</v>
+      </c>
+      <c r="L34" s="59">
+        <v>44415</v>
+      </c>
       <c r="M34"/>
+      <c r="N34" s="41">
+        <v>32</v>
+      </c>
       <c r="O34" t="s">
         <v>83</v>
       </c>
-      <c r="P34" s="78" t="s">
+      <c r="P34" s="73" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A35" s="63"/>
-      <c r="B35" s="63" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" s="63" t="s">
-        <v>127</v>
-      </c>
-      <c r="D35" s="74">
-        <v>60.175166666666669</v>
-      </c>
-      <c r="E35" s="74">
-        <v>147.81816666666666</v>
+      <c r="Q34" s="84">
+        <v>32</v>
+      </c>
+      <c r="R34" s="84">
+        <v>0</v>
+      </c>
+      <c r="S34" s="84">
+        <v>0</v>
+      </c>
+      <c r="T34" s="84">
+        <v>0</v>
+      </c>
+      <c r="U34" s="14">
+        <v>0</v>
+      </c>
+      <c r="V34" s="84">
+        <v>0</v>
+      </c>
+      <c r="W34" s="84">
+        <v>32</v>
+      </c>
+      <c r="X34" s="84">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="61"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="71">
+        <v>59.876666666666665</v>
+      </c>
+      <c r="E35" s="71">
+        <v>-151.8485</v>
       </c>
       <c r="F35">
-        <v>35</v>
-      </c>
-      <c r="G35" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="H35" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="K35"/>
-      <c r="L35"/>
+        <v>21</v>
+      </c>
+      <c r="G35" s="63">
+        <v>24</v>
+      </c>
+      <c r="H35" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="K35" s="59">
+        <v>43625</v>
+      </c>
+      <c r="L35" s="59">
+        <v>44265</v>
+      </c>
       <c r="M35"/>
+      <c r="N35" s="41">
+        <v>598</v>
+      </c>
       <c r="O35" t="s">
         <v>83</v>
       </c>
-      <c r="P35" s="78" t="s">
+      <c r="P35" s="73" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A36" s="64"/>
-      <c r="B36" s="64" t="s">
+      <c r="Q35" s="84">
+        <v>598</v>
+      </c>
+      <c r="R35" s="84">
+        <v>0</v>
+      </c>
+      <c r="S35" s="84">
+        <v>0</v>
+      </c>
+      <c r="T35" s="84">
+        <v>0</v>
+      </c>
+      <c r="U35" s="14">
+        <v>0</v>
+      </c>
+      <c r="V35" s="84">
+        <v>0</v>
+      </c>
+      <c r="W35" s="84">
+        <v>598</v>
+      </c>
+      <c r="X35" s="84">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="61"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="71">
+        <v>59.876666666666665</v>
+      </c>
+      <c r="E36" s="71">
+        <v>-151.8485</v>
+      </c>
+      <c r="F36">
+        <v>21</v>
+      </c>
+      <c r="G36" s="63">
+        <v>24</v>
+      </c>
+      <c r="H36" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="K36" s="59">
+        <v>44693</v>
+      </c>
+      <c r="L36" s="59">
+        <v>44693</v>
+      </c>
+      <c r="M36"/>
+      <c r="N36" s="41">
+        <v>450</v>
+      </c>
+      <c r="O36" t="s">
+        <v>83</v>
+      </c>
+      <c r="P36" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q36" s="84">
+        <v>450</v>
+      </c>
+      <c r="R36" s="84">
+        <v>0</v>
+      </c>
+      <c r="S36" s="84">
+        <v>0</v>
+      </c>
+      <c r="T36" s="84">
+        <v>0</v>
+      </c>
+      <c r="U36" s="14">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36" s="84">
+        <v>0</v>
+      </c>
+      <c r="X36" s="84">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="61"/>
+      <c r="B37" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="71">
+        <v>60.175166666666669</v>
+      </c>
+      <c r="E37" s="71">
+        <v>-147.818166666667</v>
+      </c>
+      <c r="F37">
+        <v>35</v>
+      </c>
+      <c r="G37" s="63">
+        <v>24</v>
+      </c>
+      <c r="H37" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="K37" s="59">
+        <v>44457</v>
+      </c>
+      <c r="L37" s="59">
+        <v>44349</v>
+      </c>
+      <c r="M37"/>
+      <c r="N37" s="41">
+        <v>97</v>
+      </c>
+      <c r="O37" t="s">
+        <v>83</v>
+      </c>
+      <c r="P37" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q37" s="84">
+        <v>97</v>
+      </c>
+      <c r="R37" s="84">
+        <v>0</v>
+      </c>
+      <c r="S37" s="84">
+        <v>0</v>
+      </c>
+      <c r="T37" s="84">
+        <v>0</v>
+      </c>
+      <c r="U37" s="14">
+        <v>0</v>
+      </c>
+      <c r="V37" s="84">
+        <v>0</v>
+      </c>
+      <c r="W37" s="84">
+        <v>97</v>
+      </c>
+      <c r="X37" s="84">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="61"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="71">
+        <v>60.175166666666669</v>
+      </c>
+      <c r="E38" s="71">
+        <v>-147.818166666667</v>
+      </c>
+      <c r="F38">
+        <v>35</v>
+      </c>
+      <c r="G38" s="63">
+        <v>24</v>
+      </c>
+      <c r="H38" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="K38" s="59">
+        <v>45044</v>
+      </c>
+      <c r="L38" s="59">
+        <v>45044</v>
+      </c>
+      <c r="M38"/>
+      <c r="N38" s="41">
+        <v>373</v>
+      </c>
+      <c r="O38" t="s">
+        <v>83</v>
+      </c>
+      <c r="P38" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q38" s="84">
+        <v>373</v>
+      </c>
+      <c r="R38" s="84">
+        <v>0</v>
+      </c>
+      <c r="S38" s="84">
+        <v>0</v>
+      </c>
+      <c r="T38" s="84">
+        <v>0</v>
+      </c>
+      <c r="U38" s="14">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38" s="84">
+        <v>0</v>
+      </c>
+      <c r="X38" s="84">
+        <v>0</v>
+      </c>
+      <c r="Y38">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A39" s="61"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="71">
+        <v>60.175166666666669</v>
+      </c>
+      <c r="E39" s="71">
+        <v>-147.818166666667</v>
+      </c>
+      <c r="F39">
+        <v>35</v>
+      </c>
+      <c r="G39" s="63">
+        <v>24</v>
+      </c>
+      <c r="H39" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="K39" s="59">
+        <v>43619</v>
+      </c>
+      <c r="L39" s="59">
+        <v>43982</v>
+      </c>
+      <c r="M39"/>
+      <c r="N39" s="41">
+        <v>464</v>
+      </c>
+      <c r="O39" t="s">
+        <v>83</v>
+      </c>
+      <c r="P39" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q39" s="84">
+        <v>464</v>
+      </c>
+      <c r="R39" s="84">
+        <v>0</v>
+      </c>
+      <c r="S39" s="84">
+        <v>0</v>
+      </c>
+      <c r="T39" s="84">
+        <v>0</v>
+      </c>
+      <c r="U39" s="14">
+        <v>0</v>
+      </c>
+      <c r="V39" s="84">
+        <v>0</v>
+      </c>
+      <c r="W39" s="84">
+        <v>464</v>
+      </c>
+      <c r="X39" s="84">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A40" s="76"/>
+      <c r="B40" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="C40" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="76">
+      <c r="D40" s="77">
         <v>59.732666666666667</v>
       </c>
-      <c r="E36" s="76">
-        <v>149.53233333333333</v>
-      </c>
-      <c r="F36" s="10">
+      <c r="E40" s="77">
+        <v>-149.53233333333301</v>
+      </c>
+      <c r="F40" s="78">
         <v>34</v>
       </c>
-      <c r="G36" s="66" t="s">
-        <v>130</v>
-      </c>
-      <c r="H36" s="66" t="s">
-        <v>130</v>
-      </c>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="10" t="s">
+      <c r="G40" s="79">
+        <v>24</v>
+      </c>
+      <c r="H40" s="79" t="s">
+        <v>138</v>
+      </c>
+      <c r="I40" s="80"/>
+      <c r="J40" s="80"/>
+      <c r="K40" s="81">
+        <v>43789</v>
+      </c>
+      <c r="L40" s="81">
+        <v>43884</v>
+      </c>
+      <c r="M40" s="78"/>
+      <c r="N40" s="82">
+        <v>12</v>
+      </c>
+      <c r="O40" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="P36" s="79" t="s">
+      <c r="P40" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="10"/>
-      <c r="U36" s="10"/>
-      <c r="V36" s="10"/>
-      <c r="W36" s="10"/>
-      <c r="X36" s="10"/>
-    </row>
-    <row r="37" spans="1:24" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="P37" s="52"/>
-      <c r="Q37" s="33" t="s">
+      <c r="Q40" s="84">
+        <v>12</v>
+      </c>
+      <c r="R40" s="84">
+        <v>0</v>
+      </c>
+      <c r="S40" s="84">
+        <v>0</v>
+      </c>
+      <c r="T40" s="84">
+        <v>0</v>
+      </c>
+      <c r="U40" s="14">
+        <v>0</v>
+      </c>
+      <c r="V40" s="84">
+        <v>0</v>
+      </c>
+      <c r="W40" s="84">
+        <v>12</v>
+      </c>
+      <c r="X40" s="84">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A41" s="76"/>
+      <c r="B41" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="62" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" s="77">
+        <v>60.148490000000002</v>
+      </c>
+      <c r="E41" s="77">
+        <v>-147.58500000000001</v>
+      </c>
+      <c r="F41" s="83" t="s">
+        <v>140</v>
+      </c>
+      <c r="G41" s="63"/>
+      <c r="H41" s="79" t="s">
+        <v>143</v>
+      </c>
+      <c r="I41" s="80"/>
+      <c r="J41" s="80"/>
+      <c r="K41" s="81"/>
+      <c r="L41" s="81"/>
+      <c r="M41" s="78"/>
+      <c r="N41" s="82"/>
+      <c r="O41" s="78"/>
+      <c r="P41" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q41" s="84">
+        <v>7717</v>
+      </c>
+      <c r="R41" s="84">
+        <v>0</v>
+      </c>
+      <c r="S41" s="84">
+        <v>0</v>
+      </c>
+      <c r="T41" s="84">
+        <v>0</v>
+      </c>
+      <c r="U41" s="14">
+        <v>0</v>
+      </c>
+      <c r="V41" s="78">
+        <v>7717</v>
+      </c>
+      <c r="W41" s="84">
+        <v>0</v>
+      </c>
+      <c r="X41" s="84">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P42" s="52"/>
+      <c r="Q42" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="R37" s="21" t="s">
+      <c r="R42" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="S37" s="21" t="s">
+      <c r="S42" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="T37" s="21" t="s">
+      <c r="T42" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="U37" s="33" t="s">
+      <c r="U42" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="V37" s="21" t="s">
+      <c r="V42" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="W42" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="W37" s="21" t="s">
+      <c r="X42" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="X37" s="67" t="s">
+      <c r="Y42" s="64" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="P38" s="52" t="s">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="H43" s="53">
+        <v>67383303</v>
+      </c>
+      <c r="P43" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="Q38" s="14">
-        <f>SUM(Q3:Q31)</f>
-        <v>83924</v>
-      </c>
-      <c r="R38" s="14">
-        <f t="shared" ref="R38:X38" si="0">SUM(R3:R31)</f>
+      <c r="Q43" s="14">
+        <f t="shared" ref="Q43:S43" si="0">SUM(Q3:Q41)</f>
+        <v>93676</v>
+      </c>
+      <c r="R43" s="14">
+        <f t="shared" si="0"/>
         <v>22944</v>
       </c>
-      <c r="S38" s="14">
+      <c r="S43" s="14">
         <f t="shared" si="0"/>
         <v>15058</v>
       </c>
-      <c r="T38" s="14">
-        <f t="shared" si="0"/>
+      <c r="T43" s="14">
+        <f>SUM(T3:T41)</f>
         <v>128593</v>
       </c>
-      <c r="U38" s="14">
-        <f t="shared" si="0"/>
+      <c r="U43" s="14">
+        <f>SUM(U3:U41)</f>
         <v>38406</v>
       </c>
-      <c r="V38" s="14">
-        <f t="shared" si="0"/>
+      <c r="V43" s="14">
+        <f>SUM(V3:V41)</f>
+        <v>7717</v>
+      </c>
+      <c r="W43" s="14">
+        <f t="shared" ref="R43:Y43" si="1">SUM(W3:W31)</f>
         <v>15427</v>
       </c>
-      <c r="W38" s="14">
-        <f t="shared" si="0"/>
+      <c r="X43" s="14">
+        <f t="shared" si="1"/>
         <v>8423</v>
       </c>
-      <c r="X38" s="14">
-        <f t="shared" si="0"/>
+      <c r="Y43" s="14">
+        <f t="shared" si="1"/>
         <v>1970</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="P1:X1"/>
+    <mergeCell ref="P1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3603,17 +4197,17 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="41"/>
-      <c r="M1" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
+      <c r="M1" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
     </row>
     <row r="2" spans="1:75" s="21" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
@@ -5317,12 +5911,12 @@
         <v>150</v>
       </c>
       <c r="H28" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="I28" s="62">
+        <v>130</v>
+      </c>
+      <c r="I28" s="60">
         <v>42680</v>
       </c>
-      <c r="J28" s="62">
+      <c r="J28" s="60">
         <v>44087</v>
       </c>
       <c r="K28" s="6">
@@ -5392,35 +5986,35 @@
         <v>79</v>
       </c>
       <c r="N33" s="14">
-        <f>SUM(N2:N28)</f>
+        <f t="shared" ref="N33:U33" si="0">SUM(N2:N28)</f>
         <v>57654</v>
       </c>
       <c r="O33" s="14">
-        <f>SUM(O2:O28)</f>
+        <f t="shared" si="0"/>
         <v>23035</v>
       </c>
       <c r="P33" s="14">
-        <f>SUM(P2:P28)</f>
+        <f t="shared" si="0"/>
         <v>9208</v>
       </c>
       <c r="Q33" s="14">
-        <f>SUM(Q2:Q28)</f>
+        <f t="shared" si="0"/>
         <v>127353</v>
       </c>
       <c r="R33" s="14">
-        <f>SUM(R2:R28)</f>
+        <f t="shared" si="0"/>
         <v>28031</v>
       </c>
       <c r="S33" s="14">
-        <f>SUM(S2:S28)</f>
+        <f t="shared" si="0"/>
         <v>12936</v>
       </c>
       <c r="T33" s="14">
-        <f>SUM(T2:T28)</f>
+        <f t="shared" si="0"/>
         <v>8423</v>
       </c>
       <c r="U33" s="14">
-        <f>SUM(U2:U28)</f>
+        <f t="shared" si="0"/>
         <v>1970</v>
       </c>
     </row>
@@ -6426,18 +7020,18 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="46"/>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61" t="s">
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
     </row>
     <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">

</xml_diff>

<commit_message>
update SMRU hydrophone, add reviewer copy
</commit_message>
<xml_diff>
--- a/Documentation/Summary.xlsx
+++ b/Documentation/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaity\Documents\GitHub\DCLDE2026\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E44F66-12BE-4F2B-ABA1-66D14825A963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6190B8F-6BCC-47FA-BDF4-D28C6634B91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7752" yWindow="684" windowWidth="18072" windowHeight="10488" activeTab="2" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
+    <workbookView xWindow="-1512" yWindow="2292" windowWidth="18072" windowHeight="10488" activeTab="1" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="175">
   <si>
     <t>Annotations</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t xml:space="preserve">RB_67424266 </t>
+  </si>
+  <si>
+    <t>Reson TC4032</t>
   </si>
 </sst>
 </file>
@@ -4338,8 +4341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCCC199-A41A-4F1A-82DB-36CD09435BF7}">
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5715,7 +5718,7 @@
         <v>150</v>
       </c>
       <c r="H22" s="46" t="s">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="I22" s="50">
         <v>42680</v>
@@ -6661,8 +6664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114EE0BB-9430-4707-8294-22F3EA198BF4}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C30"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7503,9 +7506,8 @@
         <f>NoMalahat!G22</f>
         <v>150</v>
       </c>
-      <c r="H22" s="46" t="str">
-        <f>NoMalahat!H22</f>
-        <v>HTI-xxx</v>
+      <c r="H22" t="s">
+        <v>174</v>
       </c>
       <c r="I22" s="94">
         <f>NoMalahat!I22</f>

</xml_diff>

<commit_message>
Update DFO CRP data, change BKW to TKW
</commit_message>
<xml_diff>
--- a/Documentation/Summary.xlsx
+++ b/Documentation/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaity\Documents\GitHub\DCLDE2026\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6190B8F-6BCC-47FA-BDF4-D28C6634B91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FE12C6-6BA0-4E44-AB89-961FDB066730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1512" yWindow="2292" windowWidth="18072" windowHeight="10488" activeTab="1" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
+    <workbookView xWindow="3048" yWindow="804" windowWidth="18072" windowHeight="10488" activeTab="2" xr2:uid="{72309623-07FF-4432-9886-908A2F1E9C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -969,7 +969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1095,19 +1095,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1168,8 +1155,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1515,19 +1510,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.3">
-      <c r="P1" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71"/>
+      <c r="P1" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
     </row>
     <row r="2" spans="1:79" s="18" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -1732,7 +1727,7 @@
       <c r="W4">
         <v>0</v>
       </c>
-      <c r="X4" s="98">
+      <c r="X4">
         <v>0</v>
       </c>
       <c r="Y4" s="17">
@@ -1843,7 +1838,7 @@
       <c r="W5">
         <v>0</v>
       </c>
-      <c r="X5" s="98">
+      <c r="X5">
         <v>0</v>
       </c>
       <c r="Y5" s="17">
@@ -1908,7 +1903,7 @@
       <c r="W6">
         <v>0</v>
       </c>
-      <c r="X6" s="98">
+      <c r="X6">
         <v>0</v>
       </c>
       <c r="Y6" s="17">
@@ -1973,7 +1968,7 @@
       <c r="W7">
         <v>0</v>
       </c>
-      <c r="X7" s="98">
+      <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7" s="17">
@@ -2038,7 +2033,7 @@
       <c r="W8">
         <v>0</v>
       </c>
-      <c r="X8" s="98">
+      <c r="X8">
         <v>0</v>
       </c>
       <c r="Y8" s="17">
@@ -2103,7 +2098,7 @@
       <c r="W9">
         <v>0</v>
       </c>
-      <c r="X9" s="98">
+      <c r="X9">
         <v>0</v>
       </c>
       <c r="Y9" s="17">
@@ -2168,7 +2163,7 @@
       <c r="W10">
         <v>0</v>
       </c>
-      <c r="X10" s="98">
+      <c r="X10">
         <v>0</v>
       </c>
       <c r="Y10" s="17">
@@ -2233,7 +2228,7 @@
       <c r="W11">
         <v>0</v>
       </c>
-      <c r="X11" s="98">
+      <c r="X11">
         <v>0</v>
       </c>
       <c r="Y11" s="17">
@@ -2526,7 +2521,7 @@
       <c r="W15">
         <v>364</v>
       </c>
-      <c r="X15" s="98">
+      <c r="X15">
         <v>694</v>
       </c>
       <c r="Y15" s="70">
@@ -2597,7 +2592,7 @@
       <c r="W16">
         <v>0</v>
       </c>
-      <c r="X16" s="98">
+      <c r="X16">
         <v>593</v>
       </c>
       <c r="Y16" s="17">
@@ -2668,7 +2663,7 @@
       <c r="W17">
         <v>0</v>
       </c>
-      <c r="X17" s="98">
+      <c r="X17">
         <v>324</v>
       </c>
       <c r="Y17" s="17">
@@ -2739,7 +2734,7 @@
       <c r="W18">
         <v>0</v>
       </c>
-      <c r="X18" s="98">
+      <c r="X18">
         <v>191</v>
       </c>
       <c r="Y18" s="17">
@@ -2810,7 +2805,7 @@
       <c r="W19">
         <v>0</v>
       </c>
-      <c r="X19" s="98">
+      <c r="X19">
         <v>71</v>
       </c>
       <c r="Y19" s="17">
@@ -2882,7 +2877,7 @@
       <c r="W20" s="10">
         <v>0</v>
       </c>
-      <c r="X20" s="98">
+      <c r="X20">
         <v>25</v>
       </c>
       <c r="Y20" s="68">
@@ -3018,7 +3013,7 @@
       <c r="W22">
         <v>0</v>
       </c>
-      <c r="X22" s="98">
+      <c r="X22">
         <v>318</v>
       </c>
       <c r="Y22" s="17">
@@ -3083,7 +3078,7 @@
       <c r="W23">
         <v>0</v>
       </c>
-      <c r="X23" s="98">
+      <c r="X23">
         <v>994</v>
       </c>
       <c r="Y23" s="17">
@@ -3151,7 +3146,7 @@
       <c r="W24" s="10">
         <v>0</v>
       </c>
-      <c r="X24" s="98">
+      <c r="X24">
         <v>242</v>
       </c>
       <c r="Y24" s="68">
@@ -3290,7 +3285,7 @@
       <c r="W26">
         <v>0</v>
       </c>
-      <c r="X26" s="98">
+      <c r="X26">
         <v>279</v>
       </c>
       <c r="Y26" s="17">
@@ -3355,7 +3350,7 @@
       <c r="W27">
         <v>0</v>
       </c>
-      <c r="X27" s="98">
+      <c r="X27">
         <v>1928</v>
       </c>
       <c r="Y27" s="17">
@@ -3485,7 +3480,7 @@
       <c r="W29">
         <v>0</v>
       </c>
-      <c r="X29" s="98">
+      <c r="X29">
         <v>57</v>
       </c>
       <c r="Y29" s="17">
@@ -3550,7 +3545,7 @@
       <c r="W30">
         <v>0</v>
       </c>
-      <c r="X30" s="98">
+      <c r="X30">
         <v>47</v>
       </c>
       <c r="Y30" s="17">
@@ -3761,7 +3756,7 @@
       <c r="W33">
         <v>0</v>
       </c>
-      <c r="X33" s="98">
+      <c r="X33">
         <v>9</v>
       </c>
       <c r="Y33" s="17">
@@ -3827,7 +3822,7 @@
       <c r="W34">
         <v>0</v>
       </c>
-      <c r="X34" s="98">
+      <c r="X34">
         <v>32</v>
       </c>
       <c r="Y34" s="17">
@@ -3890,7 +3885,7 @@
       <c r="W35">
         <v>0</v>
       </c>
-      <c r="X35" s="98">
+      <c r="X35">
         <v>598</v>
       </c>
       <c r="Y35" s="17">
@@ -3953,7 +3948,7 @@
       <c r="W36">
         <v>0</v>
       </c>
-      <c r="X36" s="98">
+      <c r="X36">
         <v>0</v>
       </c>
       <c r="Y36" s="17">
@@ -4019,7 +4014,7 @@
       <c r="W37">
         <v>0</v>
       </c>
-      <c r="X37" s="98">
+      <c r="X37">
         <v>97</v>
       </c>
       <c r="Y37" s="17">
@@ -4082,7 +4077,7 @@
       <c r="W38">
         <v>0</v>
       </c>
-      <c r="X38" s="98">
+      <c r="X38">
         <v>0</v>
       </c>
       <c r="Y38" s="17">
@@ -4145,7 +4140,7 @@
       <c r="W39">
         <v>0</v>
       </c>
-      <c r="X39" s="98">
+      <c r="X39">
         <v>464</v>
       </c>
       <c r="Y39" s="17">
@@ -4212,7 +4207,7 @@
       <c r="W40">
         <v>0</v>
       </c>
-      <c r="X40" s="98">
+      <c r="X40">
         <v>12</v>
       </c>
       <c r="Y40" s="17">
@@ -4273,7 +4268,7 @@
       <c r="W41">
         <v>0</v>
       </c>
-      <c r="X41" s="98">
+      <c r="X41">
         <v>0</v>
       </c>
       <c r="Y41" s="17">
@@ -4341,8 +4336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCCC199-A41A-4F1A-82DB-36CD09435BF7}">
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4351,12 +4346,12 @@
     <col min="2" max="2" width="45.6640625" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="31.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
@@ -4364,14 +4359,14 @@
       <c r="E1" s="21"/>
       <c r="H1" s="44"/>
       <c r="I1" s="35"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
     </row>
     <row r="2" spans="1:22" s="18" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -4629,7 +4624,7 @@
       <c r="S5">
         <v>0</v>
       </c>
-      <c r="T5" s="98">
+      <c r="T5">
         <v>0</v>
       </c>
       <c r="U5">
@@ -4680,19 +4675,19 @@
         <v>10</v>
       </c>
       <c r="N6" s="41">
-        <v>1626</v>
+        <v>982</v>
       </c>
       <c r="O6" s="6">
-        <v>9392</v>
+        <v>8185</v>
       </c>
       <c r="P6" s="6">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="6">
-        <v>2946</v>
-      </c>
-      <c r="R6" s="99">
-        <v>130</v>
+        <v>3539</v>
+      </c>
+      <c r="R6" s="91">
+        <v>125</v>
       </c>
       <c r="S6" s="6">
         <v>0</v>
@@ -4701,10 +4696,10 @@
         <v>0</v>
       </c>
       <c r="U6" s="6">
-        <v>834</v>
+        <v>349</v>
       </c>
       <c r="V6" s="69">
-        <v>418</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4815,7 +4810,7 @@
       <c r="N8" s="14">
         <v>6886</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8">
         <v>10696</v>
       </c>
       <c r="P8">
@@ -4898,7 +4893,7 @@
       <c r="S9">
         <v>0</v>
       </c>
-      <c r="T9" s="98">
+      <c r="T9">
         <v>364</v>
       </c>
       <c r="U9">
@@ -4963,7 +4958,7 @@
       <c r="S10">
         <v>0</v>
       </c>
-      <c r="T10" s="98">
+      <c r="T10">
         <v>0</v>
       </c>
       <c r="U10">
@@ -5028,7 +5023,7 @@
       <c r="S11">
         <v>0</v>
       </c>
-      <c r="T11" s="98">
+      <c r="T11">
         <v>0</v>
       </c>
       <c r="U11">
@@ -5093,7 +5088,7 @@
       <c r="S12">
         <v>0</v>
       </c>
-      <c r="T12" s="98">
+      <c r="T12">
         <v>0</v>
       </c>
       <c r="U12">
@@ -5158,7 +5153,7 @@
       <c r="S13">
         <v>0</v>
       </c>
-      <c r="T13" s="98">
+      <c r="T13">
         <v>0</v>
       </c>
       <c r="U13">
@@ -5359,7 +5354,7 @@
       <c r="S16">
         <v>0</v>
       </c>
-      <c r="T16" s="98">
+      <c r="T16">
         <v>0</v>
       </c>
       <c r="U16">
@@ -5424,7 +5419,7 @@
       <c r="S17">
         <v>0</v>
       </c>
-      <c r="T17" s="98">
+      <c r="T17">
         <v>0</v>
       </c>
       <c r="U17">
@@ -5531,7 +5526,7 @@
       <c r="L19" t="s">
         <v>74</v>
       </c>
-      <c r="M19" s="74" t="s">
+      <c r="M19" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N19" s="14">
@@ -5552,7 +5547,7 @@
       <c r="S19">
         <v>0</v>
       </c>
-      <c r="T19" s="98">
+      <c r="T19">
         <v>0</v>
       </c>
       <c r="U19">
@@ -5596,7 +5591,7 @@
       <c r="L20" t="s">
         <v>74</v>
       </c>
-      <c r="M20" s="74" t="s">
+      <c r="M20" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N20" s="14">
@@ -5617,7 +5612,7 @@
       <c r="S20">
         <v>0</v>
       </c>
-      <c r="T20" s="98">
+      <c r="T20">
         <v>0</v>
       </c>
       <c r="U20">
@@ -5664,7 +5659,7 @@
       <c r="L21" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="M21" s="75" t="s">
+      <c r="M21" s="16" t="s">
         <v>10</v>
       </c>
       <c r="N21" s="16">
@@ -5730,7 +5725,7 @@
       <c r="L22" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="M22" s="76" t="s">
+      <c r="M22" s="42" t="s">
         <v>108</v>
       </c>
       <c r="N22" s="10">
@@ -5798,7 +5793,7 @@
       <c r="L23" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="M23" s="74" t="s">
+      <c r="M23" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N23">
@@ -5819,7 +5814,7 @@
       <c r="S23">
         <v>0</v>
       </c>
-      <c r="T23" s="98">
+      <c r="T23">
         <v>0</v>
       </c>
       <c r="U23">
@@ -5860,7 +5855,7 @@
       <c r="L24" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="M24" s="74" t="s">
+      <c r="M24" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N24">
@@ -5881,7 +5876,7 @@
       <c r="S24">
         <v>0</v>
       </c>
-      <c r="T24" s="98">
+      <c r="T24">
         <v>0</v>
       </c>
       <c r="U24">
@@ -5925,7 +5920,7 @@
       <c r="L25" t="s">
         <v>75</v>
       </c>
-      <c r="M25" s="74" t="s">
+      <c r="M25" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N25">
@@ -5946,7 +5941,7 @@
       <c r="S25">
         <v>0</v>
       </c>
-      <c r="T25" s="98">
+      <c r="T25">
         <v>0</v>
       </c>
       <c r="U25">
@@ -5987,7 +5982,7 @@
       <c r="L26" t="s">
         <v>75</v>
       </c>
-      <c r="M26" s="74" t="s">
+      <c r="M26" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N26">
@@ -6008,7 +6003,7 @@
       <c r="S26">
         <v>0</v>
       </c>
-      <c r="T26" s="98">
+      <c r="T26">
         <v>0</v>
       </c>
       <c r="U26">
@@ -6049,7 +6044,7 @@
       <c r="L27" t="s">
         <v>75</v>
       </c>
-      <c r="M27" s="74" t="s">
+      <c r="M27" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N27">
@@ -6070,7 +6065,7 @@
       <c r="S27">
         <v>0</v>
       </c>
-      <c r="T27" s="98">
+      <c r="T27">
         <v>0</v>
       </c>
       <c r="U27">
@@ -6114,7 +6109,7 @@
       <c r="L28" t="s">
         <v>75</v>
       </c>
-      <c r="M28" s="74" t="s">
+      <c r="M28" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N28">
@@ -6135,7 +6130,7 @@
       <c r="S28">
         <v>0</v>
       </c>
-      <c r="T28" s="98">
+      <c r="T28">
         <v>0</v>
       </c>
       <c r="U28">
@@ -6176,7 +6171,7 @@
       <c r="L29" t="s">
         <v>75</v>
       </c>
-      <c r="M29" s="74" t="s">
+      <c r="M29" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N29">
@@ -6197,7 +6192,7 @@
       <c r="S29">
         <v>0</v>
       </c>
-      <c r="T29" s="98">
+      <c r="T29">
         <v>0</v>
       </c>
       <c r="U29">
@@ -6238,7 +6233,7 @@
       <c r="L30" t="s">
         <v>75</v>
       </c>
-      <c r="M30" s="74" t="s">
+      <c r="M30" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N30">
@@ -6259,7 +6254,7 @@
       <c r="S30">
         <v>0</v>
       </c>
-      <c r="T30" s="98">
+      <c r="T30">
         <v>0</v>
       </c>
       <c r="U30">
@@ -6304,7 +6299,7 @@
       <c r="L31" t="s">
         <v>75</v>
       </c>
-      <c r="M31" s="74" t="s">
+      <c r="M31" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N31">
@@ -6325,7 +6320,7 @@
       <c r="S31">
         <v>0</v>
       </c>
-      <c r="T31" s="98">
+      <c r="T31">
         <v>0</v>
       </c>
       <c r="U31">
@@ -6370,7 +6365,7 @@
       <c r="L32" t="s">
         <v>75</v>
       </c>
-      <c r="M32" s="74" t="s">
+      <c r="M32" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N32">
@@ -6391,7 +6386,7 @@
       <c r="S32">
         <v>6360</v>
       </c>
-      <c r="T32" s="98">
+      <c r="T32">
         <v>0</v>
       </c>
       <c r="U32">
@@ -6432,7 +6427,7 @@
       <c r="L33" t="s">
         <v>75</v>
       </c>
-      <c r="M33" s="74" t="s">
+      <c r="M33" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N33">
@@ -6447,13 +6442,13 @@
       <c r="Q33">
         <v>0</v>
       </c>
-      <c r="R33" s="74">
+      <c r="R33" s="14">
         <v>0</v>
       </c>
       <c r="S33">
         <v>1718</v>
       </c>
-      <c r="T33" s="98">
+      <c r="T33">
         <v>0</v>
       </c>
       <c r="U33">
@@ -6471,7 +6466,7 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="35"/>
-      <c r="M34" s="77" t="s">
+      <c r="M34" s="43" t="s">
         <v>71</v>
       </c>
       <c r="N34" s="27" t="s">
@@ -6505,24 +6500,24 @@
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.3">
       <c r="N35" s="14">
-        <f t="shared" ref="N35:S35" si="0">SUM(N3:N32)</f>
-        <v>65990</v>
+        <f>SUM(N3:N33)</f>
+        <v>67064</v>
       </c>
       <c r="O35" s="14">
-        <f t="shared" si="0"/>
-        <v>23035</v>
+        <f t="shared" ref="N35:S35" si="0">SUM(O3:O32)</f>
+        <v>21828</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="0"/>
-        <v>9257</v>
+        <v>9101</v>
       </c>
       <c r="Q35" s="14">
         <f t="shared" si="0"/>
-        <v>127353</v>
+        <v>127946</v>
       </c>
       <c r="R35" s="14">
         <f t="shared" si="0"/>
-        <v>27977</v>
+        <v>27972</v>
       </c>
       <c r="S35" s="14">
         <f t="shared" si="0"/>
@@ -6530,7 +6525,7 @@
       </c>
       <c r="T35" s="14">
         <f>SUM(U3:U21)</f>
-        <v>12936</v>
+        <v>12451</v>
       </c>
       <c r="U35" s="14">
         <f>SUM(T3:T21)</f>
@@ -6539,7 +6534,7 @@
       <c r="V35" s="14"/>
       <c r="W35" s="14">
         <f>SUM(V3:V21)</f>
-        <v>1970</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.3">
@@ -6551,6 +6546,10 @@
       </c>
       <c r="D39" t="s">
         <v>151</v>
+      </c>
+      <c r="N39">
+        <f>N35+O35+P35+Q35</f>
+        <v>225939</v>
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.3">
@@ -6664,8 +6663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114EE0BB-9430-4707-8294-22F3EA198BF4}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6689,7 +6688,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" s="78" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" s="71" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -6721,32 +6720,32 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="str">
+    <row r="3" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="71" t="str">
         <f>NoMalahat!A3</f>
         <v>Orca Sound</v>
       </c>
-      <c r="B3" s="78" t="str">
+      <c r="B3" s="71" t="str">
         <f>NoMalahat!B3</f>
         <v>Orcasound Lab</v>
       </c>
-      <c r="C3" s="78" t="str">
+      <c r="C3" s="71" t="str">
         <f>NoMalahat!C3</f>
         <v xml:space="preserve">orcasound_lab      </v>
       </c>
-      <c r="D3" s="79">
+      <c r="D3" s="72">
         <f>NoMalahat!D3</f>
         <v>48.5248469</v>
       </c>
-      <c r="E3" s="79">
+      <c r="E3" s="72">
         <f>NoMalahat!E3</f>
         <v>-123.15916470000001</v>
       </c>
-      <c r="F3" s="78">
+      <c r="F3" s="71">
         <f>NoMalahat!F3</f>
         <v>8</v>
       </c>
-      <c r="G3" s="78">
+      <c r="G3" s="71">
         <f>NoMalahat!G3</f>
         <v>32</v>
       </c>
@@ -6763,28 +6762,28 @@
         <v>44081</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="78" t="str">
+    <row r="4" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="71" t="str">
         <f>NoMalahat!B4</f>
         <v>Bush Point</v>
       </c>
-      <c r="C4" s="78" t="str">
+      <c r="C4" s="71" t="str">
         <f>NoMalahat!C4</f>
         <v xml:space="preserve">bush_point       </v>
       </c>
-      <c r="D4" s="79">
+      <c r="D4" s="72">
         <f>NoMalahat!D4</f>
         <v>48.0310074</v>
       </c>
-      <c r="E4" s="79">
+      <c r="E4" s="72">
         <f>NoMalahat!E4</f>
         <v>-122.6082001</v>
       </c>
-      <c r="F4" s="78">
+      <c r="F4" s="71">
         <f>NoMalahat!F4</f>
         <v>12.5</v>
       </c>
-      <c r="G4" s="78">
+      <c r="G4" s="71">
         <f>NoMalahat!G4</f>
         <v>32</v>
       </c>
@@ -6801,28 +6800,28 @@
         <v>44123</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="78" t="str">
+    <row r="5" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="71" t="str">
         <f>NoMalahat!B5</f>
         <v>Port Townsand</v>
       </c>
-      <c r="C5" s="78" t="str">
+      <c r="C5" s="71" t="str">
         <f>NoMalahat!C5</f>
         <v xml:space="preserve">port_townsend       </v>
       </c>
-      <c r="D5" s="79">
+      <c r="D5" s="72">
         <f>NoMalahat!D5</f>
         <v>48.135399999999997</v>
       </c>
-      <c r="E5" s="79">
+      <c r="E5" s="72">
         <f>NoMalahat!E5</f>
         <v>-122.76</v>
       </c>
-      <c r="F5" s="78">
+      <c r="F5" s="71">
         <f>NoMalahat!F5</f>
         <v>8</v>
       </c>
-      <c r="G5" s="78">
+      <c r="G5" s="71">
         <f>NoMalahat!G5</f>
         <v>32</v>
       </c>
@@ -6839,32 +6838,32 @@
         <v>44112</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="80" t="str">
+    <row r="6" spans="1:10" s="71" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="73" t="str">
         <f>NoMalahat!A6</f>
         <v>ONC</v>
       </c>
-      <c r="B6" s="80" t="str">
+      <c r="B6" s="73" t="str">
         <f>NoMalahat!B6</f>
         <v>Berkley Canyon</v>
       </c>
-      <c r="C6" s="80" t="str">
+      <c r="C6" s="73" t="str">
         <f>NoMalahat!C6</f>
         <v>Berkley Canyon</v>
       </c>
-      <c r="D6" s="81">
+      <c r="D6" s="74">
         <f>NoMalahat!D6</f>
         <v>48.426000000000002</v>
       </c>
-      <c r="E6" s="81">
+      <c r="E6" s="74">
         <f>NoMalahat!E6</f>
         <v>-126.17400000000001</v>
       </c>
-      <c r="F6" s="80">
+      <c r="F6" s="73">
         <f>NoMalahat!F6</f>
         <v>40</v>
       </c>
-      <c r="G6" s="80">
+      <c r="G6" s="73">
         <f>NoMalahat!G6</f>
         <v>64</v>
       </c>
@@ -6876,37 +6875,37 @@
         <f>NoMalahat!I6</f>
         <v>41414</v>
       </c>
-      <c r="J6" s="82">
+      <c r="J6" s="26">
         <f>NoMalahat!J6</f>
         <v>41977</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83" t="str">
+    <row r="7" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="76" t="str">
         <f>NoMalahat!A7</f>
         <v>DFO CRP</v>
       </c>
-      <c r="B7" s="83" t="str">
+      <c r="B7" s="76" t="str">
         <f>NoMalahat!B7</f>
         <v>West Vancouver Island</v>
       </c>
-      <c r="C7" s="83" t="str">
+      <c r="C7" s="76" t="str">
         <f>NoMalahat!C7</f>
         <v xml:space="preserve">WVanIsl      </v>
       </c>
-      <c r="D7" s="84" t="str">
+      <c r="D7" s="77" t="str">
         <f>NoMalahat!D7</f>
         <v>NA</v>
       </c>
-      <c r="E7" s="84" t="str">
+      <c r="E7" s="77" t="str">
         <f>NoMalahat!E7</f>
         <v>NA</v>
       </c>
-      <c r="F7" s="83">
+      <c r="F7" s="76">
         <f>NoMalahat!F7</f>
         <v>114</v>
       </c>
-      <c r="G7" s="83">
+      <c r="G7" s="76">
         <f>NoMalahat!G7</f>
         <v>16.384</v>
       </c>
@@ -6918,34 +6917,34 @@
         <f>NoMalahat!I7</f>
         <v>40681</v>
       </c>
-      <c r="J7" s="85">
+      <c r="J7" s="12">
         <f>NoMalahat!J7</f>
         <v>41053</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="86"/>
-      <c r="B8" s="86" t="str">
+    <row r="8" spans="1:10" s="71" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="79"/>
+      <c r="B8" s="79" t="str">
         <f>NoMalahat!B8</f>
         <v>Northern Mainland British Colombia</v>
       </c>
-      <c r="C8" s="86" t="str">
+      <c r="C8" s="79" t="str">
         <f>NoMalahat!C8</f>
         <v>NorthBc</v>
       </c>
-      <c r="D8" s="87" t="str">
+      <c r="D8" s="80" t="str">
         <f>NoMalahat!D8</f>
         <v>NA</v>
       </c>
-      <c r="E8" s="87" t="str">
+      <c r="E8" s="80" t="str">
         <f>NoMalahat!E8</f>
         <v>NA</v>
       </c>
-      <c r="F8" s="86">
+      <c r="F8" s="79">
         <f>NoMalahat!F8</f>
         <v>35</v>
       </c>
-      <c r="G8" s="86">
+      <c r="G8" s="79">
         <f>NoMalahat!G8</f>
         <v>16</v>
       </c>
@@ -6957,37 +6956,37 @@
         <f>NoMalahat!I8</f>
         <v>41557</v>
       </c>
-      <c r="J8" s="88">
+      <c r="J8" s="13">
         <f>NoMalahat!J8</f>
         <v>41673</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="83" t="str">
+    <row r="9" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="76" t="str">
         <f>NoMalahat!A9</f>
         <v>DFO WDLP</v>
       </c>
-      <c r="B9" s="83" t="str">
+      <c r="B9" s="76" t="str">
         <f>NoMalahat!B9</f>
         <v xml:space="preserve">Carmanah Point           </v>
       </c>
-      <c r="C9" s="83" t="str">
+      <c r="C9" s="76" t="str">
         <f>NoMalahat!C9</f>
         <v xml:space="preserve">CarmanahPt           </v>
       </c>
-      <c r="D9" s="84" t="str">
+      <c r="D9" s="77" t="str">
         <f>NoMalahat!D9</f>
         <v>NA</v>
       </c>
-      <c r="E9" s="84" t="str">
+      <c r="E9" s="77" t="str">
         <f>NoMalahat!E9</f>
         <v>NA</v>
       </c>
-      <c r="F9" s="83">
+      <c r="F9" s="76">
         <f>NoMalahat!F9</f>
         <v>55</v>
       </c>
-      <c r="G9" s="83">
+      <c r="G9" s="76">
         <f>NoMalahat!G9</f>
         <v>192</v>
       </c>
@@ -7004,28 +7003,28 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="78" t="str">
+    <row r="10" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="71" t="str">
         <f>NoMalahat!B10</f>
         <v>Strait of Georgia North 1*</v>
       </c>
-      <c r="C10" s="78" t="str">
+      <c r="C10" s="71" t="str">
         <f>NoMalahat!C10</f>
         <v>StrGeoN1</v>
       </c>
-      <c r="D10" s="79" t="str">
+      <c r="D10" s="72" t="str">
         <f>NoMalahat!D10</f>
         <v>NA</v>
       </c>
-      <c r="E10" s="79" t="str">
+      <c r="E10" s="72" t="str">
         <f>NoMalahat!E10</f>
         <v>NA</v>
       </c>
-      <c r="F10" s="78">
+      <c r="F10" s="71">
         <f>NoMalahat!F10</f>
         <v>72</v>
       </c>
-      <c r="G10" s="78">
+      <c r="G10" s="71">
         <f>NoMalahat!G10</f>
         <v>256</v>
       </c>
@@ -7042,28 +7041,28 @@
         <v>44470</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="78" t="str">
+    <row r="11" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="71" t="str">
         <f>NoMalahat!B11</f>
         <v>Strait of Georgia North 2*</v>
       </c>
-      <c r="C11" s="78" t="str">
+      <c r="C11" s="71" t="str">
         <f>NoMalahat!C11</f>
         <v>StrGeoN1</v>
       </c>
-      <c r="D11" s="79" t="str">
+      <c r="D11" s="72" t="str">
         <f>NoMalahat!D11</f>
         <v>NA</v>
       </c>
-      <c r="E11" s="79" t="str">
+      <c r="E11" s="72" t="str">
         <f>NoMalahat!E11</f>
         <v>NA</v>
       </c>
-      <c r="F11" s="78">
+      <c r="F11" s="71">
         <f>NoMalahat!F11</f>
         <v>72</v>
       </c>
-      <c r="G11" s="78">
+      <c r="G11" s="71">
         <f>NoMalahat!G11</f>
         <v>256</v>
       </c>
@@ -7080,28 +7079,28 @@
         <v>44528</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="78" t="str">
+    <row r="12" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="71" t="str">
         <f>NoMalahat!B12</f>
         <v>Strait of Georgia South 1*</v>
       </c>
-      <c r="C12" s="78" t="str">
+      <c r="C12" s="71" t="str">
         <f>NoMalahat!C12</f>
         <v>StrGeoS1</v>
       </c>
-      <c r="D12" s="79" t="str">
+      <c r="D12" s="72" t="str">
         <f>NoMalahat!D12</f>
         <v>NA</v>
       </c>
-      <c r="E12" s="79" t="str">
+      <c r="E12" s="72" t="str">
         <f>NoMalahat!E12</f>
         <v>NA</v>
       </c>
-      <c r="F12" s="78">
+      <c r="F12" s="71">
         <f>NoMalahat!F12</f>
         <v>193</v>
       </c>
-      <c r="G12" s="78">
+      <c r="G12" s="71">
         <f>NoMalahat!G12</f>
         <v>256</v>
       </c>
@@ -7118,28 +7117,28 @@
         <v>44518</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="78" t="str">
+    <row r="13" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="71" t="str">
         <f>NoMalahat!B13</f>
         <v>Strait of Georgia South 2*</v>
       </c>
-      <c r="C13" s="78" t="str">
+      <c r="C13" s="71" t="str">
         <f>NoMalahat!C13</f>
         <v>StrGeosS2</v>
       </c>
-      <c r="D13" s="79" t="str">
+      <c r="D13" s="72" t="str">
         <f>NoMalahat!D13</f>
         <v>NA</v>
       </c>
-      <c r="E13" s="79" t="str">
+      <c r="E13" s="72" t="str">
         <f>NoMalahat!E13</f>
         <v>NA</v>
       </c>
-      <c r="F13" s="78">
+      <c r="F13" s="71">
         <f>NoMalahat!F13</f>
         <v>193</v>
       </c>
-      <c r="G13" s="78">
+      <c r="G13" s="71">
         <f>NoMalahat!G13</f>
         <v>256</v>
       </c>
@@ -7156,29 +7155,29 @@
         <v>44455</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86" t="str">
+    <row r="14" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="79"/>
+      <c r="B14" s="79" t="str">
         <f>NoMalahat!B14</f>
         <v>Swansen Channel*</v>
       </c>
-      <c r="C14" s="86" t="str">
+      <c r="C14" s="79" t="str">
         <f>NoMalahat!C14</f>
         <v>SwanChan</v>
       </c>
-      <c r="D14" s="87" t="str">
+      <c r="D14" s="80" t="str">
         <f>NoMalahat!D14</f>
         <v>NA</v>
       </c>
-      <c r="E14" s="87" t="str">
+      <c r="E14" s="80" t="str">
         <f>NoMalahat!E14</f>
         <v>NA</v>
       </c>
-      <c r="F14" s="86">
+      <c r="F14" s="79">
         <f>NoMalahat!F14</f>
         <v>245</v>
       </c>
-      <c r="G14" s="86">
+      <c r="G14" s="79">
         <f>NoMalahat!G14</f>
         <v>256</v>
       </c>
@@ -7195,32 +7194,32 @@
         <v>44570</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="78" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80" t="str">
+    <row r="15" spans="1:10" s="71" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="73" t="str">
         <f>NoMalahat!A15</f>
         <v>SIMRES</v>
       </c>
-      <c r="B15" s="80" t="str">
+      <c r="B15" s="73" t="str">
         <f>NoMalahat!B15</f>
         <v>Tekteksen (East Point), Saturna Island, BC</v>
       </c>
-      <c r="C15" s="80" t="str">
+      <c r="C15" s="73" t="str">
         <f>NoMalahat!C15</f>
         <v>Tekteksen</v>
       </c>
-      <c r="D15" s="81">
+      <c r="D15" s="74">
         <f>NoMalahat!D15</f>
         <v>48.78</v>
       </c>
-      <c r="E15" s="81">
+      <c r="E15" s="74">
         <f>NoMalahat!E15</f>
         <v>-123.05200000000001</v>
       </c>
-      <c r="F15" s="80">
+      <c r="F15" s="73">
         <f>NoMalahat!F15</f>
         <v>27</v>
       </c>
-      <c r="G15" s="80">
+      <c r="G15" s="73">
         <f>NoMalahat!G15</f>
         <v>128</v>
       </c>
@@ -7232,37 +7231,37 @@
         <f>NoMalahat!I15</f>
         <v>44736</v>
       </c>
-      <c r="J15" s="82">
+      <c r="J15" s="75">
         <f>NoMalahat!J15</f>
         <v>44736</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="78" t="str">
+    <row r="16" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="71" t="str">
         <f>NoMalahat!A16</f>
         <v>SIO</v>
       </c>
-      <c r="B16" s="78" t="str">
+      <c r="B16" s="71" t="str">
         <f>NoMalahat!B16</f>
         <v>Cape Elizabeth</v>
       </c>
-      <c r="C16" s="78" t="str">
+      <c r="C16" s="71" t="str">
         <f>NoMalahat!C16</f>
         <v>CE_01</v>
       </c>
-      <c r="D16" s="79">
+      <c r="D16" s="72">
         <f>NoMalahat!D16</f>
         <v>47.357999999999997</v>
       </c>
-      <c r="E16" s="79">
+      <c r="E16" s="72">
         <f>NoMalahat!E16</f>
         <v>-124.683333333333</v>
       </c>
-      <c r="F16" s="78">
+      <c r="F16" s="71">
         <f>NoMalahat!F16</f>
         <v>100</v>
       </c>
-      <c r="G16" s="78">
+      <c r="G16" s="71">
         <f>NoMalahat!G16</f>
         <v>200</v>
       </c>
@@ -7270,37 +7269,37 @@
         <f>NoMalahat!H16</f>
         <v>HARP</v>
       </c>
-      <c r="I16" s="89">
+      <c r="I16" s="82">
         <f>NoMalahat!I16</f>
         <v>39616</v>
       </c>
-      <c r="J16" s="89">
+      <c r="J16" s="82">
         <f>NoMalahat!J16</f>
         <v>40925</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="78" t="str">
+    <row r="17" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="71" t="str">
         <f>NoMalahat!B17</f>
         <v>Quinault Canyon</v>
       </c>
-      <c r="C17" s="78" t="str">
+      <c r="C17" s="71" t="str">
         <f>NoMalahat!C17</f>
         <v>Cpe_Elz</v>
       </c>
-      <c r="D17" s="79">
+      <c r="D17" s="72">
         <f>NoMalahat!D17</f>
         <v>47.5</v>
       </c>
-      <c r="E17" s="79">
+      <c r="E17" s="72">
         <f>NoMalahat!E17</f>
         <v>-125.353333333333</v>
       </c>
-      <c r="F17" s="78">
+      <c r="F17" s="71">
         <f>NoMalahat!F17</f>
         <v>1400</v>
       </c>
-      <c r="G17" s="78">
+      <c r="G17" s="71">
         <f>NoMalahat!G17</f>
         <v>200</v>
       </c>
@@ -7308,41 +7307,41 @@
         <f>NoMalahat!H17</f>
         <v>HARP</v>
       </c>
-      <c r="I17" s="89">
+      <c r="I17" s="82">
         <f>NoMalahat!I17</f>
         <v>40570</v>
       </c>
-      <c r="J17" s="89">
+      <c r="J17" s="82">
         <f>NoMalahat!J17</f>
         <v>41455</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="83" t="str">
+    <row r="18" spans="1:10" s="71" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="76" t="str">
         <f>NoMalahat!A18</f>
         <v>JASCO/VPFA</v>
       </c>
-      <c r="B18" s="83" t="str">
+      <c r="B18" s="76" t="str">
         <f>NoMalahat!B18</f>
         <v>Haro Strait Northbound</v>
       </c>
-      <c r="C18" s="83" t="str">
+      <c r="C18" s="76" t="str">
         <f>NoMalahat!C18</f>
         <v>HaroStraitNorth</v>
       </c>
-      <c r="D18" s="90">
+      <c r="D18" s="83">
         <f>NoMalahat!D18</f>
         <v>48.518050000000002</v>
       </c>
-      <c r="E18" s="90">
+      <c r="E18" s="83">
         <f>NoMalahat!E18</f>
         <v>-123.19166666666599</v>
       </c>
-      <c r="F18" s="83">
+      <c r="F18" s="76">
         <f>NoMalahat!F18</f>
         <v>251</v>
       </c>
-      <c r="G18" s="83">
+      <c r="G18" s="76">
         <f>NoMalahat!G18</f>
         <v>0</v>
       </c>
@@ -7350,37 +7349,37 @@
         <f>NoMalahat!H18</f>
         <v>AMAR</v>
       </c>
-      <c r="I18" s="85">
+      <c r="I18" s="78">
         <f>NoMalahat!I18</f>
         <v>42924</v>
       </c>
-      <c r="J18" s="85">
+      <c r="J18" s="78">
         <f>NoMalahat!J18</f>
         <v>43032</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="78" t="str">
+    <row r="19" spans="1:10" s="71" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="71" t="str">
         <f>NoMalahat!B19</f>
         <v>Haro Strait Southbound</v>
       </c>
-      <c r="C19" s="78" t="str">
+      <c r="C19" s="71" t="str">
         <f>NoMalahat!C19</f>
         <v>HaroStraitSouth</v>
       </c>
-      <c r="D19" s="91">
+      <c r="D19" s="84">
         <f>NoMalahat!D19</f>
         <v>48.5167</v>
       </c>
-      <c r="E19" s="91">
+      <c r="E19" s="84">
         <f>NoMalahat!E19</f>
         <v>-123.207616666666</v>
       </c>
-      <c r="F19" s="78">
+      <c r="F19" s="71">
         <f>NoMalahat!F19</f>
         <v>210</v>
       </c>
-      <c r="G19" s="78">
+      <c r="G19" s="71">
         <f>NoMalahat!G19</f>
         <v>0</v>
       </c>
@@ -7388,37 +7387,37 @@
         <f>NoMalahat!H19</f>
         <v>AMAR</v>
       </c>
-      <c r="I19" s="92">
+      <c r="I19" s="85">
         <f>NoMalahat!I19</f>
         <v>42924</v>
       </c>
-      <c r="J19" s="92">
+      <c r="J19" s="85">
         <f>NoMalahat!J19</f>
         <v>43032</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="78" t="str">
+    <row r="20" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="71" t="str">
         <f>NoMalahat!B20</f>
         <v>Boundary Pass</v>
       </c>
-      <c r="C20" s="78" t="str">
+      <c r="C20" s="71" t="str">
         <f>NoMalahat!C20</f>
         <v>BoundaryPass</v>
       </c>
-      <c r="D20" s="91">
+      <c r="D20" s="84">
         <f>NoMalahat!D20</f>
         <v>48.760779999999997</v>
       </c>
-      <c r="E20" s="91">
+      <c r="E20" s="84">
         <f>NoMalahat!E20</f>
         <v>-123.06793999999999</v>
       </c>
-      <c r="F20" s="78">
+      <c r="F20" s="71">
         <f>NoMalahat!F20</f>
         <v>193</v>
       </c>
-      <c r="G20" s="78">
+      <c r="G20" s="71">
         <f>NoMalahat!G20</f>
         <v>128</v>
       </c>
@@ -7426,41 +7425,41 @@
         <f>NoMalahat!H20</f>
         <v>AMAR 418</v>
       </c>
-      <c r="I20" s="92">
+      <c r="I20" s="85">
         <f>NoMalahat!I20</f>
         <v>43345</v>
       </c>
-      <c r="J20" s="92">
+      <c r="J20" s="85">
         <f>NoMalahat!J20</f>
         <v>43557</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="78" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="78" t="str">
+    <row r="21" spans="1:10" s="71" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="71" t="str">
         <f>NoMalahat!A21</f>
         <v>JASCO/VPFA/ONC</v>
       </c>
-      <c r="B21" s="78" t="str">
+      <c r="B21" s="71" t="str">
         <f>NoMalahat!B21</f>
         <v>Roberts Bank/Strait of Georgia East</v>
       </c>
-      <c r="C21" s="86" t="str">
+      <c r="C21" s="79" t="str">
         <f>NoMalahat!C21</f>
         <v>StraitofGeorgia</v>
       </c>
-      <c r="D21" s="87">
+      <c r="D21" s="80">
         <f>NoMalahat!D21</f>
         <v>49.042645</v>
       </c>
-      <c r="E21" s="87">
+      <c r="E21" s="80">
         <f>NoMalahat!E21</f>
         <v>-123.31744</v>
       </c>
-      <c r="F21" s="86">
+      <c r="F21" s="79">
         <f>NoMalahat!F21</f>
         <v>168</v>
       </c>
-      <c r="G21" s="86">
+      <c r="G21" s="79">
         <f>NoMalahat!G21</f>
         <v>64</v>
       </c>
@@ -7468,406 +7467,406 @@
         <f>NoMalahat!H21</f>
         <v>GeoSpectrum M8</v>
       </c>
-      <c r="I21" s="88">
+      <c r="I21" s="81">
         <f>NoMalahat!I21</f>
         <v>42270</v>
       </c>
-      <c r="J21" s="88">
+      <c r="J21" s="81">
         <f>NoMalahat!J21</f>
         <v>43189</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="80" t="str">
+    <row r="22" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="73" t="str">
         <f>NoMalahat!A22</f>
         <v>SMRU</v>
       </c>
-      <c r="B22" s="80" t="str">
+      <c r="B22" s="73" t="str">
         <f>NoMalahat!B22</f>
         <v>Lime Kiln</v>
       </c>
-      <c r="C22" s="80" t="str">
+      <c r="C22" s="73" t="str">
         <f>NoMalahat!C22</f>
         <v>LmKln</v>
       </c>
-      <c r="D22" s="93">
+      <c r="D22" s="86">
         <f>NoMalahat!D22</f>
         <v>48.51</v>
       </c>
-      <c r="E22" s="93">
+      <c r="E22" s="86">
         <f>NoMalahat!E22</f>
         <v>-123.15</v>
       </c>
-      <c r="F22" s="80">
+      <c r="F22" s="73">
         <f>NoMalahat!F22</f>
         <v>23</v>
       </c>
-      <c r="G22" s="80">
+      <c r="G22" s="73">
         <f>NoMalahat!G22</f>
         <v>150</v>
       </c>
       <c r="H22" t="s">
         <v>174</v>
       </c>
-      <c r="I22" s="94">
+      <c r="I22" s="87">
         <f>NoMalahat!I22</f>
         <v>42680</v>
       </c>
-      <c r="J22" s="94">
+      <c r="J22" s="87">
         <f>NoMalahat!J22</f>
         <v>44087</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="78" t="str">
+    <row r="23" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="71" t="str">
         <f>NoMalahat!A23</f>
         <v>UAF</v>
       </c>
-      <c r="B23" s="78" t="str">
+      <c r="B23" s="71" t="str">
         <f>NoMalahat!B23</f>
         <v>Hinchinbroook Entrance</v>
       </c>
-      <c r="C23" s="78" t="str">
+      <c r="C23" s="71" t="str">
         <f>NoMalahat!C23</f>
         <v xml:space="preserve">HE_67391498    </v>
       </c>
-      <c r="D23" s="91">
+      <c r="D23" s="84">
         <f>NoMalahat!D23</f>
         <v>60.307499999999997</v>
       </c>
-      <c r="E23" s="91">
+      <c r="E23" s="84">
         <f>NoMalahat!E23</f>
         <v>-146.97300000000001</v>
       </c>
-      <c r="F23" s="78">
+      <c r="F23" s="71">
         <f>NoMalahat!F23</f>
         <v>42</v>
       </c>
-      <c r="G23" s="95">
+      <c r="G23" s="88">
         <f>NoMalahat!G23</f>
         <v>24</v>
       </c>
-      <c r="H23" s="95" t="str">
+      <c r="H23" s="88" t="str">
         <f>NoMalahat!H23</f>
         <v>ST300-67391498</v>
       </c>
-      <c r="I23" s="96">
+      <c r="I23" s="89">
         <f>NoMalahat!I23</f>
         <v>43648</v>
       </c>
-      <c r="J23" s="96">
+      <c r="J23" s="89">
         <f>NoMalahat!J23</f>
         <v>43662</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="78" t="str">
+    <row r="24" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="71" t="str">
         <f>NoMalahat!B25</f>
         <v>Kachemak Bay</v>
       </c>
-      <c r="C24" s="78" t="str">
+      <c r="C24" s="71" t="str">
         <f>NoMalahat!C25</f>
         <v xml:space="preserve">KB_5354    </v>
       </c>
-      <c r="D24" s="91">
+      <c r="D24" s="84">
         <f>NoMalahat!D25</f>
         <v>59.876666666666665</v>
       </c>
-      <c r="E24" s="91">
+      <c r="E24" s="84">
         <f>NoMalahat!E25</f>
         <v>-151.8485</v>
       </c>
-      <c r="F24" s="78">
+      <c r="F24" s="71">
         <f>NoMalahat!F25</f>
         <v>21</v>
       </c>
-      <c r="G24" s="95">
+      <c r="G24" s="88">
         <f>NoMalahat!G25</f>
         <v>24</v>
       </c>
-      <c r="H24" s="95" t="str">
+      <c r="H24" s="88" t="str">
         <f>NoMalahat!H25</f>
         <v>ST300-5354</v>
       </c>
-      <c r="I24" s="96">
+      <c r="I24" s="89">
         <f>NoMalahat!I25</f>
         <v>44406</v>
       </c>
-      <c r="J24" s="96">
+      <c r="J24" s="89">
         <f>NoMalahat!J25</f>
         <v>44415</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="78" t="str">
+    <row r="25" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="71" t="str">
         <f>NoMalahat!C26</f>
         <v xml:space="preserve">KB_67424266        </v>
       </c>
-      <c r="D25" s="91">
+      <c r="D25" s="84">
         <f>NoMalahat!D26</f>
         <v>59.876666666666665</v>
       </c>
-      <c r="E25" s="91">
+      <c r="E25" s="84">
         <f>NoMalahat!E26</f>
         <v>-151.8485</v>
       </c>
-      <c r="F25" s="78">
+      <c r="F25" s="71">
         <f>NoMalahat!F26</f>
         <v>21</v>
       </c>
-      <c r="G25" s="95">
+      <c r="G25" s="88">
         <f>NoMalahat!G26</f>
         <v>24</v>
       </c>
-      <c r="H25" s="95" t="str">
+      <c r="H25" s="88" t="str">
         <f>NoMalahat!H26</f>
         <v>ST300-67424266</v>
       </c>
-      <c r="I25" s="96">
+      <c r="I25" s="89">
         <f>NoMalahat!I26</f>
         <v>44056</v>
       </c>
-      <c r="J25" s="96">
+      <c r="J25" s="89">
         <f>NoMalahat!J26</f>
         <v>44284</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="78" t="str">
+    <row r="26" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="71" t="str">
         <f>NoMalahat!C27</f>
         <v xml:space="preserve">KB_67383303    </v>
       </c>
-      <c r="D26" s="91">
+      <c r="D26" s="84">
         <f>NoMalahat!D27</f>
         <v>59.876666666666665</v>
       </c>
-      <c r="E26" s="91">
+      <c r="E26" s="84">
         <f>NoMalahat!E27</f>
         <v>-151.8485</v>
       </c>
-      <c r="F26" s="78">
+      <c r="F26" s="71">
         <f>NoMalahat!F27</f>
         <v>21</v>
       </c>
-      <c r="G26" s="95">
+      <c r="G26" s="88">
         <f>NoMalahat!G27</f>
         <v>24</v>
       </c>
-      <c r="H26" s="95" t="str">
+      <c r="H26" s="88" t="str">
         <f>NoMalahat!H27</f>
         <v>ST300-67383303</v>
       </c>
-      <c r="I26" s="96">
+      <c r="I26" s="89">
         <f>NoMalahat!I27</f>
         <v>44694</v>
       </c>
-      <c r="J26" s="96">
+      <c r="J26" s="89">
         <f>NoMalahat!J27</f>
         <v>44694</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="78" t="str">
+    <row r="27" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="71" t="str">
         <f>NoMalahat!B28</f>
         <v>Montague Strait</v>
       </c>
-      <c r="C27" s="78" t="str">
+      <c r="C27" s="71" t="str">
         <f>NoMalahat!C28</f>
         <v xml:space="preserve">MS_5360 </v>
       </c>
-      <c r="D27" s="91">
+      <c r="D27" s="84">
         <f>NoMalahat!D28</f>
         <v>60.175166666666669</v>
       </c>
-      <c r="E27" s="91">
+      <c r="E27" s="84">
         <f>NoMalahat!E28</f>
         <v>-147.818166666667</v>
       </c>
-      <c r="F27" s="78">
+      <c r="F27" s="71">
         <f>NoMalahat!F28</f>
         <v>35</v>
       </c>
-      <c r="G27" s="95">
+      <c r="G27" s="88">
         <f>NoMalahat!G28</f>
         <v>24</v>
       </c>
-      <c r="H27" s="95" t="str">
+      <c r="H27" s="88" t="str">
         <f>NoMalahat!H28</f>
         <v>ST500-5360</v>
       </c>
-      <c r="I27" s="96">
+      <c r="I27" s="89">
         <f>NoMalahat!I28</f>
         <v>44092</v>
       </c>
-      <c r="J27" s="96">
+      <c r="J27" s="89">
         <f>NoMalahat!J28</f>
         <v>44349</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="78" t="str">
+    <row r="28" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="71" t="str">
         <f>NoMalahat!C29</f>
         <v xml:space="preserve">MS_6897   </v>
       </c>
-      <c r="D28" s="91">
+      <c r="D28" s="84">
         <f>NoMalahat!D29</f>
         <v>60.175166666666669</v>
       </c>
-      <c r="E28" s="91">
+      <c r="E28" s="84">
         <f>NoMalahat!E29</f>
         <v>-147.818166666667</v>
       </c>
-      <c r="F28" s="78">
+      <c r="F28" s="71">
         <f>NoMalahat!F29</f>
         <v>35</v>
       </c>
-      <c r="G28" s="95">
+      <c r="G28" s="88">
         <f>NoMalahat!G29</f>
         <v>24</v>
       </c>
-      <c r="H28" s="95" t="str">
+      <c r="H28" s="88" t="str">
         <f>NoMalahat!H29</f>
         <v>ST600-6897</v>
       </c>
-      <c r="I28" s="96">
+      <c r="I28" s="89">
         <f>NoMalahat!I29</f>
         <v>45044</v>
       </c>
-      <c r="J28" s="96">
+      <c r="J28" s="89">
         <f>NoMalahat!J29</f>
         <v>45044</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="78" t="str">
+    <row r="29" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="71" t="str">
         <f>NoMalahat!C30</f>
         <v xml:space="preserve">MS_671879205        </v>
       </c>
-      <c r="D29" s="91">
+      <c r="D29" s="84">
         <f>NoMalahat!D30</f>
         <v>60.175166666666669</v>
       </c>
-      <c r="E29" s="91">
+      <c r="E29" s="84">
         <f>NoMalahat!E30</f>
         <v>-147.818166666667</v>
       </c>
-      <c r="F29" s="78">
+      <c r="F29" s="71">
         <f>NoMalahat!F30</f>
         <v>35</v>
       </c>
-      <c r="G29" s="95">
+      <c r="G29" s="88">
         <f>NoMalahat!G30</f>
         <v>24</v>
       </c>
-      <c r="H29" s="95" t="str">
+      <c r="H29" s="88" t="str">
         <f>NoMalahat!H30</f>
         <v>ST500-671879205</v>
       </c>
-      <c r="I29" s="96">
+      <c r="I29" s="89">
         <f>NoMalahat!I30</f>
         <v>43619</v>
       </c>
-      <c r="J29" s="96">
+      <c r="J29" s="89">
         <f>NoMalahat!J30</f>
         <v>43982</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="91"/>
-      <c r="B30" s="91" t="str">
+    <row r="30" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="84"/>
+      <c r="B30" s="84" t="str">
         <f>NoMalahat!B31</f>
         <v>Resurrection Bay</v>
       </c>
-      <c r="C30" s="91" t="str">
+      <c r="C30" s="84" t="str">
         <f>NoMalahat!C31</f>
         <v xml:space="preserve">RB_67424266 </v>
       </c>
-      <c r="D30" s="91">
+      <c r="D30" s="84">
         <f>NoMalahat!D31</f>
         <v>59.732666666666667</v>
       </c>
-      <c r="E30" s="91">
+      <c r="E30" s="84">
         <f>NoMalahat!E31</f>
         <v>-149.53233333333301</v>
       </c>
-      <c r="F30" s="78">
+      <c r="F30" s="71">
         <f>NoMalahat!F31</f>
         <v>34</v>
       </c>
-      <c r="G30" s="95">
+      <c r="G30" s="88">
         <f>NoMalahat!G31</f>
         <v>24</v>
       </c>
-      <c r="H30" s="95" t="str">
+      <c r="H30" s="88" t="str">
         <f>NoMalahat!H31</f>
         <v>ST300-335826997</v>
       </c>
-      <c r="I30" s="96">
+      <c r="I30" s="89">
         <f>NoMalahat!I31</f>
         <v>43790</v>
       </c>
-      <c r="J30" s="96">
+      <c r="J30" s="89">
         <f>NoMalahat!J31</f>
         <v>43884</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="91"/>
-      <c r="B31" s="91" t="str">
+    <row r="31" spans="1:10" s="71" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="84"/>
+      <c r="B31" s="84" t="str">
         <f>NoMalahat!B32</f>
         <v>Kenai Fjords and Prince William Sound*</v>
       </c>
-      <c r="C31" s="91" t="str">
+      <c r="C31" s="84" t="str">
         <f>NoMalahat!C32</f>
         <v xml:space="preserve">Field_HTI </v>
       </c>
-      <c r="D31" s="91">
+      <c r="D31" s="84">
         <f>NoMalahat!D32</f>
         <v>60.148490000000002</v>
       </c>
-      <c r="E31" s="91">
+      <c r="E31" s="84">
         <f>NoMalahat!E32</f>
         <v>-147.58500000000001</v>
       </c>
-      <c r="F31" s="97" t="str">
+      <c r="F31" s="90" t="str">
         <f>NoMalahat!F32</f>
         <v xml:space="preserve"> 8-10</v>
       </c>
-      <c r="G31" s="95">
+      <c r="G31" s="88">
         <f>NoMalahat!G32</f>
         <v>24</v>
       </c>
-      <c r="H31" s="95" t="str">
+      <c r="H31" s="88" t="str">
         <f>NoMalahat!H32</f>
         <v xml:space="preserve">HTI-96 min  TASCAM DR100  </v>
       </c>
-      <c r="I31" s="96">
+      <c r="I31" s="89">
         <f>NoMalahat!I32</f>
         <v>43605</v>
       </c>
-      <c r="J31" s="96">
+      <c r="J31" s="89">
         <f>NoMalahat!J32</f>
         <v>44362</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="78" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="78" t="str">
+    <row r="32" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="71" t="str">
         <f>NoMalahat!C33</f>
         <v xml:space="preserve">Field_SondTrap             </v>
       </c>
-      <c r="D32" s="91">
+      <c r="D32" s="84">
         <f>NoMalahat!D33</f>
         <v>60.148490000000002</v>
       </c>
-      <c r="E32" s="91">
+      <c r="E32" s="84">
         <f>NoMalahat!E33</f>
         <v>-147.58500000000001</v>
       </c>
-      <c r="F32" s="97" t="str">
+      <c r="F32" s="90" t="str">
         <f>NoMalahat!F33</f>
         <v xml:space="preserve"> 8-10</v>
       </c>
-      <c r="G32" s="95">
+      <c r="G32" s="88">
         <f>NoMalahat!G33</f>
         <v>24</v>
       </c>
@@ -7875,11 +7874,11 @@
         <f>NoMalahat!H33</f>
         <v>ST300</v>
       </c>
-      <c r="I32" s="96">
+      <c r="I32" s="89">
         <f>NoMalahat!I33</f>
         <v>44364</v>
       </c>
-      <c r="J32" s="96">
+      <c r="J32" s="89">
         <f>NoMalahat!J33</f>
         <v>44376</v>
       </c>
@@ -7917,19 +7916,19 @@
       </c>
       <c r="G48" s="33">
         <f>SUM('Table 2'!E3:E25)</f>
-        <v>57935</v>
+        <v>57435</v>
       </c>
       <c r="H48" s="34">
         <f>SUM('Table 2'!F3:F25)</f>
-        <v>23035</v>
+        <v>21684</v>
       </c>
       <c r="I48" s="34">
         <f>SUM('Table 2'!G3:G25)</f>
-        <v>9257</v>
+        <v>9101</v>
       </c>
       <c r="J48" s="34">
         <f>SUM('Table 2'!H3:H25)</f>
-        <v>127353</v>
+        <v>127946</v>
       </c>
       <c r="K48" s="34">
         <f>SUM('Table 2'!J3:J25)</f>
@@ -7941,7 +7940,7 @@
       </c>
       <c r="M48" s="2">
         <f>SUM('Table 2'!L3:L25)</f>
-        <v>13271</v>
+        <v>12788</v>
       </c>
     </row>
   </sheetData>
@@ -7953,8 +7952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C891EA49-1228-4754-8524-0795D1247222}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="M32" sqref="A1:M32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7976,19 +7975,19 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="40"/>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="73" t="s">
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
     </row>
     <row r="2" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -8213,24 +8212,22 @@
         <v>Call, pulsed only</v>
       </c>
       <c r="E6" s="41">
-        <f>NoMalahat!N6</f>
-        <v>1626</v>
+        <v>1126</v>
       </c>
       <c r="F6" s="6">
-        <f>NoMalahat!O6</f>
-        <v>9392</v>
+        <v>8041</v>
       </c>
       <c r="G6" s="6">
         <f>NoMalahat!P6</f>
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="H6" s="69">
         <f>NoMalahat!Q6</f>
-        <v>2946</v>
+        <v>3539</v>
       </c>
       <c r="I6" s="41">
         <f>NoMalahat!R6</f>
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J6" s="6">
         <f>NoMalahat!S6</f>
@@ -8241,11 +8238,9 @@
         <v>0</v>
       </c>
       <c r="L6" s="6">
-        <f>NoMalahat!U6</f>
-        <v>834</v>
+        <v>351</v>
       </c>
       <c r="M6" s="6">
-        <f>NoMalahat!V6</f>
         <v>418</v>
       </c>
     </row>

</xml_diff>